<commit_message>
joint model outputs sc ss layer offset, width, start, end and modifies offset to keep it within bounds
</commit_message>
<xml_diff>
--- a/examples/17_blade_joint/outputs_struct/blade_out.xlsx
+++ b/examples/17_blade_joint/outputs_struct/blade_out.xlsx
@@ -2475,16 +2475,16 @@
   0.00435823 0.00435168 0.00430703 0.0042194  0.00408392 0.00389572
   0.00364992 0.00334165 0.00298133 0.00257936 0.00214615 0.00169212
   0.00122768 0.001      0.001      0.001      0.001      0.001     ]
- [0.         0.01036386 0.01802123 0.02536166 0.03206819 0.03782389
-  0.04231181 0.045215   0.04621651 0.04569527 0.04403017 0.04160014
-  0.03878408 0.03596091 0.03350953 0.03135807 0.02943466 0.02766741
-  0.02598444 0.02431388 0.02258386 0.02080428 0.01898505 0.01713608
-  0.0152673  0.0133886  0.0115099  0.0096312  0.0077525  0.00587381]
- [0.         0.01247806 0.01761157 0.02274509 0.02766418 0.03215441
-  0.03600136 0.0389906  0.04090771 0.04153826 0.04110173 0.03981761
-  0.0379054  0.03558457 0.03307463 0.03059505 0.02815655 0.02576987
-  0.02344572 0.02119482 0.01902789 0.01695567 0.01496235 0.01303217
-  0.01114933 0.00929806 0.00746257 0.00562708 0.00379159 0.00195611]
+ [0.         0.00583337 0.01166673 0.0175001  0.02246982 0.02719278
+  0.03191574 0.03417685 0.03446848 0.0347601  0.03413613 0.03168096
+  0.02922579 0.02681664 0.02477562 0.0227346  0.02069359 0.04046992
+  0.06297342 0.08547692 0.08260286 0.06704002 0.05147718 0.03807502
+  0.02737371 0.01667241 0.00817846 0.00741024 0.00664202 0.00587381]
+ [0.         0.00583337 0.01166673 0.0175001  0.02246982 0.02719278
+  0.03191574 0.03417685 0.03446848 0.0347601  0.03413613 0.03168096
+  0.02922579 0.02681664 0.02477562 0.0227346  0.02069359 0.04046992
+  0.06297342 0.08547692 0.08260286 0.06704002 0.05147718 0.03807502
+  0.02737371 0.01667241 0.00817846 0.00741024 0.00664202 0.00587381]
  [0.         0.         0.00665003 0.00814812 0.00964621 0.0111443
   0.01260256 0.01398116 0.01524026 0.01634003 0.01724065 0.01790228
   0.01832761 0.01851932 0.01848012 0.01821267 0.01771968 0.01700382
@@ -2698,57 +2698,74 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>[[0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8
-  0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8
-  0.8    0.8    0.8    0.8    0.7536 0.7059 0.6587 0.611  0.5383 0.3419]
- [0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8
-  0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8
-  0.8    0.8    0.8    0.7855 0.7453 0.7019 0.6571 0.6099 0.5246 0.331 ]
- [0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094
-  0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094
-  0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.2801 0.2223 0.1635 0.1035]
- [1.152  1.1549 1.162  1.1673 1.1737 1.1797 1.1989 1.2105 1.2239 1.2277
-  1.2238 1.2183 1.2132 1.2126 1.2149 1.2212 1.2323 1.1573 1.0747 0.993
-  0.9128 0.8335 0.7545 0.6725 0.5489 0.4694 0.3894 0.3082 0.226  0.1426]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]]</t>
+          <t>[[0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.8     0.8     0.8     0.8     0.8     0.8     0.8     0.8     0.8
+  0.8     0.8     0.8     0.8     0.8     0.8     0.8     0.8     0.8
+  0.8     0.8     1.27728 0.8     0.8     0.8     0.7536  0.7059  0.6587
+  0.611   0.5383  0.3419 ]
+ [0.8     0.8     0.8     0.8     0.8     0.8     0.8     0.8     0.8
+  0.8     0.8     0.8     0.8     0.8     0.8     0.8     0.8     0.8
+  0.8     0.8     1.27728 0.8     0.8     0.7855  0.7453  0.7019  0.6571
+  0.6099  0.5246  0.331  ]
+ [0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094
+  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094
+  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.3094  0.2801
+  0.2223  0.1635  0.1035 ]
+ [1.152   1.1549  1.162   1.1673  1.1737  1.1797  1.1989  1.2105  1.2239
+  1.2277  1.2238  1.2183  1.2132  1.2126  1.2149  1.2212  1.2323  1.1573
+  1.0747  0.993   0.9128  0.8335  0.7545  0.6725  0.5489  0.4694  0.3894
+  0.3082  0.226   0.1426 ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]
+ [0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.      0.      0.      0.      0.      0.      0.
+  0.      0.      0.     ]]</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -3288,16 +3305,16 @@
   0.00435823 0.00435168 0.00430703 0.0042194  0.00408392 0.00389572
   0.00364992 0.00334165 0.00298133 0.00257936 0.00214615 0.00169212
   0.00122768 0.001      0.001      0.001      0.001      0.001     ]
- [0.         0.01036386 0.01802123 0.02536166 0.03206819 0.03782389
-  0.04231181 0.045215   0.04621651 0.04569527 0.04403017 0.04160014
-  0.03878408 0.03596091 0.03350953 0.03135807 0.02943466 0.02766741
-  0.02598444 0.02431388 0.02258386 0.02080428 0.01898505 0.01713608
-  0.0152673  0.0133886  0.0115099  0.0096312  0.0077525  0.00587381]
- [0.         0.01247806 0.01761157 0.02274509 0.02766418 0.03215441
-  0.03600136 0.0389906  0.04090771 0.04153826 0.04110173 0.03981761
-  0.0379054  0.03558457 0.03307463 0.03059505 0.02815655 0.02576987
-  0.02344572 0.02119482 0.01902789 0.01695567 0.01496235 0.01303217
-  0.01114933 0.00929806 0.00746257 0.00562708 0.00379159 0.00195611]
+ [0.         0.00583337 0.01166673 0.0175001  0.02246982 0.02719278
+  0.03191574 0.03417685 0.03446848 0.0347601  0.03413613 0.03168096
+  0.02922579 0.02681664 0.02477562 0.0227346  0.02069359 0.04046992
+  0.06297342 0.08547692 0.08260286 0.06704002 0.05147718 0.03807502
+  0.02737371 0.01667241 0.00817846 0.00741024 0.00664202 0.00587381]
+ [0.         0.00583337 0.01166673 0.0175001  0.02246982 0.02719278
+  0.03191574 0.03417685 0.03446848 0.0347601  0.03413613 0.03168096
+  0.02922579 0.02681664 0.02477562 0.0227346  0.02069359 0.04046992
+  0.06297342 0.08547692 0.08260286 0.06704002 0.05147718 0.03807502
+  0.02737371 0.01667241 0.00817846 0.00741024 0.00664202 0.00587381]
  [0.         0.         0.00665003 0.00814812 0.00964621 0.0111443
   0.01260256 0.01398116 0.01524026 0.01634003 0.01724065 0.01790228
   0.01832761 0.01851932 0.01848012 0.01821267 0.01771968 0.01700382
@@ -3380,10 +3397,8 @@
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
-          <t>[0.         0.05263158 0.10526316 0.15789474 0.21052632 0.26315789
- 0.31578947 0.36842105 0.42105263 0.47368421 0.52631579 0.57894737
- 0.63157895 0.68421053 0.73684211 0.78947368 0.84210526 0.89473684
- 0.94736842 1.        ]</t>
+          <t>[0.         0.11111111 0.22222222 0.33333333 0.44444444 0.55555556
+ 0.66666667 0.77777778 0.88888889 1.        ]</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3405,10 +3420,8 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>[0.         0.014274   0.02559803 0.035278   0.042476   0.04572004
- 0.04531975 0.04226395 0.03807994 0.03402034 0.03074453 0.02792861
- 0.02535178 0.04142444 0.02228027 0.01717876 0.01437916 0.011476
- 0.0086438  0.00587381]</t>
+          <t>[0.         0.01800887 0.03239023 0.03382215 0.02655211 0.02235925
+ 0.09258877 0.04592492 0.0095078  0.00587381]</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3426,10 +3439,8 @@
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
-          <t>[0.         0.05263158 0.10526316 0.15789474 0.21052632 0.26315789
- 0.31578947 0.36842105 0.42105263 0.47368421 0.52631579 0.57894737
- 0.63157895 0.68421053 0.73684211 0.78947368 0.84210526 0.89473684
- 0.94736842 1.        ]</t>
+          <t>[0.         0.11111111 0.22222222 0.33333333 0.44444444 0.55555556
+ 0.66666667 0.77777778 0.88888889 1.        ]</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3451,10 +3462,8 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>[0.         0.01439406 0.02571464 0.03540044 0.04261741 0.04584753
- 0.04543236 0.04236752 0.03818973 0.03415463 0.03085191 0.02803946
- 0.0254569  0.02285702 0.02013403 0.01733071 0.01447627 0.01160878
- 0.00874129 0.00587381]</t>
+          <t>[0.         0.01860448 0.03292068 0.03434412 0.02708432 0.02289096
+ 0.0845189  0.04403153 0.010066   0.00587381]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -6503,16 +6512,16 @@
   0.00435823 0.00435168 0.00430703 0.0042194  0.00408392 0.00389572
   0.00364992 0.00334165 0.00298133 0.00257936 0.00214615 0.00169212
   0.00122768 0.001      0.001      0.001      0.001      0.001     ]
- [0.         0.00935193 0.01778836 0.02520755 0.03160629 0.03726366
-  0.04197958 0.04437768 0.04562342 0.04536116 0.04363379 0.0413983
-  0.03865705 0.03598015 0.03345555 0.03130932 0.02938512 0.02757318
-  0.02588492 0.03255677 0.03944401 0.02690128 0.0201693  0.01698569
-  0.01515147 0.01327796 0.01137834 0.00952276 0.00768863 0.00587381]
- [0.         0.00935193 0.01778836 0.02520755 0.03160629 0.03726366
-  0.04197958 0.04437768 0.04562342 0.04536116 0.04363379 0.0413983
-  0.03865705 0.03598015 0.03345555 0.03130932 0.02938512 0.02757318
-  0.02588492 0.03255677 0.03944401 0.02690128 0.0201693  0.01698569
-  0.01515147 0.01327796 0.01137834 0.00952276 0.00768863 0.00587381]
+ [0.         0.00558896 0.01117792 0.01676688 0.02148023 0.02594341
+  0.03040659 0.03263711 0.0330815  0.03352589 0.03307007 0.03081386
+  0.02855764 0.02640753 0.0251063  0.02380507 0.02250383 0.04173291
+  0.06352828 0.08532365 0.08293418 0.0684523  0.05397041 0.04090187
+  0.02960001 0.01829814 0.00925718 0.00812939 0.0070016  0.00587381]
+ [0.         0.00558896 0.01117792 0.01676688 0.02148023 0.02594341
+  0.03040659 0.03263711 0.0330815  0.03352589 0.03307007 0.03081386
+  0.02855764 0.02640753 0.0251063  0.02380507 0.02250383 0.04173291
+  0.06352828 0.08532365 0.08293418 0.0684523  0.05397041 0.04090187
+  0.02960001 0.01829814 0.00925718 0.00812939 0.0070016  0.00587381]
  [0.         0.         0.00665003 0.00814812 0.00964621 0.0111443
   0.01260256 0.01398116 0.01524026 0.01634003 0.01724065 0.01790228
   0.01832761 0.01851932 0.01848012 0.01821267 0.01771968 0.01700382
@@ -6608,12 +6617,12 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -6633,7 +6642,7 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -6643,7 +6652,7 @@
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.         0.         0.         0.         0.         0.
   0.         0.         0.         0.         0.         0.
@@ -6710,12 +6719,12 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -6730,7 +6739,7 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -6740,7 +6749,7 @@
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.95925412 0.95895293 0.9565692  0.95388656 0.95056337 0.94780072
   0.9455854  0.94397287 0.94256868 0.94189525 0.94165198 0.94093289
@@ -6983,7 +6992,7 @@
       <c r="B144" t="inlineStr"/>
       <c r="C144" t="inlineStr">
         <is>
-          <t>[976.61986675]</t>
+          <t>[786.34407823]</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -8040,12 +8049,12 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>[2266.13610201 1853.00054762 1560.01660122 1302.77401846 1006.3192668
-  822.33415501  703.12958261  614.07751948  549.96141798  505.30318073
-  474.82503771  451.99615657  433.05904977  409.75492819  384.12608968
-  347.90003847  315.5419586   279.39709388  244.5120374   233.31434508
-  509.09459578  170.26361066  132.86137652  106.68223292   84.17854644
-   66.22613645   51.27575971   37.64284272   25.65292264   12.16854716]</t>
+          <t>[2266.13610201 1843.38483627 1543.49501144 1281.40868305  980.83112629
+  794.00714581  673.89570668  584.2234188   517.99024983  475.12850153
+  447.89569235  425.01428037  407.3122037   385.33795392  362.81593765
+  328.7293466   297.95030531  315.61382436  340.82599289  368.34989294
+  819.09943481  276.62146785  219.39189467  167.35567139  118.84123654
+   77.541249     46.80596808   34.91721243   24.48170766   12.16854716]</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -8134,14 +8143,14 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>[ 1277.32213347  1333.66454013  1575.72233364  1923.62455217
-  2398.44802251  2986.95809745  3532.40487805  4369.70111609
-  5399.44395166  6572.67691964  7784.63220523  9157.13455125
- 10676.99699663 11864.12085972 12896.53014651 13502.5292014
- 13910.69990874 14175.98068984 14331.25045083 14313.90156797
- 15620.65379692 13759.44219581 13115.64858014 12086.88521829
- 10337.88408717  8762.20030543  7572.93982553  6265.8578703
-  4804.97872049  3092.77926624]</t>
+          <t>[ 1277.32213347  1328.77489494  1565.94929473  1909.79248554
+  2380.88285742  2966.13453618  3508.94501981  4342.62437696
+  5365.60602419  6535.37897945  7746.55618808  9114.41981769
+ 10631.49423935 11814.18342107 12845.40800214 13450.2376201
+ 13857.31815444 14300.58689052 14711.12534088 14909.29558868
+ 17112.49739161 14320.11801464 13619.76169977 12472.78523353
+ 10576.08252165  8846.04701738  7537.14605807  6242.25387193
+  4794.09314384  3092.77926624]</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -8163,14 +8172,14 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>[  536.83457993   575.11022232   493.61045586   224.13252526
-  -231.14772655  -674.24543528 -1014.68076261 -1480.84749507
- -1945.99250883 -2330.5195834  -2569.72728371 -2819.25349697
- -3082.56835541 -3196.57228357 -3304.66354281 -3366.2182337
- -3402.8352313  -3405.99985864 -3366.42386412 -3275.92081957
- -3172.43358994 -3144.95672731 -3079.48757462 -2910.31855232
- -2508.9805439  -2110.64524653 -1839.22259848 -1536.19596679
- -1186.61896131  -774.11428704]</t>
+          <t>[  536.83457993   573.45585212   490.57813707   220.25675853
+  -235.51243783  -678.59194534 -1018.40930317 -1483.93941871
+ -1949.00815806 -2333.78783452 -2573.06632682 -2823.00286203
+ -3086.56505294 -3200.90254452 -3308.77570824 -3369.93230952
+ -3406.10212828 -3399.34682102 -3348.6176041  -3251.86861264
+ -3123.20640151 -3131.74338824 -3074.61632835 -2913.0762323
+ -2514.71367588 -2113.86135153 -1837.41124596 -1534.73202762
+ -1185.83001417  -774.11428704]</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -8192,14 +8201,14 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>[-17562.08341165 -10000.49062362  -4745.4425266    -895.6100005
-   1676.0611966    3303.05818753   4475.94371695   5349.9064811
-   6080.04379118   6769.82016172   7474.04945227   8174.39975929
-   8846.80778492   9327.74156639   9638.75253475   9540.5497714
-   9389.23351102   8962.48224161   8408.3351963    8563.01458068
-  19865.81148052   7037.79167909   5797.31860013   4900.47641079
-   4060.62106428   3346.82446095   2708.61270602   2074.21785592
-   1472.01185096    726.28962308]</t>
+          <t>[-17562.08341165  -9948.59542513  -4695.18520582   -880.92210544
+   1633.60977518   3189.27748285   4289.84831356   5089.81448677
+   5726.58971967   6365.55365515   7050.16435159   7686.42958705
+   8320.83471416   8771.90877415   9104.02373771   9014.82709332
+   8865.77811597  10124.24022284  11720.40126277  13519.03803007
+  31962.772912    11434.05955726   9573.02073068   7687.52675499
+   5732.68663783   3918.64847928   2472.49851734   1924.02858691
+   1404.80538289    726.28962308]</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -8247,14 +8256,14 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>[3.27488196e+10 2.87471934e+10 2.65377243e+10 2.32086681e+10
- 2.03855816e+10 1.90201540e+10 1.84692760e+10 1.78476324e+10
- 1.72845685e+10 1.66291512e+10 1.58565282e+10 1.50891541e+10
- 1.42602129e+10 1.33915354e+10 1.25204286e+10 1.15831412e+10
- 1.07403795e+10 9.82182456e+09 8.95291059e+09 1.02357678e+10
- 1.16172937e+10 8.14237593e+09 6.17420116e+09 5.09710893e+09
- 4.21485719e+09 3.43120466e+09 2.72481453e+09 2.08437908e+09
- 1.45340227e+09 6.99425947e+08]</t>
+          <t>[3.27488196e+10 2.78000519e+10 2.49103580e+10 2.11041959e+10
+ 1.78750157e+10 1.62299613e+10 1.55897575e+10 1.49070221e+10
+ 1.41354285e+10 1.36569641e+10 1.32040046e+10 1.24314562e+10
+ 1.17241647e+10 1.09864787e+10 1.04213920e+10 9.69484005e+09
+ 9.00761266e+09 1.33891499e+10 1.84397750e+10 2.35366849e+10
+ 4.83321861e+10 1.86185584e+10 1.46974031e+10 1.10734047e+10
+ 7.62911050e+09 4.54573617e+09 2.28454285e+09 1.81590619e+09
+ 1.33803833e+09 6.99425947e+08]</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -8276,14 +8285,14 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>[7.98178777e+10 6.94950688e+10 6.39224922e+10 5.18452599e+10
- 4.01621269e+10 3.26900480e+10 2.80924838e+10 2.48048894e+10
- 2.26903758e+10 2.13570182e+10 2.04192766e+10 1.94561008e+10
- 1.84049573e+10 1.68132033e+10 1.46473005e+10 1.17379538e+10
- 9.42436022e+09 7.14235324e+09 5.26301787e+09 3.98006025e+09
- 2.98013431e+09 1.96635432e+09 1.29338525e+09 8.49407154e+08
- 5.18207337e+08 3.10758614e+08 1.77868347e+08 9.42368162e+07
- 4.22294979e+07 7.73841653e+06]</t>
+          <t>[7.98178777e+10 6.77955372e+10 6.16229623e+10 4.90937545e+10
+ 3.78829826e+10 3.09720516e+10 2.68436700e+10 2.38227437e+10
+ 2.17573530e+10 2.05009297e+10 1.96527336e+10 1.86585013e+10
+ 1.76229151e+10 1.60527986e+10 1.40332368e+10 1.12773654e+10
+ 9.06231436e+09 7.57635362e+09 6.04878709e+09 4.80627651e+09
+ 1.37163466e+10 2.53853853e+09 1.75121005e+09 1.15969691e+09
+ 6.75023384e+08 3.55843426e+08 1.62307510e+08 8.61377452e+07
+ 3.95959900e+07 7.73841653e+06]</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -8305,14 +8314,14 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>[7.98160892e+10 7.18036153e+10 5.81316140e+10 4.06655590e+10
- 2.79779113e+10 2.02177462e+10 1.59567443e+10 1.22132080e+10
- 9.76988069e+09 8.42351097e+09 7.36390913e+09 6.39653552e+09
- 5.54365867e+09 4.63290762e+09 3.76617624e+09 2.94108664e+09
- 2.28032835e+09 1.75517022e+09 1.33499619e+09 1.27968254e+09
- 1.16540995e+09 6.37019351e+08 3.64492707e+08 2.18785875e+08
- 1.26417304e+08 6.76231210e+07 3.27985379e+07 1.35686765e+07
- 4.24497980e+06 7.26140362e+05]</t>
+          <t>[7.98160892e+10 6.88965047e+10 5.30347178e+10 3.56228834e+10
+ 2.31529522e+10 1.61977652e+10 1.27371437e+10 9.68423536e+09
+ 7.57840388e+09 6.59649563e+09 5.87213893e+09 5.02427955e+09
+ 4.33169491e+09 3.60288169e+09 2.98202154e+09 2.35107558e+09
+ 1.83111569e+09 2.48404476e+09 2.82264788e+09 2.79388235e+09
+ 3.38357719e+09 1.36247949e+09 8.25625641e+08 4.58386248e+08
+ 2.23100692e+08 8.89372997e+07 2.75010568e+07 1.18877054e+07
+ 3.93640157e+06 7.26140362e+05]</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -8334,14 +8343,14 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>[ 1.62026992e+06  5.70088271e+09  1.11708696e+10  1.30375677e+10
-  1.30899655e+10  1.05434092e+10  7.70662280e+09  5.22692562e+09
-  3.84877615e+09  3.53075981e+09  3.30947972e+09  3.06562553e+09
-  2.81262373e+09  2.44767013e+09  1.94996114e+09  1.39036335e+09
-  9.74698027e+08  6.57469688e+08  4.34522063e+08  3.08518947e+08
-  2.05108149e+08  9.54326372e+07  3.23673646e+07 -1.05009584e+06
- -1.32572645e+07 -1.34694318e+07 -9.74331572e+06 -5.79861767e+06
- -3.02396754e+06 -6.65447126e+05]</t>
+          <t>[ 1.62026992e+06  3.52750463e+09  7.84301602e+09  1.02552756e+10
+  1.06024756e+10  8.74606477e+09  6.54919954e+09  4.52440104e+09
+  3.34332656e+09  3.10432650e+09  2.95174610e+09  2.72567426e+09
+  2.50367141e+09  2.18076963e+09  1.75751641e+09  1.26240989e+09
+  8.89563207e+08  7.66176600e+08  6.22910020e+08  4.77356072e+08
+  6.08758326e+08  1.46446430e+08  4.80662105e+07 -4.04224334e+06
+ -1.95580255e+07 -1.59563706e+07 -8.80785270e+06 -5.30673199e+06
+ -2.83461618e+06 -6.65447126e+05]</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -8363,14 +8372,14 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>[4.67030345e+10 3.82371171e+10 5.75547622e+10 4.59766687e+10
- 3.02417512e+10 2.02493133e+10 1.43246895e+10 1.00272753e+10
- 7.44674413e+09 6.41529303e+09 5.71892471e+09 5.01387951e+09
- 4.41263846e+09 3.54562295e+09 2.73304007e+09 1.88794696e+09
- 1.26586695e+09 8.61606769e+08 5.74938738e+08 3.96329457e+08
- 2.58633761e+08 1.42065635e+08 7.27307051e+07 3.50737424e+07
- 1.85510853e+07 9.42401573e+06 4.57702793e+06 1.86513462e+06
- 5.91578467e+05 1.07204742e+05]</t>
+          <t>[4.67030345e+10 3.81358036e+10 5.69140008e+10 4.50213974e+10
+ 2.92638028e+10 1.93890111e+10 1.36319804e+10 9.48336085e+09
+ 6.97065384e+09 5.99124618e+09 5.34947088e+09 4.65550317e+09
+ 4.08358251e+09 3.27505996e+09 2.54154587e+09 1.77054321e+09
+ 1.19127522e+09 9.40814269e+08 6.82196335e+08 4.58746183e+08
+ 2.34797592e+08 1.64574415e+08 8.70047497e+07 4.18050255e+07
+ 2.15330292e+07 1.02096385e+07 4.31866701e+06 1.78399071e+06
+ 5.77208667e+05 1.07204742e+05]</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -8392,14 +8401,14 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>[1.10488682e+04 9.11187259e+03 7.18268404e+03 5.00549162e+03
- 3.29704037e+03 2.37730094e+03 1.88095853e+03 1.54177756e+03
- 1.32546105e+03 1.19613733e+03 1.11449399e+03 1.03924531e+03
- 9.72887815e+02 8.67840328e+02 7.50659128e+02 5.95238802e+02
- 4.72859949e+02 3.61154054e+02 2.68408164e+02 2.02981344e+02
- 1.49683643e+02 9.76820656e+01 6.29320278e+01 3.96402212e+01
- 2.32551820e+01 1.31136166e+01 6.89121157e+00 3.13988179e+00
- 1.18937133e+00 2.07959203e-01]</t>
+          <t>[1.10488682e+04 9.06654355e+03 7.10961536e+03 4.92421565e+03
+ 3.21989804e+03 2.31106237e+03 1.82540315e+03 1.49450889e+03
+ 1.28022226e+03 1.15522014e+03 1.07898336e+03 1.00427090e+03
+ 9.40368282e+02 8.37479065e+02 7.26473263e+02 5.76879730e+02
+ 4.58268147e+02 3.83003752e+02 3.09382710e+02 2.41108919e+02
+ 2.90494847e+02 1.16340845e+02 7.55239818e+01 4.67558933e+01
+ 2.63455260e+01 1.38846318e+01 6.65987406e+00 3.03813423e+00
+ 1.15965207e+00 2.07959203e-01]</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -8421,14 +8430,14 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>[ 3.05311332e-16 -2.89698820e-16 -1.38777878e-16 -2.19678980e-03
- -1.66065590e-03 -1.12158440e-03 -7.21840232e-04 -4.21549738e-04
- -2.78242977e-04 -2.32236547e-04 -2.20450251e-04 -2.39603945e-04
- -2.64096454e-04 -3.16594543e-04 -3.02107198e-04 -2.55288834e-04
- -2.11028331e-04 -1.59200319e-04 -1.16378406e-04 -4.91570567e-05
- -1.91454646e-05 -1.96296804e-05 -1.19177475e-05 -8.26216470e-06
-  4.96884008e-06  1.07929454e-05  1.21632903e-05  1.09281550e-05
-  8.63500418e-06 -1.04083409e-17]</t>
+          <t>[ 3.05311332e-16 -3.92914867e-16 -7.63278329e-16 -2.27850696e-03
+ -2.10853677e-03 -1.61982365e-03 -1.11490524e-03 -7.13784990e-04
+ -5.25521536e-04 -4.53254139e-04 -4.19353456e-04 -4.55342447e-04
+ -4.86739117e-04 -5.42787986e-04 -4.84660353e-04 -3.93688541e-04
+ -3.16770038e-04 -7.72707849e-05 -2.10982858e-05 -6.23335785e-06
+ -6.22340560e-06 -2.08568123e-06 -6.72812120e-07 -2.90182579e-06
+  1.24372582e-06  6.23320379e-06  1.70051778e-05  1.39445881e-05
+  9.76336247e-06 -1.04083409e-17]</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -8450,14 +8459,14 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>[ 3.54913581e-16  2.46330734e-16  5.55111512e-17  3.83508210e-03
-  1.30529653e-03 -8.58765410e-04 -1.99322080e-03 -2.68691776e-03
- -2.88812850e-03 -2.80165172e-03 -2.82551380e-03 -2.89334296e-03
- -2.96179122e-03 -3.02466114e-03 -2.88972541e-03 -2.51059267e-03
- -2.20691727e-03 -1.78923009e-03 -1.40960698e-03 -6.58213891e-04
- -3.08626724e-04 -4.30966508e-04 -4.85978002e-04 -4.38696769e-04
- -3.48525518e-04 -2.80860755e-04 -2.40018862e-04 -2.29831886e-04
- -2.96251808e-04  9.54097912e-18]</t>
+          <t>[ 3.54913581e-16  6.50521303e-17  2.49800181e-16  2.96108600e-03
+ -5.94225147e-05 -2.55809327e-03 -3.73360837e-03 -4.46060357e-03
+ -4.80229302e-03 -4.59139750e-03 -4.46459582e-03 -4.67160525e-03
+ -4.78499557e-03 -4.87538886e-03 -4.46478076e-03 -3.80440685e-03
+ -3.29890802e-03 -8.64102065e-04 -2.44087344e-04 -7.86726187e-05
+ -7.28377864e-06 -6.59413343e-05 -8.11439669e-05 -1.00677857e-04
+ -1.23372772e-04 -1.77954365e-04 -3.11707722e-04 -2.72217038e-04
+ -3.22344548e-04  9.54097912e-18]</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -8479,14 +8488,14 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>[7.98151328e+10 6.48327786e+10 4.94870403e+10 3.20696826e+10
- 1.96317514e+10 1.42042769e+10 1.22158885e+10 1.03262351e+10
- 8.71029175e+09 7.52241410e+09 6.57289377e+09 5.71270912e+09
- 4.95546712e+09 4.15944350e+09 3.42728594e+09 2.72656780e+09
- 2.14973242e+09 1.67609121e+09 1.28750310e+09 1.24488262e+09
- 1.14251653e+09 6.30203214e+08 3.63366228e+08 2.18784126e+08
- 1.25969222e+08 6.68792057e+07 3.21470736e+07 1.31539898e+07
- 4.00574656e+06 6.63549801e+05]</t>
+          <t>[7.98151328e+10 6.47758219e+10 4.83872302e+10 3.00887306e+10
+ 1.76083779e+10 1.21366076e+10 1.01654099e+10 8.36035901e+09
+ 6.82960402e+09 5.93489499e+09 5.26650075e+09 4.49956942e+09
+ 3.87571871e+09 3.23194176e+09 2.70924934e+09 2.17597268e+09
+ 1.72329164e+09 2.37126535e+09 2.70655281e+09 2.68639124e+09
+ 3.34783563e+09 1.34451786e+09 8.23136227e+08 4.58362950e+08
+ 2.22255852e+08 8.79867697e+07 2.69280138e+07 1.15103452e+07
+ 3.71248087e+06 6.63549801e+05]</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -8508,14 +8517,14 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>[7.98188341e+10 7.64659055e+10 7.25670659e+10 6.04406830e+10
- 4.85081958e+10 3.87034794e+10 3.18332565e+10 2.66917303e+10
- 2.37498192e+10 2.22579837e+10 2.12101646e+10 2.01398001e+10
- 1.89930228e+10 1.72865436e+10 1.49860851e+10 1.19523989e+10
- 9.55490336e+09 7.22140055e+09 5.31049305e+09 4.01485570e+09
- 3.00302662e+09 1.97316894e+09 1.29451027e+09 8.49407922e+08
- 5.18654908e+08 3.11502258e+08 1.78519654e+08 9.46513925e+07
- 4.24686035e+07 7.80100709e+06]</t>
+          <t>[7.98188341e+10 7.19162200e+10 6.62704498e+10 5.46276126e+10
+ 4.34274774e+10 3.50330604e+10 2.94151672e+10 2.51463158e+10
+ 2.25058229e+10 2.11622396e+10 2.02581063e+10 1.91829375e+10
+ 1.80786201e+10 1.64234741e+10 1.43057988e+10 1.14523265e+10
+ 9.17003948e+09 7.68912295e+09 6.16488105e+09 4.91376748e+09
+ 1.37520882e+10 2.55650008e+09 1.75369937e+09 1.15972010e+09
+ 6.75868108e+08 3.56793812e+08 1.62880330e+08 8.65149705e+07
+ 3.98197715e+07 7.80100709e+06]</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -8537,11 +8546,11 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>[30.55251326 50.72304745 37.73448418 33.396764   32.52131522 29.69836566
- 25.89232328 19.85013459 15.39255336 14.31705478 13.44238579 12.5747098
- 11.81181196 10.94780474  9.85917236  8.77100584  7.63139564  6.85847097
-  6.23765047  6.43557556  6.36878563  4.08533143  1.99325604 -0.09540907
- -1.93580583 -3.16122874 -3.82525706 -4.09053094 -4.52338717 -5.37331236]</t>
+          <t>[30.55251326 49.43486844 30.64944808 28.35224956 27.60702659 24.90731949
+ 21.43894558 16.30997632 12.62418539 12.03105717 11.59505421 10.89656444
+ 10.3218013   9.65342811  8.82213662  7.89686379  6.91112837  8.37367625
+ 10.55739414 12.69020784  3.36010519  6.99239523  2.96477795 -0.33022947
+ -2.47344663 -3.40911355 -3.72244464 -4.06744114 -4.51670881 -5.37331236]</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -8563,14 +8572,14 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>[-3.48176418e+07 -3.26389882e+07 -2.92716934e+07 -3.19960854e+07
- -3.11989678e+07 -2.99064659e+07 -2.88189400e+07 -2.75536837e+07
- -2.56726448e+07 -2.32654324e+07 -2.07774528e+07 -1.83832677e+07
- -1.61037967e+07 -1.39572094e+07 -1.19590939e+07 -1.01150856e+07
- -8.42836025e+06 -6.90453071e+06 -5.54903682e+06 -4.36358600e+06
- -3.34616543e+06 -2.48286920e+06 -1.75960673e+06 -1.18496156e+06
- -7.48517220e+05 -4.32339997e+05 -2.16572064e+05 -8.36799124e+04
- -1.71054148e+04  2.83850017e+00]</t>
+          <t>[-3.49475571e+07 -3.27227091e+07 -3.12035510e+07 -3.40649595e+07
+ -3.25038652e+07 -3.08643310e+07 -2.93712780e+07 -2.76651160e+07
+ -2.54786421e+07 -2.29635206e+07 -2.04477650e+07 -1.80461145e+07
+ -1.57738394e+07 -1.36445712e+07 -1.16723102e+07 -9.86345069e+06
+ -8.22088493e+06 -6.74834090e+06 -5.44164119e+06 -4.29289835e+06
+ -3.31671456e+06 -2.47551879e+06 -1.76914295e+06 -1.19522074e+06
+ -7.57111476e+05 -4.39065623e+05 -2.20785699e+05 -8.54283199e+04
+ -1.75485171e+04  3.01134316e+00]</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -8592,14 +8601,14 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>[ 3.46361181e+07  3.25690789e+07  3.16723777e+07  2.42880821e+07
-  2.03409180e+07  1.69123952e+07  1.27651238e+07  8.17190417e+06
-  4.29760102e+06  2.52610201e+06  1.96553843e+06  1.53341102e+06
-  1.18081099e+06  8.75478933e+05  5.51845758e+05  2.37571304e+05
- -1.16923027e+04 -1.57155828e+05 -2.11192828e+05 -1.93997314e+05
- -1.56239687e+05 -1.77002675e+05 -2.05047295e+05 -1.94972087e+05
- -1.59687243e+05 -1.10136881e+05 -6.15145142e+04 -2.54398971e+04
- -5.54443133e+03  9.37112041e-02]</t>
+          <t>[ 3.43400918e+07  3.22608410e+07  2.94824675e+07  2.08362140e+07
+  1.76112084e+07  1.43746365e+07  1.04687516e+07  6.32816123e+06
+  3.00404280e+06  1.63019453e+06  1.33881701e+06  1.08276032e+06
+  8.42829073e+05  6.35584012e+05  4.00694135e+05  1.54319027e+05
+ -5.16331437e+04 -4.66363925e+04  1.15751955e+05  2.37519564e+05
+ -3.81283481e+04 -1.65991616e+05 -1.38048934e+05 -1.84504514e+05
+ -1.64668214e+05 -1.14022991e+05 -6.25543725e+04 -2.56714985e+04
+ -5.62488618e+03  9.62241177e-02]</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -8621,14 +8630,14 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>[4.92881120e+05 5.40320187e+05 5.65700010e+05 5.75409054e+05
- 5.74065788e+05 5.65496024e+05 5.52107268e+05 5.35195599e+05
- 5.15523047e+05 4.93406624e+05 4.68890922e+05 4.41957740e+05
- 4.12661849e+05 3.81380895e+05 3.48736892e+05 3.15726615e+05
- 2.83145796e+05 2.51559914e+05 2.21662296e+05 1.92452217e+05
- 1.43522212e+05 9.72173309e+04 7.51263028e+04 5.67138934e+04
- 4.12905842e+04 2.85413291e+04 1.81190697e+04 9.88714567e+03
- 3.78358604e+03 1.63709046e-11]</t>
+          <t>[ 5.94274706e+05  6.41624454e+05  6.66828461e+05  6.76425726e+05
+  6.75130244e+05  6.66829377e+05  6.53956750e+05  6.37813032e+05
+  6.19196479e+05  5.98384200e+05  5.75293861e+05  5.49930111e+05
+  5.22379358e+05  4.92960342e+05  4.62193346e+05  4.31008255e+05
+  4.00233218e+05  3.67548724e+05  3.29951026e+05  2.86510401e+05
+  2.08229806e+05  1.33537756e+05  9.73816167e+04  6.76737883e+04
+  4.45757147e+04  2.79644100e+04  1.69643473e+04  9.39730552e+03
+  3.66791413e+03 -1.10958354e-10]</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -8646,11 +8655,11 @@
       <c r="B209" t="inlineStr"/>
       <c r="C209" t="inlineStr">
         <is>
-          <t>[0.01845476 1.80647192 1.78210746 1.66717674 1.36915096 1.14381813
- 1.01969255 0.91190033 0.83269731 0.7832859  0.74728939 0.71222546
- 0.68100664 0.64119226 0.60127384 0.55699699 0.5138373  0.4742272
- 0.43518793 0.39949138 0.36185089 0.32137889 0.28319047 0.24434672
- 0.20761114 0.17177406 0.13739079 0.10355928 0.07093337 0.04180818]</t>
+          <t>[0.01845476 1.80610553 1.77511121 1.67439061 1.35798653 1.12606451
+ 1.00299863 0.8971396  0.81882232 0.76997042 0.73484888 0.69891837
+ 0.66747315 0.62805161 0.59043996 0.54853259 0.50710681 0.48136415
+ 0.44555329 0.40613319 0.36029216 0.32439993 0.2850244  0.24467818
+ 0.20715457 0.1713492  0.13774788 0.10378081 0.07100616 0.04180818]</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -8668,11 +8677,11 @@
       <c r="B210" t="inlineStr"/>
       <c r="C210" t="inlineStr">
         <is>
-          <t>[ 0.01845476 -1.81173964 -1.86308381 -1.53733695 -1.51424662 -1.35766188
- -1.19780477 -1.04634594 -0.93871091 -0.884776   -0.84890053 -0.81606427
- -0.78765485 -0.75033126 -0.70183517 -0.64105273 -0.58392254 -0.52923598
- -0.47761529 -0.42532554 -0.37734019 -0.33427371 -0.29141927 -0.25036702
- -0.20866153 -0.17011766 -0.13445922 -0.10000234 -0.066506   -0.03885717]</t>
+          <t>[ 0.01845476 -1.81210603 -1.87008005 -1.53012308 -1.52541105 -1.3754155
+ -1.21449869 -1.06110668 -0.95258589 -0.89809148 -0.86134104 -0.82937136
+ -0.80118835 -0.76347191 -0.71266904 -0.64951713 -0.59065303 -0.52209903
+ -0.46724993 -0.41868374 -0.37701056 -0.33125267 -0.28958533 -0.25003556
+ -0.2091181  -0.17054253 -0.13410213 -0.09978081 -0.06643321 -0.03885717]</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -8690,14 +8699,14 @@
       <c r="B211" t="inlineStr"/>
       <c r="C211" t="inlineStr">
         <is>
-          <t>[-2.24984856e+00  1.34247025e+00  1.05955058e+00  2.58067194e-01
-  1.09478110e-01 -4.02411750e-02 -1.44344992e-01 -2.26544806e-01
- -2.69374000e-01 -2.76640749e-01 -2.88445188e-01 -3.04602749e-01
- -3.18722442e-01 -3.36363575e-01 -3.36580833e-01 -3.11964250e-01
- -2.93850597e-01 -2.52787538e-01 -2.10089714e-01 -1.30069932e-01
- -7.93462982e-02 -8.71440460e-02 -8.47967341e-02 -7.29765737e-02
- -5.62024275e-02 -4.27169079e-02 -3.10092805e-02 -1.94402856e-02
- -8.56094043e-03  1.32614033e-03]</t>
+          <t>[-2.24984856e+00  1.34226720e+00  1.04900062e+00  1.93695644e-01
+  2.70912654e-02 -1.31270540e-01 -2.32877644e-01 -3.14310063e-01
+ -3.64311402e-01 -3.68549544e-01 -3.74394974e-01 -3.98150227e-01
+ -4.15180873e-01 -4.35781496e-01 -4.24892036e-01 -3.88748659e-01
+ -3.62798285e-01 -1.71788927e-01 -8.11670575e-02 -3.90255568e-02
+  2.20626280e-02 -3.02188736e-02 -3.28270168e-02 -3.54742862e-02
+ -3.52197968e-02 -3.51796916e-02 -3.46228078e-02 -2.07453567e-02
+ -8.64082046e-03  1.32614033e-03]</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -8715,14 +8724,14 @@
       <c r="B212" t="inlineStr"/>
       <c r="C212" t="inlineStr">
         <is>
-          <t>[-2.24984856e+00 -1.34061374e+00 -1.28752163e+00 -1.55930828e+00
- -1.27009765e+00 -1.02120288e+00 -8.13060176e-01 -6.56327557e-01
- -5.74139790e-01 -5.58159063e-01 -5.57139754e-01 -5.61535686e-01
- -5.65344145e-01 -5.67079184e-01 -5.36981059e-01 -4.74634114e-01
- -4.22064932e-01 -3.54674805e-01 -2.90976615e-01 -1.92486406e-01
- -1.24369037e-01 -1.14876488e-01 -9.36867525e-02 -6.50364986e-02
- -3.67326407e-02 -1.82494606e-02 -6.26409963e-03  2.05089906e-03
-  6.76865553e-03  1.10211452e-02]</t>
+          <t>[-2.24984856e+00 -1.34081679e+00 -1.29807159e+00 -1.62367983e+00
+ -1.35248449e+00 -1.11223225e+00 -9.01592827e-01 -7.44092814e-01
+ -6.69077191e-01 -6.50067858e-01 -6.43089540e-01 -6.55083164e-01
+ -6.61802576e-01 -6.66497105e-01 -6.25292261e-01 -5.51418523e-01
+ -4.91012620e-01 -2.73676194e-01 -1.62053958e-01 -1.01442031e-01
+  3.13133265e-04 -5.79513161e-02 -4.17170351e-02 -2.75342111e-02
+ -1.57500100e-02 -1.07122443e-02 -9.87762695e-03  7.45827951e-04
+  6.68877550e-03  1.10211452e-02]</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -8740,11 +8749,11 @@
       <c r="B213" t="inlineStr"/>
       <c r="C213" t="inlineStr">
         <is>
-          <t>[ 0.01845476  0.00733979 -0.06819624 -0.25712788 -0.22310211 -0.20692138
- -0.16789737 -0.15446169 -0.13287621 -0.13463984 -0.13356057 -0.13235376
- -0.13183974 -0.12574355 -0.11690578 -0.12425034 -0.10213034 -0.08391371
- -0.06953864 -0.05433115 -0.04244348 -0.03407349 -0.0227879  -0.01244195
- -0.00253607  0.00232586  0.00399133  0.00474265  0.00549329  0.00438864]</t>
+          <t>[ 0.01845476  0.00697339 -0.07519249 -0.24991401 -0.23426654 -0.224675
+ -0.18459129 -0.16922242 -0.1467512  -0.14795533 -0.14600109 -0.14566084
+ -0.14537323 -0.1388842  -0.12773965 -0.13271474 -0.10886083 -0.07677676
+ -0.05917328 -0.04768934 -0.04415977 -0.03105245 -0.02095396 -0.01211049
+ -0.00299264  0.001901    0.00434842  0.00496418  0.00556609  0.00438864]</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
@@ -8762,11 +8771,11 @@
       <c r="B214" t="inlineStr"/>
       <c r="C214" t="inlineStr">
         <is>
-          <t>[ 0.01845476  0.00733979 -0.06819624 -0.25712788 -0.22310211 -0.20692138
- -0.16789737 -0.15446169 -0.13287621 -0.13463984 -0.13356057 -0.13235376
- -0.13183974 -0.12574355 -0.11690578 -0.12425034 -0.10213034 -0.08391371
- -0.06953864 -0.05433115 -0.04244348 -0.03407349 -0.0227879  -0.01244195
- -0.00253607  0.00232586  0.00399133  0.00474265  0.00549329  0.00438864]</t>
+          <t>[ 0.01845476  0.00697339 -0.07519249 -0.24991401 -0.23426654 -0.224675
+ -0.18459129 -0.16922242 -0.1467512  -0.14795533 -0.14600109 -0.14566084
+ -0.14537323 -0.1388842  -0.12773965 -0.13271474 -0.10886083 -0.07677676
+ -0.05917328 -0.04768934 -0.04415977 -0.03105245 -0.02095396 -0.01211049
+ -0.00299264  0.001901    0.00434842  0.00496418  0.00556609  0.00438864]</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
@@ -8784,11 +8793,11 @@
       <c r="B215" t="inlineStr"/>
       <c r="C215" t="inlineStr">
         <is>
-          <t>[-2.24984856 -2.25754228 -2.38113078 -2.1714672  -2.08165648 -2.04469026
- -2.01771295 -2.01094915 -2.02443133 -2.0523633  -2.09018704 -2.08312528
- -2.06463481 -1.94750117 -1.84857251 -1.68832028 -1.54315582 -1.39506614
- -1.25524938 -1.08934189 -0.96237671 -0.90138559 -0.83492761 -0.75942715
- -0.67769362 -0.59842159 -0.51997399 -0.44051458 -0.35953443 -0.24509332]</t>
+          <t>[-2.24984856 -2.25774534 -2.39168074 -2.23583875 -2.16404332 -2.13571963
+ -2.1062456  -2.09871441 -2.11936873 -2.14427209 -2.17613683 -2.17667275
+ -2.16109324 -2.04691909 -1.93688371 -1.76510469 -1.61210351 -1.31406753
+ -1.12632673 -0.99829751 -0.89240329 -0.84446042 -0.78295789 -0.72192487
+ -0.65671099 -0.59088437 -0.52358751 -0.44181965 -0.35961431 -0.24509332]</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -8806,11 +8815,11 @@
       <c r="B216" t="inlineStr"/>
       <c r="C216" t="inlineStr">
         <is>
-          <t>[-2.24984856 -2.25754228 -2.38113078 -2.1714672  -2.08165648 -2.04469026
- -2.01771295 -2.01094915 -2.02443133 -2.0523633  -2.09018704 -2.08312528
- -2.06463481 -1.94750117 -1.84857251 -1.68832028 -1.54315582 -1.39506614
- -1.25524938 -1.08934189 -0.96237671 -0.90138559 -0.83492761 -0.75942715
- -0.67769362 -0.59842159 -0.51997399 -0.44051458 -0.35953443 -0.24509332]</t>
+          <t>[-2.24984856 -2.25774534 -2.39168074 -2.23583875 -2.16404332 -2.13571963
+ -2.1062456  -2.09871441 -2.11936873 -2.14427209 -2.17613683 -2.17667275
+ -2.16109324 -2.04691909 -1.93688371 -1.76510469 -1.61210351 -1.31406753
+ -1.12632673 -0.99829751 -0.89240329 -0.84446042 -0.78295789 -0.72192487
+ -0.65671099 -0.59088437 -0.52358751 -0.44181965 -0.35961431 -0.24509332]</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
@@ -8832,7 +8841,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>[12.81919827]</t>
+          <t>[13.0530476]</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
@@ -8854,7 +8863,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>[-3.4573195]</t>
+          <t>[-3.64229652]</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
@@ -8876,7 +8885,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>[-0.00204917]</t>
+          <t>[-0.00259821]</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
@@ -8968,14 +8977,14 @@
       <c r="B224" t="inlineStr"/>
       <c r="C224" t="inlineStr">
         <is>
-          <t>[ 3.15790711e-04 -1.02896471e-03 -1.31316820e-03 -1.72711262e-03
- -2.11666392e-03 -2.39598236e-03 -2.46919246e-03 -2.55347966e-03
- -2.59981392e-03 -2.58013029e-03 -2.52916225e-03 -2.46879838e-03
- -2.39643356e-03 -2.34466889e-03 -2.28761851e-03 -2.24148992e-03
- -2.17636799e-03 -2.09375943e-03 -1.99408708e-03 -1.46546701e-03
- -1.09338340e-03 -1.30509122e-03 -1.40883807e-03 -1.35072271e-03
- -1.25090346e-03 -1.12026158e-03 -9.30060335e-04 -6.60239420e-04
- -3.03522220e-04  1.78621441e-07]</t>
+          <t>[ 3.03656383e-04 -1.10836038e-03 -1.47078910e-03 -1.96448549e-03
+ -2.50087953e-03 -2.92473702e-03 -3.03869298e-03 -3.17160169e-03
+ -3.29814341e-03 -3.23941097e-03 -3.11616876e-03 -3.08405059e-03
+ -3.00644807e-03 -2.95478378e-03 -2.82958541e-03 -2.74524793e-03
+ -2.65592592e-03 -1.45455475e-03 -9.28467548e-04 -6.61498996e-04
+ -3.59236893e-04 -6.06169899e-04 -6.23469929e-04 -6.49455001e-04
+ -7.16427940e-04 -8.63733625e-04 -1.13272602e-03 -7.70886337e-04
+ -3.36127967e-04  1.89497061e-07]</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -8993,14 +9002,14 @@
       <c r="B225" t="inlineStr"/>
       <c r="C225" t="inlineStr">
         <is>
-          <t>[ 3.15790711e-04  9.95012134e-04  1.32620841e-03  1.26261384e-03
-  1.70623817e-03  2.06960338e-03  2.17767584e-03  2.29921748e-03
-  2.33376635e-03  2.28111135e-03  2.23944745e-03  2.19563062e-03
-  2.14486297e-03  2.11750359e-03  2.08802064e-03  2.06589219e-03
-  2.02235974e-03  1.95542034e-03  1.87171199e-03  1.37549151e-03
-  1.03695364e-03  1.25702421e-03  1.36596465e-03  1.33064368e-03
-  1.22761634e-03  1.09311251e-03  9.00925095e-04  6.31343410e-04
-  2.79793523e-04 -1.61251425e-07]</t>
+          <t>[ 3.03656383e-04  1.06635004e-03  1.50492298e-03  1.44168392e-03
+  2.07320581e-03  2.59174839e-03  2.72884745e-03  2.89041854e-03
+  2.99342462e-03  2.89389707e-03  2.78365484e-03  2.77059572e-03
+  2.71788039e-03  2.69124621e-03  2.59693185e-03  2.53696645e-03
+  2.46777809e-03  1.32701478e-03  8.50532381e-04  6.14165110e-04
+  3.68513298e-04  5.78849588e-04  6.05842541e-04  6.42129616e-04
+  7.06531847e-04  8.46374337e-04  1.09458861e-03  7.35448428e-04
+  3.09497576e-04 -1.71064424e-07]</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -9018,14 +9027,14 @@
       <c r="B226" t="inlineStr"/>
       <c r="C226" t="inlineStr">
         <is>
-          <t>[ 3.15790711e-04 -2.94600600e-04 -1.12666583e-05 -2.17727189e-04
- -7.21410619e-04 -9.63228329e-04 -9.94908535e-04 -8.69210503e-04
- -8.76437251e-04 -9.66393516e-04 -9.63644803e-04 -9.16018383e-04
- -8.55660335e-04 -7.57253555e-04 -6.62623662e-04 -4.93233691e-04
- -4.34840903e-04 -3.99045986e-04 -3.64565326e-04 -3.10145823e-04
- -2.51477987e-04 -2.11909188e-04 -1.74808140e-04 -1.11203452e-04
- -6.72156416e-05 -2.13049630e-05  2.13547248e-05  4.68739365e-05
-  4.82456123e-05 -7.65542097e-08]</t>
+          <t>[ 3.03656383e-04 -2.35543409e-04  1.61119225e-04 -1.89375742e-04
+ -6.84019989e-04 -9.76624924e-04 -1.04811797e-03 -9.36836516e-04
+ -9.57253517e-04 -1.04936730e-03 -1.04366265e-03 -9.98636443e-04
+ -9.38080445e-04 -8.36941053e-04 -7.26169641e-04 -5.24040023e-04
+ -4.63366673e-04 -3.63840107e-04 -2.94851207e-04 -2.40697108e-04
+ -1.49300924e-05 -1.94371308e-04 -1.10323843e-04 -7.85238663e-05
+ -5.89340747e-05 -2.88176376e-05  3.49399645e-05  5.97900280e-05
+  5.41910139e-05 -8.13158341e-08]</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -9043,14 +9052,14 @@
       <c r="B227" t="inlineStr"/>
       <c r="C227" t="inlineStr">
         <is>
-          <t>[ 3.15790711e-04 -2.94600600e-04 -1.12666583e-05 -2.17727189e-04
- -7.21410619e-04 -9.63228329e-04 -9.94908535e-04 -8.69210503e-04
- -8.76437251e-04 -9.66393516e-04 -9.63644803e-04 -9.16018383e-04
- -8.55660335e-04 -7.57253555e-04 -6.62623662e-04 -4.93233691e-04
- -4.34840903e-04 -3.99045986e-04 -3.64565326e-04 -3.10145823e-04
- -2.51477987e-04 -2.11909188e-04 -1.74808140e-04 -1.11203452e-04
- -6.72156416e-05 -2.13049630e-05  2.13547248e-05  4.68739365e-05
-  4.82456123e-05 -7.65542097e-08]</t>
+          <t>[ 3.03656383e-04 -2.35543409e-04  1.61119225e-04 -1.89375742e-04
+ -6.84019989e-04 -9.76624924e-04 -1.04811797e-03 -9.36836516e-04
+ -9.57253517e-04 -1.04936730e-03 -1.04366265e-03 -9.98636443e-04
+ -9.38080445e-04 -8.36941053e-04 -7.26169641e-04 -5.24040023e-04
+ -4.63366673e-04 -3.63840107e-04 -2.94851207e-04 -2.40697108e-04
+ -1.49300924e-05 -1.94371308e-04 -1.10323843e-04 -7.85238663e-05
+ -5.89340747e-05 -2.88176376e-05  3.49399645e-05  5.97900280e-05
+  5.41910139e-05 -8.13158341e-08]</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -9140,10 +9149,8 @@
       <c r="B232" t="inlineStr"/>
       <c r="C232" t="inlineStr">
         <is>
-          <t>[0.         0.05263158 0.10526316 0.15789474 0.21052632 0.26315789
- 0.31578947 0.36842105 0.42105263 0.47368421 0.52631579 0.57894737
- 0.63157895 0.68421053 0.73684211 0.78947368 0.84210526 0.89473684
- 0.94736842 1.        ]</t>
+          <t>[0.         0.11111111 0.22222222 0.33333333 0.44444444 0.55555556
+ 0.66666667 0.77777778 0.88888889 1.        ]</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -9161,10 +9168,8 @@
       <c r="B233" t="inlineStr"/>
       <c r="C233" t="inlineStr">
         <is>
-          <t>[0.         0.05263158 0.10526316 0.15789474 0.21052632 0.26315789
- 0.31578947 0.36842105 0.42105263 0.47368421 0.52631579 0.57894737
- 0.63157895 0.68421053 0.73684211 0.78947368 0.84210526 0.89473684
- 0.94736842 1.        ]</t>
+          <t>[0.         0.11111111 0.22222222 0.33333333 0.44444444 0.55555556
+ 0.66666667 0.77777778 0.88888889 1.        ]</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -9252,7 +9257,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>[ 0.58971311  1.69176047  3.29988048  7.61942099 10.93851804]</t>
+          <t>[0.48376794 1.91393545 3.38508001 5.95236759 7.78548957]</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -9274,7 +9279,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>[0.89366771 2.66278862 4.88079197 5.8239762  9.72007212]</t>
+          <t>[ 0.77555807  2.85313168  5.04057647  9.74351024 14.4304181 ]</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -9344,16 +9349,16 @@
   0.00435823 0.00435168 0.00430703 0.0042194  0.00408392 0.00389572
   0.00364992 0.00334165 0.00298133 0.00257936 0.00214615 0.00169212
   0.00122768 0.001      0.001      0.001      0.001      0.001     ]
- [0.         0.00935193 0.01778836 0.02520755 0.03160629 0.03726366
-  0.04197958 0.04437768 0.04562342 0.04536116 0.04363379 0.0413983
-  0.03865705 0.03598015 0.03345555 0.03130932 0.02938512 0.02757318
-  0.02588492 0.03255677 0.03944401 0.02690128 0.0201693  0.01698569
-  0.01515147 0.01327796 0.01137834 0.00952276 0.00768863 0.00587381]
- [0.         0.00935193 0.01778836 0.02520755 0.03160629 0.03726366
-  0.04197958 0.04437768 0.04562342 0.04536116 0.04363379 0.0413983
-  0.03865705 0.03598015 0.03345555 0.03130932 0.02938512 0.02757318
-  0.02588492 0.03255677 0.03944401 0.02690128 0.0201693  0.01698569
-  0.01515147 0.01327796 0.01137834 0.00952276 0.00768863 0.00587381]
+ [0.         0.00558896 0.01117792 0.01676688 0.02148023 0.02594341
+  0.03040659 0.03263711 0.0330815  0.03352589 0.03307007 0.03081386
+  0.02855764 0.02640753 0.0251063  0.02380507 0.02250383 0.04173291
+  0.06352828 0.08532365 0.08293418 0.0684523  0.05397041 0.04090187
+  0.02960001 0.01829814 0.00925718 0.00812939 0.0070016  0.00587381]
+ [0.         0.00558896 0.01117792 0.01676688 0.02148023 0.02594341
+  0.03040659 0.03263711 0.0330815  0.03352589 0.03307007 0.03081386
+  0.02855764 0.02640753 0.0251063  0.02380507 0.02250383 0.04173291
+  0.06352828 0.08532365 0.08293418 0.0684523  0.05397041 0.04090187
+  0.02960001 0.01829814 0.00925718 0.00812939 0.0070016  0.00587381]
  [0.         0.         0.00665003 0.00814812 0.00964621 0.0111443
   0.01260256 0.01398116 0.01524026 0.01634003 0.01724065 0.01790228
   0.01832761 0.01851932 0.01848012 0.01821267 0.01771968 0.01700382
@@ -9449,12 +9454,12 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -9474,7 +9479,7 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -9484,7 +9489,7 @@
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.         0.         0.         0.         0.         0.
   0.         0.         0.         0.         0.         0.
@@ -9551,12 +9556,12 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -9571,7 +9576,7 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -9581,7 +9586,7 @@
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.95925412 0.95895293 0.9565692  0.95388656 0.95056337 0.94780072
   0.9455854  0.94397287 0.94256868 0.94189525 0.94165198 0.94093289
@@ -9644,7 +9649,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>[ 12822625.22254687 -47407884.75872526        -0.        ]</t>
+          <t>[ 12551595.06251095 -47360632.37422645        -0.        ]</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -9760,7 +9765,7 @@
       <c r="B250" t="inlineStr"/>
       <c r="C250" t="inlineStr">
         <is>
-          <t>[2.]</t>
+          <t>[1.2]</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -9814,7 +9819,7 @@
       <c r="B253" t="inlineStr"/>
       <c r="C253" t="inlineStr">
         <is>
-          <t>[2.]</t>
+          <t>[1.2]</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -10280,7 +10285,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>[0.02]</t>
+          <t>[0.8]</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -10302,7 +10307,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>[0.8]</t>
+          <t>[0.02]</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -10360,16 +10365,16 @@
   0.00435823 0.00435168 0.00430703 0.0042194  0.00408392 0.00389572
   0.00364992 0.00334165 0.00298133 0.00257936 0.00214615 0.00169212
   0.00122768 0.001      0.001      0.001      0.001      0.001     ]
- [0.         0.00935193 0.01778836 0.02520755 0.03160629 0.03726366
-  0.04197958 0.04437768 0.04562342 0.04536116 0.04363379 0.0413983
-  0.03865705 0.03598015 0.03345555 0.03130932 0.02938512 0.02757318
-  0.02588492 0.03255677 0.03944401 0.02690128 0.0201693  0.01698569
-  0.01515147 0.01327796 0.01137834 0.00952276 0.00768863 0.00587381]
- [0.         0.00935193 0.01778836 0.02520755 0.03160629 0.03726366
-  0.04197958 0.04437768 0.04562342 0.04536116 0.04363379 0.0413983
-  0.03865705 0.03598015 0.03345555 0.03130932 0.02938512 0.02757318
-  0.02588492 0.03255677 0.03944401 0.02690128 0.0201693  0.01698569
-  0.01515147 0.01327796 0.01137834 0.00952276 0.00768863 0.00587381]
+ [0.         0.00558896 0.01117792 0.01676688 0.02148023 0.02594341
+  0.03040659 0.03263711 0.0330815  0.03352589 0.03307007 0.03081386
+  0.02855764 0.02640753 0.0251063  0.02380507 0.02250383 0.04173291
+  0.06352828 0.08532365 0.08293418 0.0684523  0.05397041 0.04090187
+  0.02960001 0.01829814 0.00925718 0.00812939 0.0070016  0.00587381]
+ [0.         0.00558896 0.01117792 0.01676688 0.02148023 0.02594341
+  0.03040659 0.03263711 0.0330815  0.03352589 0.03307007 0.03081386
+  0.02855764 0.02640753 0.0251063  0.02380507 0.02250383 0.04173291
+  0.06352828 0.08532365 0.08293418 0.0684523  0.05397041 0.04090187
+  0.02960001 0.01829814 0.00925718 0.00812939 0.0070016  0.00587381]
  [0.         0.         0.00665003 0.00814812 0.00964621 0.0111443
   0.01260256 0.01398116 0.01524026 0.01634003 0.01724065 0.01790228
   0.01832761 0.01851932 0.01848012 0.01821267 0.01771968 0.01700382
@@ -10465,12 +10470,12 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -10490,7 +10495,7 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -10500,7 +10505,7 @@
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.         0.         0.         0.         0.         0.
   0.         0.         0.         0.         0.         0.
@@ -10567,12 +10572,12 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -10587,7 +10592,7 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -10597,7 +10602,7 @@
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.95925412 0.95895293 0.9565692  0.95388656 0.95056337 0.94780072
   0.9455854  0.94397287 0.94256868 0.94189525 0.94165198 0.94093289
@@ -10769,14 +10774,14 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>[-3.48176418e+07 -3.26389882e+07 -2.92716934e+07 -3.19960854e+07
- -3.11989678e+07 -2.99064659e+07 -2.88189400e+07 -2.75536837e+07
- -2.56726448e+07 -2.32654324e+07 -2.07774528e+07 -1.83832677e+07
- -1.61037967e+07 -1.39572094e+07 -1.19590939e+07 -1.01150856e+07
- -8.42836025e+06 -6.90453071e+06 -5.54903682e+06 -4.36358600e+06
- -3.34616543e+06 -2.48286920e+06 -1.75960673e+06 -1.18496156e+06
- -7.48517220e+05 -4.32339997e+05 -2.16572064e+05 -8.36799124e+04
- -1.71054148e+04  2.83850017e+00]</t>
+          <t>[-3.49475571e+07 -3.27227091e+07 -3.12035510e+07 -3.40649595e+07
+ -3.25038652e+07 -3.08643310e+07 -2.93712780e+07 -2.76651160e+07
+ -2.54786421e+07 -2.29635206e+07 -2.04477650e+07 -1.80461145e+07
+ -1.57738394e+07 -1.36445712e+07 -1.16723102e+07 -9.86345069e+06
+ -8.22088493e+06 -6.74834090e+06 -5.44164119e+06 -4.29289835e+06
+ -3.31671456e+06 -2.47551879e+06 -1.76914295e+06 -1.19522074e+06
+ -7.57111476e+05 -4.39065623e+05 -2.20785699e+05 -8.54283199e+04
+ -1.75485171e+04  3.01134316e+00]</t>
         </is>
       </c>
       <c r="D283" t="inlineStr">
@@ -10798,14 +10803,14 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>[ 3.46361181e+07  3.25690789e+07  3.16723777e+07  2.42880821e+07
-  2.03409180e+07  1.69123952e+07  1.27651238e+07  8.17190417e+06
-  4.29760102e+06  2.52610201e+06  1.96553843e+06  1.53341102e+06
-  1.18081099e+06  8.75478933e+05  5.51845758e+05  2.37571304e+05
- -1.16923027e+04 -1.57155828e+05 -2.11192828e+05 -1.93997314e+05
- -1.56239687e+05 -1.77002675e+05 -2.05047295e+05 -1.94972087e+05
- -1.59687243e+05 -1.10136881e+05 -6.15145142e+04 -2.54398971e+04
- -5.54443133e+03  9.37112041e-02]</t>
+          <t>[ 3.43400918e+07  3.22608410e+07  2.94824675e+07  2.08362140e+07
+  1.76112084e+07  1.43746365e+07  1.04687516e+07  6.32816123e+06
+  3.00404280e+06  1.63019453e+06  1.33881701e+06  1.08276032e+06
+  8.42829073e+05  6.35584012e+05  4.00694135e+05  1.54319027e+05
+ -5.16331437e+04 -4.66363925e+04  1.15751955e+05  2.37519564e+05
+ -3.81283481e+04 -1.65991616e+05 -1.38048934e+05 -1.84504514e+05
+ -1.64668214e+05 -1.14022991e+05 -6.25543725e+04 -2.56714985e+04
+ -5.62488618e+03  9.62241177e-02]</t>
         </is>
       </c>
       <c r="D284" t="inlineStr">
@@ -10827,14 +10832,14 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>[ 6.34509588e+05  6.32399112e+05  6.06559344e+05  7.02049212e+05
-  7.30612347e+05  7.49174784e+05  7.72904831e+05  7.92222826e+05
-  7.93250671e+05  7.75947406e+05  7.50568152e+05  7.20397053e+05
-  6.85032483e+05  6.44904686e+05  6.00952595e+05  5.54032281e+05
-  5.05142628e+05  4.55000711e+05  4.04309168e+05  3.53652171e+05
-  2.99688337e+05  2.46335801e+05  2.00944807e+05  1.55971782e+05
-  1.16085825e+05  8.25695642e+04  5.44152764e+04  3.09274739e+04
-  1.23548449e+04 -6.72107320e+02]</t>
+          <t>[ 6.48030117e+05  6.45869090e+05  6.57101741e+05  7.59727994e+05
+  7.75643883e+05  7.89436595e+05  8.06116323e+05  8.16139092e+05
+  8.10035043e+05  7.90301618e+05  7.64476750e+05  7.34092595e+05
+  6.98645796e+05  6.58484127e+05  6.14496817e+05  5.67587098e+05
+  5.18796200e+05  4.68801734e+05  4.17335598e+05  3.64316996e+05
+  3.05716034e+05  2.47805650e+05  2.03363417e+05  1.56575169e+05
+  1.15658742e+05  8.20225437e+04  5.42738925e+04  3.10874176e+04
+  1.24867633e+04 -5.93718997e+02]</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
@@ -11168,16 +11173,16 @@
   0.00435823 0.00435168 0.00430703 0.0042194  0.00408392 0.00389572
   0.00364992 0.00334165 0.00298133 0.00257936 0.00214615 0.00169212
   0.00122768 0.001      0.001      0.001      0.001      0.001     ]
- [0.         0.01036386 0.01802123 0.02536166 0.03206819 0.03782389
-  0.04231181 0.045215   0.04621651 0.04569527 0.04403017 0.04160014
-  0.03878408 0.03596091 0.03350953 0.03135807 0.02943466 0.02766741
-  0.02598444 0.02431388 0.02258386 0.02080428 0.01898505 0.01713608
-  0.0152673  0.0133886  0.0115099  0.0096312  0.0077525  0.00587381]
- [0.         0.01247806 0.01761157 0.02274509 0.02766418 0.03215441
-  0.03600136 0.0389906  0.04090771 0.04153826 0.04110173 0.03981761
-  0.0379054  0.03558457 0.03307463 0.03059505 0.02815655 0.02576987
-  0.02344572 0.02119482 0.01902789 0.01695567 0.01496235 0.01303217
-  0.01114933 0.00929806 0.00746257 0.00562708 0.00379159 0.00195611]
+ [0.         0.00583337 0.01166673 0.0175001  0.02246982 0.02719278
+  0.03191574 0.03417685 0.03446848 0.0347601  0.03413613 0.03168096
+  0.02922579 0.02681664 0.02477562 0.0227346  0.02069359 0.04046992
+  0.06297342 0.08547692 0.08260286 0.06704002 0.05147718 0.03807502
+  0.02737371 0.01667241 0.00817846 0.00741024 0.00664202 0.00587381]
+ [0.         0.00583337 0.01166673 0.0175001  0.02246982 0.02719278
+  0.03191574 0.03417685 0.03446848 0.0347601  0.03413613 0.03168096
+  0.02922579 0.02681664 0.02477562 0.0227346  0.02069359 0.04046992
+  0.06297342 0.08547692 0.08260286 0.06704002 0.05147718 0.03807502
+  0.02737371 0.01667241 0.00817846 0.00741024 0.00664202 0.00587381]
  [0.         0.         0.00665003 0.00814812 0.00964621 0.0111443
   0.01260256 0.01398116 0.01524026 0.01634003 0.01724065 0.01790228
   0.01832761 0.01851932 0.01848012 0.01821267 0.01771968 0.01700382
@@ -11273,12 +11278,12 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -11298,7 +11303,7 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -11308,7 +11313,7 @@
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.         0.         0.         0.         0.         0.
   0.         0.         0.         0.         0.         0.
@@ -11375,12 +11380,12 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -11395,7 +11400,7 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -11405,7 +11410,7 @@
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.95925412 0.95895293 0.9565692  0.95388656 0.95056337 0.94780072
   0.9455854  0.94397287 0.94256868 0.94189525 0.94165198 0.94093289
@@ -11864,7 +11869,7 @@
       <c r="B321" t="inlineStr"/>
       <c r="C321" t="inlineStr">
         <is>
-          <t>[976.61986675]</t>
+          <t>[786.34407823]</t>
         </is>
       </c>
       <c r="D321" t="inlineStr">
@@ -12269,7 +12274,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>[2.05575658e+08 1.02787829e+08 1.02787829e+08 0.00000000e+00
+          <t>[2.47961882e+08 1.23980941e+08 1.23980941e+08 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -12384,7 +12389,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>[33987318.11456916]</t>
+          <t>[40994928.44980011]</t>
         </is>
       </c>
       <c r="D348" t="inlineStr"/>
@@ -12724,7 +12729,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>[50995.25314794]</t>
+          <t>[52661.47228171]</t>
         </is>
       </c>
       <c r="D368" t="inlineStr"/>
@@ -12792,7 +12797,7 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>[-47407884.75872526]</t>
+          <t>[-47360632.37422645]</t>
         </is>
       </c>
       <c r="D372" t="inlineStr"/>
@@ -12810,7 +12815,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>[24267.56957112]</t>
+          <t>[24855.33719394]</t>
         </is>
       </c>
       <c r="D373" t="inlineStr"/>
@@ -12846,7 +12851,7 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>[218408.12614006 109204.06307003 109204.06307003      0.
+          <t>[223698.03474543 111849.01737272 111849.01737272      0.
       0.              0.        ]</t>
         </is>
       </c>
@@ -12865,7 +12870,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>[7006.7224947]</t>
+          <t>[8453.66722938]</t>
         </is>
       </c>
       <c r="D376" t="inlineStr"/>
@@ -12901,7 +12906,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>[2.75289412]</t>
+          <t>[2.75301885]</t>
         </is>
       </c>
       <c r="D378" t="inlineStr"/>
@@ -12919,7 +12924,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>[42040.3349682 42040.3349682 42040.3349682     0.            0.
+          <t>[50722.0033763 50722.0033763 50722.0033763     0.            0.
      0.       ]</t>
         </is>
       </c>
@@ -14876,7 +14881,7 @@
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>[152985.75944382]</t>
+          <t>[157984.41684513]</t>
         </is>
       </c>
       <c r="D487" t="inlineStr"/>
@@ -14894,7 +14899,7 @@
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>[34375.31495201]</t>
+          <t>[36410.02730951]</t>
         </is>
       </c>
       <c r="D488" t="inlineStr"/>
@@ -14930,7 +14935,7 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>[2.77518573]</t>
+          <t>[2.7740541]</t>
         </is>
       </c>
       <c r="D490" t="inlineStr"/>
@@ -14966,7 +14971,7 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>[289520.55066633 180488.75850131 180488.75850131      0.
+          <t>[303492.1276798  191816.16096321 191816.16096321      0.
       0.              0.        ]</t>
         </is>
       </c>
@@ -15351,9 +15356,9 @@
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>[[ 2123166.21289209]
+          <t>[[ 2121774.35772799]
  [   41405.87527761]
- [-1166445.32177558]]</t>
+ [-1186349.77795496]]</t>
         </is>
       </c>
       <c r="D513" t="inlineStr"/>
@@ -15452,8 +15457,8 @@
       <c r="C518" t="inlineStr">
         <is>
           <t>[[     -0.        ]
- [3866283.78687793]
- [2687385.72469201]]</t>
+ [3881455.07317849]
+ [2687372.49074165]]</t>
         </is>
       </c>
       <c r="D518" t="inlineStr"/>
@@ -15471,9 +15476,9 @@
       </c>
       <c r="C519" t="inlineStr">
         <is>
-          <t>[[37769251.53853859]
- [      -0.        ]
- [      -0.        ]]</t>
+          <t>[[37769251.5385386]
+ [      -0.       ]
+ [      -0.       ]]</t>
         </is>
       </c>
       <c r="D519" t="inlineStr"/>
@@ -16801,7 +16806,7 @@
       </c>
       <c r="C589" t="inlineStr">
         <is>
-          <t>[421443.65817399]</t>
+          <t>[428477.0279328]</t>
         </is>
       </c>
       <c r="D589" t="inlineStr"/>
@@ -16819,8 +16824,8 @@
       </c>
       <c r="C590" t="inlineStr">
         <is>
-          <t>[ 2.08546242e+08  1.32824718e+08  1.31782070e+08 -1.66639598e+01
- -6.43161299e+05  4.82222779e+04]</t>
+          <t>[ 2.50905849e+08  1.55068890e+08  1.54066831e+08 -1.66639598e+01
+ -1.87087268e+06  4.82222779e+04]</t>
         </is>
       </c>
       <c r="D590" t="inlineStr"/>
@@ -16838,7 +16843,7 @@
       </c>
       <c r="C591" t="inlineStr">
         <is>
-          <t>[-5.21344714 -0.07454204  2.09295425]</t>
+          <t>[-5.32135284 -0.07331844  2.10755   ]</t>
         </is>
       </c>
       <c r="D591" t="inlineStr"/>
@@ -17448,7 +17453,7 @@
       </c>
       <c r="C623" t="inlineStr">
         <is>
-          <t>[ 2199361.42160199    41405.95953997 -2466864.63319846]</t>
+          <t>[ 2199361.16592555    41406.03687367 -2486818.06298609]</t>
         </is>
       </c>
       <c r="D623" t="inlineStr"/>
@@ -17466,7 +17471,7 @@
       </c>
       <c r="C624" t="inlineStr">
         <is>
-          <t>[15682220.2180832   2135803.94066418  1127332.34182628]</t>
+          <t>[15682220.23527616  2104472.63685562  1127331.99235724]</t>
         </is>
       </c>
       <c r="D624" t="inlineStr"/>
@@ -17991,7 +17996,7 @@
       </c>
       <c r="C652" t="inlineStr">
         <is>
-          <t>[2199361.42160199]</t>
+          <t>[2199361.16592555]</t>
         </is>
       </c>
       <c r="D652" t="inlineStr"/>
@@ -18009,7 +18014,7 @@
       </c>
       <c r="C653" t="inlineStr">
         <is>
-          <t>[41405.95953997]</t>
+          <t>[41406.03687367]</t>
         </is>
       </c>
       <c r="D653" t="inlineStr"/>
@@ -18027,7 +18032,7 @@
       </c>
       <c r="C654" t="inlineStr">
         <is>
-          <t>[-2466864.63319846]</t>
+          <t>[-2486818.06298609]</t>
         </is>
       </c>
       <c r="D654" t="inlineStr"/>
@@ -18045,7 +18050,7 @@
       </c>
       <c r="C655" t="inlineStr">
         <is>
-          <t>[15682220.2180832]</t>
+          <t>[15682220.23527616]</t>
         </is>
       </c>
       <c r="D655" t="inlineStr"/>
@@ -18063,7 +18068,7 @@
       </c>
       <c r="C656" t="inlineStr">
         <is>
-          <t>[2135803.94066418]</t>
+          <t>[2104472.63685562]</t>
         </is>
       </c>
       <c r="D656" t="inlineStr"/>
@@ -18081,7 +18086,7 @@
       </c>
       <c r="C657" t="inlineStr">
         <is>
-          <t>[1127332.34182628]</t>
+          <t>[1127331.99235724]</t>
         </is>
       </c>
       <c r="D657" t="inlineStr"/>
@@ -18245,14 +18250,14 @@
       </c>
       <c r="C665" t="inlineStr">
         <is>
-          <t>[-9931629.12087864 -9492004.72238001 -9052380.32388137 -8659115.29522039
- -8265850.26655938 -7872585.23789839 -7523691.55816138 -7174797.87842438
- -6825904.19868737 -6515970.87015947 -6206037.54163157 -5896104.21310369
- -5622459.95773027 -5348815.70235683 -5075171.44698341 -4837701.64147476
- -4600231.83596612 -4362762.0304575  -4161055.65345227 -3959349.27644706
- -3757642.89944181 -3589530.81123417 -3421418.72302654 -3253306.63481891
- -3113092.20878868 -2973733.87135341 -2835231.63344629 -2709850.8539877
- -2587061.8575495  -2466864.63319846]</t>
+          <t>[-9951582.55066614 -9511958.15216751 -9072333.75366888 -8679068.72500789
+ -8285803.69634688 -7892538.66768589 -7543644.98794887 -7194751.30821188
+ -6845857.62847487 -6535924.29994697 -6225990.97141909 -5916057.64289117
+ -5642413.3875178  -5368769.13214438 -5095124.87677096 -4857655.07126236
+ -4620185.26575373 -4382715.4602451  -4181009.08323988 -3979302.70623463
+ -3777596.32922941 -3609484.24102176 -3441372.15281411 -3273260.06460648
+ -3133045.63857625 -2993687.301141   -2855185.06323387 -2729804.28377531
+ -2607015.28733709 -2486818.06298608]</t>
         </is>
       </c>
       <c r="D665" t="inlineStr"/>
@@ -18270,14 +18275,14 @@
       </c>
       <c r="C666" t="inlineStr">
         <is>
-          <t>[2280562.64427271 2279770.05413786 2278672.81598016 2277253.63856015
- 2275732.35833533 2274043.21671441 2272030.05823047 2270053.33291015
- 2267950.19580608 2265500.8753819  2263168.55372593 2260731.31672743
- 2257913.05778896 2255280.40975585 2252556.37080163 2249398.64370402
- 2246501.6974388  2243522.81235573 2240061.78120053 2236926.30139759
- 2233715.94206915 2230001.97457721 2226647.5214219  2223223.70876772
- 2219347.82260043 2215810.02359946 2212229.49023216 2208447.70998157
- 2204837.86516156 2201243.30517403]</t>
+          <t>[2280562.39752461 2279769.82516708 2278672.60460251 2277253.43891874
+ 2275732.17555393 2274043.0502648  2272029.89658648 2270053.18618753
+ 2267950.06313824 2265500.74143011 2263168.43175552 2260731.20554176
+ 2257912.93876146 2255280.29880151 2252556.26640344 2249398.52413985
+ 2246501.58111301 2243522.69746062 2240061.64495677 2236926.16270557
+ 2233715.79884497 2230001.8068529  2226647.34477608 2223223.5208791
+ 2219347.6113174  2215809.79584213 2212229.24333136 2208447.44141973
+ 2204837.57149407 2201242.98291472]</t>
         </is>
       </c>
       <c r="D666" t="inlineStr"/>
@@ -18295,14 +18300,14 @@
       </c>
       <c r="C667" t="inlineStr">
         <is>
-          <t>[41401.1098487  41390.8990243  41380.51372095 41373.22447787
- 41362.5188499  41351.64440961 41347.38331438 41336.19915007
- 41324.85121511 41323.06853921 41311.41831745 41299.60875452
- 41300.82174096 41288.71741515 41276.45761438 41282.01341695
- 41269.46666053 41256.76785922 41267.38656577 41254.40769817
- 41241.27998078 41256.57123133 41243.16897376 41229.62106681
- 41246.31712174 41233.34537042 41220.14177334 41223.71171475
- 41212.23825929 41200.27735505]</t>
+          <t>[41401.18551928 41390.97136982 41380.5827479  41373.2912497
+ 41362.5823369  41351.7046329  41347.44241337 41336.25504951
+ 41324.90395267 41323.1210767  41311.46779132 41299.6552213
+ 41300.86904498 41288.76184978 41276.49925778 41282.05724227
+ 41269.50787807 41256.80657225 41267.42886736 41254.44773215
+ 41241.31788054 41256.61385096 41243.20976042 41229.6601903
+ 41246.36119382 41233.3883504  41220.18387274 41223.75629844
+ 41212.28288922 41200.32232042]</t>
         </is>
       </c>
       <c r="D667" t="inlineStr"/>
@@ -18320,14 +18325,14 @@
       </c>
       <c r="C668" t="inlineStr">
         <is>
-          <t>[10873069.40812827 11059049.17163842 11243118.5144097  11425323.66089842
- 11605674.86920421 11784335.27992343 11961350.62867679 12136698.20588863
- 12310551.54049785 12482965.2016698  12653898.90033725 12823536.29826988
- 12991933.21968439 13159018.92345533 13324986.751249   13489880.15524416
- 13653571.12292981 13816261.93245484 13977974.43914849 14138507.18803503
- 14298070.56567955 14456660.41819829 14614001.05176772 14770310.19945163
- 14925566.84352306 15079436.13724521 15232084.82694429 15383532.24029338
- 15533572.27781731 15682226.55215925]</t>
+          <t>[10876605.76965806 11062578.61179022 11246636.11783682 11428824.22239867
+ 11609152.86208236 11787785.16332132 11964766.50090758 12140073.75971516
+ 12313880.44867646 12486240.72048981 12657113.8158561  12826683.36918215
+ 12995004.69444892 13162006.47474091 13327882.01459575 13492674.0852527
+ 13656253.90966897 13818823.71530198 13980404.4223942  14140793.53596996
+ 14300201.37354428 14458622.51067519 14615779.85780394 14771891.05533159
+ 14926933.46794325 15080570.33000097 15232967.91770947 15384143.9746539
+ 15533890.20674071 15682226.56941667]</t>
         </is>
       </c>
       <c r="D668" t="inlineStr"/>
@@ -18345,14 +18350,14 @@
       </c>
       <c r="C669" t="inlineStr">
         <is>
-          <t>[3.10579367e+08 3.00074687e+08 2.89524225e+08 2.78932991e+08
- 2.68305283e+08 2.57648563e+08 2.46966951e+08 2.36263308e+08
- 2.25544286e+08 2.14813680e+08 2.04073538e+08 1.93329802e+08
- 1.82585846e+08 1.71842844e+08 1.61106073e+08 1.50378355e+08
- 1.39659812e+08 1.28955097e+08 1.18266530e+08 1.07593320e+08
- 9.69395530e+07 8.63071897e+07 7.56949521e+07 6.51064059e+07
- 5.45433984e+07 4.40047383e+07 3.34931699e+07 2.30106844e+07
- 1.25576362e+07 2.13580689e+06]</t>
+          <t>[3.10598174e+08 3.00093301e+08 2.89542528e+08 2.78950859e+08
+ 2.68322594e+08 2.57665196e+08 2.46982785e+08 2.36278220e+08
+ 2.25558160e+08 2.14826396e+08 2.04084977e+08 1.93339852e+08
+ 1.82594392e+08 1.71849773e+08 1.61111278e+08 1.50381728e+08
+ 1.39661246e+08 1.28954495e+08 1.18263790e+08 1.07588346e+08
+ 9.69322558e+07 8.62974805e+07 7.56827467e+07 6.50916311e+07
+ 5.45259834e+07 4.39846201e+07 3.34702978e+07 2.29850165e+07
+ 1.25291438e+07 2.10447557e+06]</t>
         </is>
       </c>
       <c r="D669" t="inlineStr"/>
@@ -18370,14 +18375,14 @@
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>[1127486.62417985 1127480.08348777 1127473.54287157 1127482.87867613
- 1127476.33802734 1127469.79745443 1127479.90856295 1127473.3679488
- 1127466.82741054 1127476.37242403 1127469.83185071 1127463.29135328
- 1127473.25137812 1127466.71084154 1127460.17038084 1127472.10847033
- 1127465.56794643 1127459.02749841 1127473.79208699 1127467.25154368
- 1127460.71107625 1127478.51922755 1127471.97862944 1127465.43810721
- 1127484.08113859 1127478.43255931 1127472.75465461 1127480.22606922
- 1127476.66926903 1127473.10010393]</t>
+          <t>[1127486.57153003 1127480.03083652 1127473.49021891 1127482.86102093
+ 1127476.32037032 1127469.77979559 1127479.93311182 1127473.39249536
+ 1127466.85195479 1127476.44399328 1127469.90341711 1127463.36291682
+ 1127473.3787872  1127466.83824711 1127460.2977829  1127472.30852958
+ 1127465.76800132 1127459.22754896 1127474.08958915 1127467.54904036
+ 1127461.00856745 1127478.94602959 1127472.4054245  1127465.8648953
+ 1127484.66240744 1127479.01953842 1127473.34741464 1127480.91745227
+ 1127477.38261744 1127473.83636465]</t>
         </is>
       </c>
       <c r="D670" t="inlineStr"/>
@@ -18455,7 +18460,7 @@
       </c>
       <c r="C674" t="inlineStr">
         <is>
-          <t>[0.46294619]</t>
+          <t>[0.46290446]</t>
         </is>
       </c>
       <c r="D674" t="inlineStr"/>
@@ -18489,7 +18494,7 @@
       </c>
       <c r="C676" t="inlineStr">
         <is>
-          <t>[12.50700477]</t>
+          <t>[12.73527134]</t>
         </is>
       </c>
       <c r="D676" t="inlineStr"/>
@@ -18705,7 +18710,7 @@
       </c>
       <c r="C686" t="inlineStr">
         <is>
-          <t>[50995.25314794]</t>
+          <t>[52661.47228171]</t>
         </is>
       </c>
       <c r="D686" t="inlineStr"/>
@@ -18741,7 +18746,7 @@
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>[436863.13576807]</t>
+          <t>[479007.74999438]</t>
         </is>
       </c>
       <c r="D688" t="inlineStr"/>
@@ -18759,7 +18764,7 @@
       </c>
       <c r="C689" t="inlineStr">
         <is>
-          <t>[7006.7224947]</t>
+          <t>[8453.66722938]</t>
         </is>
       </c>
       <c r="D689" t="inlineStr"/>
@@ -18795,7 +18800,7 @@
       </c>
       <c r="C691" t="inlineStr">
         <is>
-          <t>[24267.56957112]</t>
+          <t>[24855.33719394]</t>
         </is>
       </c>
       <c r="D691" t="inlineStr"/>
@@ -18867,7 +18872,7 @@
       </c>
       <c r="C695" t="inlineStr">
         <is>
-          <t>[27326.21772933]</t>
+          <t>[32969.3021946]</t>
         </is>
       </c>
       <c r="D695" t="inlineStr"/>
@@ -18885,7 +18890,7 @@
       </c>
       <c r="C696" t="inlineStr">
         <is>
-          <t>[536313.2875217]</t>
+          <t>[549302.95198601]</t>
         </is>
       </c>
       <c r="D696" t="inlineStr"/>
@@ -18977,7 +18982,7 @@
       </c>
       <c r="C702" t="inlineStr">
         <is>
-          <t>[436863.13576807]</t>
+          <t>[479007.74999438]</t>
         </is>
       </c>
       <c r="D702" t="inlineStr"/>
@@ -18995,7 +19000,7 @@
       </c>
       <c r="C703" t="inlineStr">
         <is>
-          <t>[598060.85928779]</t>
+          <t>[616693.60821736]</t>
         </is>
       </c>
       <c r="D703" t="inlineStr"/>
@@ -19013,7 +19018,7 @@
       </c>
       <c r="C704" t="inlineStr">
         <is>
-          <t>[34375.31495201]</t>
+          <t>[36410.02730951]</t>
         </is>
       </c>
       <c r="D704" t="inlineStr"/>
@@ -20091,7 +20096,7 @@
       </c>
       <c r="C766" t="inlineStr">
         <is>
-          <t>[1908650.266592]</t>
+          <t>[2053716.85820051]</t>
         </is>
       </c>
       <c r="D766" t="inlineStr"/>
@@ -20109,7 +20114,7 @@
       </c>
       <c r="C767" t="inlineStr">
         <is>
-          <t>[187361.07439584]</t>
+          <t>[194394.44415464]</t>
         </is>
       </c>
       <c r="D767" t="inlineStr"/>
@@ -20237,7 +20242,7 @@
       </c>
       <c r="C775" t="inlineStr">
         <is>
-          <t>[6730303.87151292]</t>
+          <t>[6875370.46312143]</t>
         </is>
       </c>
       <c r="D775" t="inlineStr"/>
@@ -20255,7 +20260,7 @@
       </c>
       <c r="C776" t="inlineStr">
         <is>
-          <t>[1346.0607743]</t>
+          <t>[1375.07409262]</t>
         </is>
       </c>
       <c r="D776" t="inlineStr"/>
@@ -20273,7 +20278,7 @@
       </c>
       <c r="C777" t="inlineStr">
         <is>
-          <t>[1283916.81761933]</t>
+          <t>[1290950.18737814]</t>
         </is>
       </c>
       <c r="D777" t="inlineStr"/>
@@ -20463,7 +20468,7 @@
       </c>
       <c r="C788" t="inlineStr">
         <is>
-          <t>[50995.25314794]</t>
+          <t>[52661.47228171]</t>
         </is>
       </c>
       <c r="D788" t="inlineStr">
@@ -20485,7 +20490,7 @@
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>[34375.31495201]</t>
+          <t>[36410.02730951]</t>
         </is>
       </c>
       <c r="D789" t="inlineStr">
@@ -21907,10 +21912,10 @@
         <is>
           <t xml:space="preserve">{'components':   Component  Mass tonne  Lift height m  Surface area sq m  Coeff drag  Coeff drag (installed)  Section height m  Lever arm m  Cycle time installation hrs  Offload hook height m  Offload cycle time hrs  Multplier drag rotor  Multiplier tower drag Operation
 0   Nacelle  234.082584     140.000000          33.000000         0.8                     0.8          0.000000    80.000000                          1.5                      6                     0.5              1.000000                      0       Top
-1       Hub   34.387161     140.000000          11.300000         1.1                     1.1          0.000000    80.000000                          1.0                      6                     0.5              0.000000                      0       Top
-2   Blade 1   51.003992     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
-2   Blade 2   51.003992     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
-2   Blade 3   51.003992     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
+1       Hub   36.410027     140.000000          11.300000         1.1                     1.1          0.000000    80.000000                          1.0                      6                     0.5              0.000000                      0       Top
+2   Blade 1   52.661472     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
+2   Blade 2   52.661472     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
+2   Blade 3   52.661472     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
 5   Tower 1   78.406651      12.727273          67.572802         0.6                     1.1         12.727273     6.363636                          1.0                      6                     0.5              0.000000                      1      Base
 5   Tower 2   78.406651      25.454545          67.572802         0.6                     1.1         12.727273    19.090909                          1.0                      6                     0.5              0.000000                      1      Base
 5   Tower 3   78.406651      38.181818          67.572802         0.6                     1.1         12.727273    31.818182                          1.0                      6                     0.5              0.000000                      1      Base
@@ -22116,7 +22121,7 @@
       </c>
       <c r="C852" t="inlineStr">
         <is>
-          <t>[1346.0607743]</t>
+          <t>[1375.07409262]</t>
         </is>
       </c>
       <c r="D852" t="inlineStr"/>
@@ -22286,7 +22291,7 @@
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>[50995.25314794]</t>
+          <t>[52661.47228171]</t>
         </is>
       </c>
       <c r="D862" t="inlineStr"/>
@@ -22304,7 +22309,7 @@
       </c>
       <c r="C863" t="inlineStr">
         <is>
-          <t>[38.02842356]</t>
+          <t>[38.54575678]</t>
         </is>
       </c>
       <c r="D863" t="inlineStr"/>
@@ -22454,7 +22459,7 @@
       </c>
       <c r="C872" t="inlineStr">
         <is>
-          <t>[12.50700477]</t>
+          <t>[12.73527134]</t>
         </is>
       </c>
       <c r="D872" t="inlineStr"/>
@@ -24625,10 +24630,8 @@
       <c r="B937" t="inlineStr"/>
       <c r="C937" t="inlineStr">
         <is>
-          <t>[0.         0.05263158 0.10526316 0.15789474 0.21052632 0.26315789
- 0.31578947 0.36842105 0.42105263 0.47368421 0.52631579 0.57894737
- 0.63157895 0.68421053 0.73684211 0.78947368 0.84210526 0.89473684
- 0.94736842 1.        ]</t>
+          <t>[0.         0.11111111 0.22222222 0.33333333 0.44444444 0.55555556
+ 0.66666667 0.77777778 0.88888889 1.        ]</t>
         </is>
       </c>
       <c r="D937" t="inlineStr"/>
@@ -24642,10 +24645,8 @@
       <c r="B938" t="inlineStr"/>
       <c r="C938" t="inlineStr">
         <is>
-          <t>[0.         0.05263158 0.10526316 0.15789474 0.21052632 0.26315789
- 0.31578947 0.36842105 0.42105263 0.47368421 0.52631579 0.57894737
- 0.63157895 0.68421053 0.73684211 0.78947368 0.84210526 0.89473684
- 0.94736842 1.        ]</t>
+          <t>[0.         0.11111111 0.22222222 0.33333333 0.44444444 0.55555556
+ 0.66666667 0.77777778 0.88888889 1.        ]</t>
         </is>
       </c>
       <c r="D938" t="inlineStr"/>
@@ -24663,10 +24664,8 @@
       </c>
       <c r="C939" t="inlineStr">
         <is>
-          <t>[0.         0.014274   0.02559803 0.035278   0.042476   0.04572004
- 0.04531975 0.04226395 0.03807994 0.03402034 0.03074453 0.02792861
- 0.02535178 0.04142444 0.02228027 0.01717876 0.01437916 0.011476
- 0.0086438  0.00587381]</t>
+          <t>[0.         0.01800887 0.03239023 0.03382215 0.02655211 0.02235925
+ 0.09258877 0.04592492 0.0095078  0.00587381]</t>
         </is>
       </c>
       <c r="D939" t="inlineStr"/>
@@ -24684,10 +24683,8 @@
       </c>
       <c r="C940" t="inlineStr">
         <is>
-          <t>[0.         0.01439406 0.02571464 0.03540044 0.04261741 0.04584753
- 0.04543236 0.04236752 0.03818973 0.03415463 0.03085191 0.02803946
- 0.0254569  0.02285702 0.02013403 0.01733071 0.01447627 0.01160878
- 0.00874129 0.00587381]</t>
+          <t>[0.         0.01860448 0.03292068 0.03434412 0.02708432 0.02289096
+ 0.0845189  0.04403153 0.010066   0.00587381]</t>
         </is>
       </c>
       <c r="D940" t="inlineStr"/>
@@ -26287,7 +26284,7 @@
       <c r="B972" t="inlineStr"/>
       <c r="C972" t="inlineStr">
         <is>
-          <t>[2000.]</t>
+          <t>[0.]</t>
         </is>
       </c>
       <c r="D972" t="inlineStr">
@@ -26602,12 +26599,12 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -26627,7 +26624,7 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -26637,7 +26634,7 @@
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.         0.         0.         0.         0.         0.
   0.         0.         0.         0.         0.         0.
@@ -26704,12 +26701,12 @@
  [0.22272986 0.22632952 0.22948212 0.30080193 0.31138242 0.32272784
   0.33028459 0.33580147 0.33842316 0.33783338 0.33690305 0.33920465
   0.34192828 0.35209392 0.35827412 0.36697208 0.37551861 0.38277512
-  0.38964944 0.39578046 0.40125954 0.40631466 0.41134025 0.41753853
+  0.38964944 0.39578046 0.48232206 0.40631466 0.41134025 0.41753853
   0.41993132 0.42260813 0.42604197 0.43129105 0.43340579 0.41037074]
  [0.72273926 0.72686687 0.73692268 0.68392783 0.69466754 0.70325628
   0.71188804 0.71980021 0.72485974 0.72743733 0.7296189  0.72912358
   0.72821111 0.72164078 0.72019359 0.71820211 0.71699693 0.71742121
-  0.7190506  0.72270791 0.72871712 0.73735997 0.74903991 0.76192904
+  0.7190506  0.72270791 0.80977964 0.73735997 0.74903991 0.76192904
   0.77438828 0.79040881 0.81299166 0.84716618 0.89494952 0.91659409]
  [0.51094271 0.51093158 0.51109232 0.51151394 0.51274861 0.51314609
   0.51310658 0.51395159 0.51467968 0.51507905 0.51562235 0.51627311
@@ -26724,7 +26721,7 @@
  [0.16613836 0.16946286 0.16968068 0.23759495 0.2439899  0.25193115
   0.25766523 0.26174662 0.2633434  0.26210837 0.26061866 0.2616315
   0.26295985 0.26995749 0.2725209  0.27588271 0.27838647 0.27891556
-  0.27802616 0.2750634  0.26980807 0.26207131 0.25166728 0.23859669
+  0.27802616 0.2750634  0.18874555 0.26207131 0.25166728 0.23859669
   0.22787547 0.21289915 0.19074836 0.15633559 0.10381686 0.08009451]
  [0.48905595 0.48893839 0.48796411 0.48706864 0.48668455 0.48576547
   0.48502104 0.48531088 0.48564258 0.4857924  0.48611936 0.48627169
@@ -26734,7 +26731,7 @@
  [0.66614777 0.6700002  0.67712123 0.62072086 0.62727502 0.63245959
   0.63926867 0.64574535 0.64977998 0.65171232 0.65333451 0.65155042
   0.64924268 0.63950434 0.63444037 0.62711273 0.61986479 0.61356165
-  0.60742732 0.60199085 0.59726565 0.59311662 0.58936694 0.58623052
+  0.60742732 0.60199085 0.51620312 0.59311662 0.58936694 0.58623052
   0.58444769 0.58188815 0.57826958 0.57270573 0.57374879 0.59684729]
  [0.95925412 0.95895293 0.9565692  0.95388656 0.95056337 0.94780072
   0.9455854  0.94397287 0.94256868 0.94189525 0.94165198 0.94093289
@@ -26805,10 +26802,10 @@
    0.     0.     0.     0.     0.     0.     0.     0.     0.     0.   ]
  [ 0.     0.     0.    -0.8   -0.768 -0.736 -0.704 -0.672 -0.64  -0.608
   -0.576 -0.544 -0.512 -0.48  -0.448 -0.416 -0.384 -0.352 -0.32  -0.288
-  -0.256 -0.224 -0.192 -0.16  -0.128 -0.096 -0.064 -0.032  0.     0.   ]
+   0.    -0.224 -0.192 -0.16  -0.128 -0.096 -0.064 -0.032  0.     0.   ]
  [ 0.     0.     0.    -0.8   -0.768 -0.736 -0.704 -0.672 -0.64  -0.608
   -0.576 -0.544 -0.512 -0.48  -0.448 -0.416 -0.384 -0.352 -0.32  -0.288
-  -0.256 -0.224 -0.192 -0.16  -0.128 -0.096 -0.064 -0.032  0.     0.   ]
+   0.    -0.224 -0.192 -0.16  -0.128 -0.096 -0.064 -0.032  0.     0.   ]
  [ 0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
    0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
    0.     0.     0.     0.     0.     0.     0.     0.     0.     0.   ]
@@ -26869,57 +26866,91 @@
       </c>
       <c r="C984" t="inlineStr">
         <is>
-          <t>[[0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8
-  0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8
-  0.8    0.8    0.8    0.8    0.7536 0.7059 0.6587 0.611  0.5383 0.3419]
- [0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8
-  0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8    0.8
-  0.8    0.8    0.8    0.7855 0.7453 0.7019 0.6571 0.6099 0.5246 0.331 ]
- [0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094
-  0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.3094
-  0.3094 0.3094 0.3094 0.3094 0.3094 0.3094 0.2801 0.2223 0.1635 0.1035]
- [1.152  1.1549 1.162  1.1673 1.1737 1.1797 1.1989 1.2105 1.2239 1.2277
-  1.2238 1.2183 1.2132 1.2126 1.2149 1.2212 1.2323 1.1573 1.0747 0.993
-  0.9128 0.8335 0.7545 0.6725 0.5489 0.4694 0.3894 0.3082 0.226  0.1426]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]
- [0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.
-  0.     0.     0.     0.     0.     0.     0.     0.     0.     0.    ]]</t>
+          <t>[[0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.8        0.8        0.8        0.8        0.8        0.8
+  0.8        0.8        0.8        0.8        0.8        0.8
+  0.8        0.8        0.8        0.8        0.8        0.8
+  0.8        0.8        1.78667617 0.8        0.8        0.8
+  0.7536     0.7059     0.6587     0.611      0.5383     0.3419    ]
+ [0.8        0.8        0.8        0.8        0.8        0.8
+  0.8        0.8        0.8        0.8        0.8        0.8
+  0.8        0.8        0.8        0.8        0.8        0.8
+  0.8        0.8        1.78667617 0.8        0.8        0.7855
+  0.7453     0.7019     0.6571     0.6099     0.5246     0.331     ]
+ [0.3094     0.3094     0.3094     0.3094     0.3094     0.3094
+  0.3094     0.3094     0.3094     0.3094     0.3094     0.3094
+  0.3094     0.3094     0.3094     0.3094     0.3094     0.3094
+  0.3094     0.3094     0.3094     0.3094     0.3094     0.3094
+  0.3094     0.3094     0.2801     0.2223     0.1635     0.1035    ]
+ [1.152      1.1549     1.162      1.1673     1.1737     1.1797
+  1.1989     1.2105     1.2239     1.2277     1.2238     1.2183
+  1.2132     1.2126     1.2149     1.2212     1.2323     1.1573
+  1.0747     0.993      0.9128     0.8335     0.7545     0.6725
+  0.5489     0.4694     0.3894     0.3082     0.226      0.1426    ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]
+ [0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.
+  0.         0.         0.         0.         0.         0.        ]]</t>
         </is>
       </c>
       <c r="D984" t="inlineStr">
@@ -26951,16 +26982,16 @@
   0.00435823 0.00435168 0.00430703 0.0042194  0.00408392 0.00389572
   0.00364992 0.00334165 0.00298133 0.00257936 0.00214615 0.00169212
   0.00122768 0.001      0.001      0.001      0.001      0.001     ]
- [0.         0.00935193 0.01778836 0.02520755 0.03160629 0.03726366
-  0.04197958 0.04437768 0.04562342 0.04536116 0.04363379 0.0413983
-  0.03865705 0.03598015 0.03345555 0.03130932 0.02938512 0.02757318
-  0.02588492 0.03255677 0.03944401 0.02690128 0.0201693  0.01698569
-  0.01515147 0.01327796 0.01137834 0.00952276 0.00768863 0.00587381]
- [0.         0.00935193 0.01778836 0.02520755 0.03160629 0.03726366
-  0.04197958 0.04437768 0.04562342 0.04536116 0.04363379 0.0413983
-  0.03865705 0.03598015 0.03345555 0.03130932 0.02938512 0.02757318
-  0.02588492 0.03255677 0.03944401 0.02690128 0.0201693  0.01698569
-  0.01515147 0.01327796 0.01137834 0.00952276 0.00768863 0.00587381]
+ [0.         0.00558896 0.01117792 0.01676688 0.02148023 0.02594341
+  0.03040659 0.03263711 0.0330815  0.03352589 0.03307007 0.03081386
+  0.02855764 0.02640753 0.0251063  0.02380507 0.02250383 0.04173291
+  0.06352828 0.08532365 0.08293418 0.0684523  0.05397041 0.04090187
+  0.02960001 0.01829814 0.00925718 0.00812939 0.0070016  0.00587381]
+ [0.         0.00558896 0.01117792 0.01676688 0.02148023 0.02594341
+  0.03040659 0.03263711 0.0330815  0.03352589 0.03307007 0.03081386
+  0.02855764 0.02640753 0.0251063  0.02380507 0.02250383 0.04173291
+  0.06352828 0.08532365 0.08293418 0.0684523  0.05397041 0.04090187
+  0.02960001 0.01829814 0.00925718 0.00812939 0.0070016  0.00587381]
  [0.         0.         0.00665003 0.00814812 0.00964621 0.0111443
   0.01260256 0.01398116 0.01524026 0.01634003 0.01724065 0.01790228
   0.01832761 0.01851932 0.01848012 0.01821267 0.01771968 0.01700382
@@ -30615,11 +30646,11 @@
       </c>
       <c r="C1121" t="inlineStr">
         <is>
-          <t>[30.55250184 41.30390771 17.82478227 20.22725151 18.52692143 15.8308358
- 12.60471261  9.47973865  7.66474322  7.49847232  7.42617445  7.3294747
-  7.21477513  7.01650366  6.5085588   5.8700593   5.19580738  4.65901969
-  4.20752566  3.89371307  3.48012488  2.62623433  1.54627847  0.26165696
- -1.01437504 -2.08257615 -2.93165156 -3.59063973 -4.15885855 -4.53873956]</t>
+          <t>[30.55250184 36.69846006 15.26518571 18.91550005 17.41608682 14.92252834
+ 11.89835971  8.97704532  7.26226157  7.13925881  7.11606159  7.03017509
+  6.93753459  6.76784661  6.30731421  5.70152717  5.05641301  4.91129006
+  4.80982845  4.6216554   3.11103487  3.05501567  1.7464672   0.22212994
+ -1.15747512 -2.16830425 -2.8850273  -3.56700082 -4.14860943 -4.53873956]</t>
         </is>
       </c>
       <c r="D1121" t="inlineStr">
@@ -30641,11 +30672,11 @@
       </c>
       <c r="C1122" t="inlineStr">
         <is>
-          <t>[-0.01845476 -0.00733979  0.06819624  0.25712788  0.22310211  0.20692138
-  0.16789737  0.15446169  0.13287621  0.13463984  0.13356057  0.13235376
-  0.13183974  0.12574355  0.11690578  0.12425034  0.10213034  0.08391371
-  0.06953864  0.05433115  0.04244348  0.03407349  0.0227879   0.01244195
-  0.00253607 -0.00232586 -0.00399133 -0.00474265 -0.00549329 -0.00438864]</t>
+          <t>[-0.01845476 -0.00697339  0.07519249  0.24991401  0.23426654  0.224675
+  0.18459129  0.16922242  0.1467512   0.14795533  0.14600109  0.14566084
+  0.14537323  0.1388842   0.12773965  0.13271474  0.10886083  0.07677676
+  0.05917328  0.04768934  0.04415977  0.03105245  0.02095396  0.01211049
+  0.00299264 -0.001901   -0.00434842 -0.00496418 -0.00556609 -0.00438864]</t>
         </is>
       </c>
       <c r="D1122" t="inlineStr">
@@ -30667,14 +30698,14 @@
       </c>
       <c r="C1123" t="inlineStr">
         <is>
-          <t>[-1.51443081e-04  7.54229806e-03  1.31130791e-01 -7.85327739e-02
- -1.68343522e-01 -2.05309735e-01 -2.32287048e-01 -2.39050849e-01
- -2.25568666e-01 -1.97636698e-01 -1.59812958e-01 -1.16874741e-01
- -7.53652034e-02 -3.24988514e-02 -1.47823054e-02 -2.54389952e-02
- -2.78639609e-02 -4.94578347e-02 -7.01544972e-02 -1.27067496e-01
- -1.54295903e-01 -1.23068644e-01 -1.02784000e-01 -9.08770860e-02
- -8.11966635e-02 -6.49073066e-02 -4.44173814e-02 -2.19597681e-02
-  2.34201733e-03 -4.90668081e-03]</t>
+          <t>[-1.51443081e-04  7.74535239e-03  1.41680751e-01 -1.41612232e-02
+ -8.59566773e-02 -1.14280370e-01 -1.43754396e-01 -1.51285592e-01
+ -1.30631265e-01 -1.05727903e-01 -7.38631711e-02 -2.33272632e-02
+  2.10932273e-02  6.69190694e-02  7.35288972e-02  5.13454139e-02
+  4.10837269e-02 -1.30456446e-01 -1.99077154e-01 -2.18111871e-01
+ -2.24269319e-01 -1.79993816e-01 -1.54753717e-01 -1.28379373e-01
+ -1.02179294e-01 -7.24445229e-02 -4.08038541e-02 -2.06546970e-02
+  2.42189735e-03 -4.90668081e-03]</t>
         </is>
       </c>
       <c r="D1123" t="inlineStr">
@@ -30696,11 +30727,11 @@
       </c>
       <c r="C1124" t="inlineStr">
         <is>
-          <t>[-0.01845476 -0.00733979  0.06819624  0.25932467  0.22476277  0.20804296
-  0.16861921  0.15488324  0.13315446  0.13487208  0.13378102  0.13259336
-  0.13210383  0.12606015  0.11720789  0.12450563  0.10234137  0.08407291
-  0.06965502  0.0543803   0.04246263  0.03409312  0.02279981  0.01245021
-  0.0025311  -0.00233665 -0.0040035  -0.00475358 -0.00550193 -0.00438864]</t>
+          <t>[-0.01845476 -0.00697339  0.07519249  0.25219252  0.23637508  0.22629482
+  0.18570619  0.16993621  0.14727672  0.14840858  0.14642044  0.14611619
+  0.14585997  0.13942699  0.12822431  0.13310843  0.1091776   0.07685403
+  0.05919438  0.04769557  0.04416599  0.03105453  0.02095463  0.0121134
+  0.00299139 -0.00190723 -0.00436543 -0.00497812 -0.00557585 -0.00438864]</t>
         </is>
       </c>
       <c r="D1124" t="inlineStr">
@@ -30722,14 +30753,14 @@
       </c>
       <c r="C1125" t="inlineStr">
         <is>
-          <t>[-1.51443081e-04  7.54229806e-03  1.31130791e-01 -8.23678559e-02
- -1.69648819e-01 -2.04450970e-01 -2.30293827e-01 -2.36363931e-01
- -2.22680537e-01 -1.94835046e-01 -1.56987444e-01 -1.13981398e-01
- -7.24034122e-02 -2.94741903e-02 -1.18925800e-02 -2.29284025e-02
- -2.56570437e-02 -4.76686046e-02 -6.87448902e-02 -1.26409282e-01
- -1.53987276e-01 -1.22637677e-01 -1.02298022e-01 -9.04383892e-02
- -8.08481380e-02 -6.46264459e-02 -4.41773625e-02 -2.17299362e-02
-  2.63826913e-03 -4.90668081e-03]</t>
+          <t>[-1.51443081e-04  7.74535239e-03  1.41680751e-01 -1.71223092e-02
+ -8.58972547e-02 -1.11722277e-01 -1.40020788e-01 -1.46824988e-01
+ -1.25828972e-01 -1.01136505e-01 -6.93985753e-02 -1.86556579e-02
+  2.58782229e-02  7.17944583e-02  7.79936780e-02  5.51498207e-02
+  4.43826350e-02 -1.29592344e-01 -1.98833066e-01 -2.18033198e-01
+ -2.24262035e-01 -1.79927875e-01 -1.54672573e-01 -1.28278696e-01
+ -1.02055921e-01 -7.22665685e-02 -4.04921464e-02 -2.03824800e-02
+  2.74424190e-03 -4.90668081e-03]</t>
         </is>
       </c>
       <c r="D1125" t="inlineStr">
@@ -30751,11 +30782,11 @@
       </c>
       <c r="C1126" t="inlineStr">
         <is>
-          <t>[-0.01845476 -0.00653056  0.07414013  0.20130523  0.21864156  0.23436199
-  0.20975806  0.2029116   0.18141722  0.1866877   0.18737798  0.18588317
-  0.184074    0.17474578  0.16085623  0.16094001  0.13331236  0.11065152
-  0.09249141  0.07358288  0.05683131  0.04514656  0.02953848  0.01391401
-  0.00084789 -0.0058164  -0.00812157 -0.00840506 -0.00779905 -0.00495543]</t>
+          <t>[-0.01845476 -0.00647057  0.07534207  0.19921233  0.22061135  0.23903092
+  0.21549421  0.20920732  0.18825304  0.19387517  0.19433411  0.19323046
+  0.19132842  0.18165282  0.16659574  0.16561317  0.13721866  0.10451017
+  0.08031274  0.06221768  0.04960938  0.03882605  0.02563021  0.01315321
+  0.00163607 -0.00505464 -0.00869267 -0.00880755 -0.00794877 -0.00495543]</t>
         </is>
       </c>
       <c r="D1126" t="inlineStr">
@@ -30777,14 +30808,14 @@
       </c>
       <c r="C1127" t="inlineStr">
         <is>
-          <t>[-1.51443081e-04  7.99373925e-03  1.03730779e-01  6.17817870e-02
-  3.66735994e-02  5.10234862e-02  6.85062478e-02  9.12377587e-02
-  1.28342111e-01  1.72515495e-01  2.14622532e-01  2.60669467e-01
-  2.97602699e-01  3.50759695e-01  3.57938136e-01  3.24373791e-01
-  3.10737003e-01  2.71705404e-01  2.29971978e-01  1.45438962e-01
-  7.12757043e-02  8.05690487e-02  7.11587256e-02  5.03697926e-02
-  2.56565880e-02  1.10142018e-02  4.97484153e-03  2.17347676e-03
-  2.87615706e-03 -1.78285697e-02]</t>
+          <t>[-1.51443081e-04  8.02619173e-03  1.05157861e-01  7.47900834e-02
+  5.71610565e-02  7.90128839e-02  1.02333682e-01  1.30864778e-01
+  1.76515558e-01  2.22868883e-01  2.62879202e-01  3.12433672e-01
+  3.49380906e-01  4.03831941e-01  4.05590278e-01  3.67769190e-01
+  3.51892945e-01  1.99965839e-01  7.43503116e-02 -1.35119996e-02
+ -1.25996433e-01 -3.66204122e-02 -3.27931731e-02 -2.60369201e-02
+ -1.91940081e-02 -4.55658742e-03  1.14868317e-02  4.75023297e-03
+  2.94908977e-03 -1.78285697e-02]</t>
         </is>
       </c>
       <c r="D1127" t="inlineStr">
@@ -30806,14 +30837,14 @@
       </c>
       <c r="C1128" t="inlineStr">
         <is>
-          <t>[5.52430606e+03 4.48222661e+03 3.19468179e+03 1.91487439e+03
- 9.80172588e+02 5.53052094e+02 3.73302116e+02 2.55960885e+02
- 1.87922949e+02 1.51957481e+02 1.29018850e+02 1.10789199e+02
- 9.66208998e+01 8.09090162e+01 6.65132716e+01 5.21294466e+01
- 4.02335088e+01 3.05939003e+01 2.27942359e+01 1.93435005e+01
- 1.60357437e+01 9.21906467e+00 5.40259973e+00 3.19423167e+00
- 1.78878384e+00 9.39311808e-01 4.54947025e-01 1.88207955e-01
- 5.99763926e-02 1.08172781e-02]</t>
+          <t>[5.52430606e+03 4.47931264e+03 3.16451942e+03 1.88359435e+03
+ 9.48759953e+02 5.23771869e+02 3.46920920e+02 2.33364235e+02
+ 1.67521595e+02 1.34868534e+02 1.15040897e+02 9.79169563e+01
+ 8.52460454e+01 7.12259956e+01 5.90834211e+01 4.64791882e+01
+ 3.58892943e+01 3.76903432e+01 3.73342395e+01 3.41805564e+01
+ 3.75684339e+01 1.64054091e+01 9.99506183e+00 5.58376871e+00
+ 2.74973254e+00 1.14985508e+00 4.02995839e-01 1.71912450e-01
+ 5.71008934e-02 1.08172781e-02]</t>
         </is>
       </c>
       <c r="D1128" t="inlineStr">
@@ -30835,14 +30866,14 @@
       </c>
       <c r="C1129" t="inlineStr">
         <is>
-          <t>[5.52456218e+03 4.62964598e+03 3.98800225e+03 3.09061722e+03
- 2.31686779e+03 1.82424885e+03 1.50765641e+03 1.28581667e+03
- 1.13753810e+03 1.04417985e+03 9.85475142e+02 9.28456110e+02
- 8.76266915e+02 7.86931312e+02 6.84145857e+02 5.43109355e+02
- 4.32626440e+02 3.30560153e+02 2.45613928e+02 1.83637843e+02
- 1.33647899e+02 8.84630009e+01 5.75294280e+01 3.64459895e+01
- 2.14663981e+01 1.21743048e+01 6.43626455e+00 2.95167384e+00
- 1.12939494e+00 1.97141925e-01]</t>
+          <t>[5.52456218e+03 4.58723091e+03 3.94509594e+03 3.04062131e+03
+ 2.27113809e+03 1.78729050e+03 1.47848222e+03 1.26114466e+03
+ 1.11270067e+03 1.02035161e+03 9.63942461e+02 9.06353944e+02
+ 8.55122237e+02 7.66253070e+02 6.67389842e+02 5.30400541e+02
+ 4.22378853e+02 3.45313409e+02 2.72048470e+02 2.06928363e+02
+ 2.52926413e+02 9.99354359e+01 6.55289199e+01 4.11721245e+01
+ 2.35957934e+01 1.27347767e+01 6.25687823e+00 2.86622178e+00
+ 1.10255118e+00 1.97141925e-01]</t>
         </is>
       </c>
       <c r="D1129" t="inlineStr">
@@ -30864,7 +30895,7 @@
       </c>
       <c r="C1130" t="inlineStr">
         <is>
-          <t>[50995.25314794]</t>
+          <t>[52661.47228171]</t>
         </is>
       </c>
       <c r="D1130" t="inlineStr">
@@ -30886,7 +30917,7 @@
       </c>
       <c r="C1131" t="inlineStr">
         <is>
-          <t>[68525219.17722951]</t>
+          <t>[82653960.74229212]</t>
         </is>
       </c>
       <c r="D1131" t="inlineStr">
@@ -30908,7 +30939,7 @@
       </c>
       <c r="C1132" t="inlineStr">
         <is>
-          <t>[152985.75944382]</t>
+          <t>[157984.41684513]</t>
         </is>
       </c>
       <c r="D1132" t="inlineStr">
@@ -30930,7 +30961,7 @@
       </c>
       <c r="C1133" t="inlineStr">
         <is>
-          <t>[2.05575658e+08 1.02787829e+08 1.02787829e+08 0.00000000e+00
+          <t>[2.47961882e+08 1.23980941e+08 1.23980941e+08 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -32157,14 +32188,14 @@
       </c>
       <c r="C1176" t="inlineStr">
         <is>
-          <t>[ 1277.32213347  1333.66454013  1575.72233364  1923.62455217
-  2398.44802251  2986.95809745  3532.40487805  4369.70111609
-  5399.44395166  6572.67691964  7784.63220523  9157.13455125
- 10676.99699663 11864.12085972 12896.53014651 13502.5292014
- 13910.69990874 14175.98068984 14331.25045083 14313.90156797
- 15620.65379692 13759.44219581 13115.64858014 12086.88521829
- 10337.88408717  8762.20030543  7572.93982553  6265.8578703
-  4804.97872049  3092.77926624]</t>
+          <t>[ 1277.32213347  1328.77489494  1565.94929473  1909.79248554
+  2380.88285742  2966.13453618  3508.94501981  4342.62437696
+  5365.60602419  6535.37897945  7746.55618808  9114.41981769
+ 10631.49423935 11814.18342107 12845.40800214 13450.2376201
+ 13857.31815444 14300.58689052 14711.12534088 14909.29558868
+ 17112.49739161 14320.11801464 13619.76169977 12472.78523353
+ 10576.08252165  8846.04701738  7537.14605807  6242.25387193
+  4794.09314384  3092.77926624]</t>
         </is>
       </c>
       <c r="D1176" t="inlineStr">
@@ -32186,14 +32217,14 @@
       </c>
       <c r="C1177" t="inlineStr">
         <is>
-          <t>[  536.83457993   575.11022232   493.61045586   224.13252526
-  -231.14772655  -674.24543528 -1014.68076261 -1480.84749507
- -1945.99250883 -2330.5195834  -2569.72728371 -2819.25349697
- -3082.56835541 -3196.57228357 -3304.66354281 -3366.2182337
- -3402.8352313  -3405.99985864 -3366.42386412 -3275.92081957
- -3172.43358994 -3144.95672731 -3079.48757462 -2910.31855232
- -2508.9805439  -2110.64524653 -1839.22259848 -1536.19596679
- -1186.61896131  -774.11428704]</t>
+          <t>[  536.83457993   573.45585212   490.57813707   220.25675853
+  -235.51243783  -678.59194534 -1018.40930317 -1483.93941871
+ -1949.00815806 -2333.78783452 -2573.06632682 -2823.00286203
+ -3086.56505294 -3200.90254452 -3308.77570824 -3369.93230952
+ -3406.10212828 -3399.34682102 -3348.6176041  -3251.86861264
+ -3123.20640151 -3131.74338824 -3074.61632835 -2913.0762323
+ -2514.71367588 -2113.86135153 -1837.41124596 -1534.73202762
+ -1185.83001417  -774.11428704]</t>
         </is>
       </c>
       <c r="D1177" t="inlineStr">
@@ -32215,14 +32246,14 @@
       </c>
       <c r="C1178" t="inlineStr">
         <is>
-          <t>[-17562.08341165 -10000.49062362  -4745.4425266    -895.6100005
-   1676.0611966    3303.05818753   4475.94371695   5349.9064811
-   6080.04379118   6769.82016172   7474.04945227   8174.39975929
-   8846.80778492   9327.74156639   9638.75253475   9540.5497714
-   9389.23351102   8962.48224161   8408.3351963    8563.01458068
-  19865.81148052   7037.79167909   5797.31860013   4900.47641079
-   4060.62106428   3346.82446095   2708.61270602   2074.21785592
-   1472.01185096    726.28962308]</t>
+          <t>[-17562.08341165  -9948.59542513  -4695.18520582   -880.92210544
+   1633.60977518   3189.27748285   4289.84831356   5089.81448677
+   5726.58971967   6365.55365515   7050.16435159   7686.42958705
+   8320.83471416   8771.90877415   9104.02373771   9014.82709332
+   8865.77811597  10124.24022284  11720.40126277  13519.03803007
+  31962.772912    11434.05955726   9573.02073068   7687.52675499
+   5732.68663783   3918.64847928   2472.49851734   1924.02858691
+   1404.80538289    726.28962308]</t>
         </is>
       </c>
       <c r="D1178" t="inlineStr">
@@ -32244,7 +32275,7 @@
       </c>
       <c r="C1179" t="inlineStr">
         <is>
-          <t>[-839460.41554989 -247801.23446215  492881.12033966]</t>
+          <t>[-852205.24634777 -248131.30675559  594274.70550392]</t>
         </is>
       </c>
       <c r="D1179" t="inlineStr">
@@ -32266,7 +32297,7 @@
       </c>
       <c r="C1180" t="inlineStr">
         <is>
-          <t>[ 12822625.22254687 -47407884.75872526        -0.        ]</t>
+          <t>[ 12551595.06251095 -47360632.37422645        -0.        ]</t>
         </is>
       </c>
       <c r="D1180" t="inlineStr">
@@ -32284,16 +32315,16 @@
       <c r="B1181" t="inlineStr"/>
       <c r="C1181" t="inlineStr">
         <is>
-          <t>[[ 6.01600319e-02  1.26897403e+00  5.87048535e-01 -1.81999881e+00
-   9.03816210e-01]
- [-1.77490059e-01 -1.39939200e+00  1.91094782e+00 -1.01075274e+00
-   1.67668698e+00]
- [ 9.86399557e-03  4.49411734e+00 -2.76161108e+00 -1.78474839e+01
-   1.71051136e+01]
- [ 3.05242304e+01 -2.24696073e+02  5.78822777e+02 -6.27085583e+02
-   2.43434648e+02]
- [ 1.42425102e+01 -1.22210301e+02  3.49577875e+02 -4.08051581e+02
-   1.67441496e+02]]</t>
+          <t>[[ 2.41256658e-01 -5.82920418e-01  7.82540462e+00 -1.10876449e+01
+   4.60390403e+00]
+ [ 1.78903381e+00 -1.93138559e+01  5.15068093e+01 -5.50676657e+01
+   2.20856785e+01]
+ [ 1.82854282e+00 -1.05256997e+01  3.56654954e+01 -5.65667799e+01
+   3.05984413e+01]
+ [ 7.19332077e+00 -7.91478759e+01  2.55717369e+02 -3.21517208e+02
+   1.38754394e+02]
+ [-1.81642908e+05  1.35233945e+06 -3.51465931e+06  3.83557261e+06
+  -1.49765631e+06]]</t>
         </is>
       </c>
       <c r="D1181" t="inlineStr">
@@ -32311,11 +32342,16 @@
       <c r="B1182" t="inlineStr"/>
       <c r="C1182" t="inlineStr">
         <is>
-          <t>[[  0.34039225   4.13559702  -8.76218758   7.6708747   -2.3846764 ]
- [ -0.82735907  -1.06101504   4.96746827  -4.06930511   1.99021095]
- [  1.52550478   2.86146965 -19.27812409  17.60751159  -1.71636192]
- [ -1.93579959  29.95391186 -90.69274819  94.91284481 -31.23820889]
- [ -4.84281195  11.3263772   26.25462077 -81.3197582   49.58157218]]</t>
+          <t>[[ 4.73294566e-01  3.20058457e+00 -5.69742020e+00  4.04448466e+00
+  -1.02094360e+00]
+ [-6.35702626e+02  4.26266002e+04 -1.33941819e+05  1.49065458e+05
+  -6.08665379e+04]
+ [ 1.99837428e+00 -3.35789829e+00 -6.15220680e-01 -2.40077603e+00
+   5.37552072e+00]
+ [-4.28381404e+00  7.22150393e+00  3.54066144e+01 -8.90402367e+01
+   5.16959323e+01]
+ [ 2.49697030e+01 -1.88394907e+02  4.93617970e+02 -5.42290339e+02
+   2.13097573e+02]]</t>
         </is>
       </c>
       <c r="D1182" t="inlineStr">
@@ -32333,26 +32369,26 @@
       <c r="B1183" t="inlineStr"/>
       <c r="C1183" t="inlineStr">
         <is>
-          <t>[[ 6.01600319e-02  1.26897403e+00  5.87048535e-01 -1.81999881e+00
-   9.03816210e-01]
- [ 3.40392255e-01  4.13559702e+00 -8.76218758e+00  7.67087470e+00
-  -2.38467640e+00]
- [-1.77490059e-01 -1.39939200e+00  1.91094782e+00 -1.01075274e+00
-   1.67668698e+00]
- [-8.27359068e-01 -1.06101504e+00  4.96746827e+00 -4.06930511e+00
-   1.99021095e+00]
- [ 9.86399557e-03  4.49411734e+00 -2.76161108e+00 -1.78474839e+01
-   1.71051136e+01]
- [ 1.52550478e+00  2.86146965e+00 -1.92781241e+01  1.76075116e+01
-  -1.71636192e+00]
- [ 3.05242304e+01 -2.24696073e+02  5.78822777e+02 -6.27085583e+02
-   2.43434648e+02]
- [-1.93579959e+00  2.99539119e+01 -9.06927482e+01  9.49128448e+01
-  -3.12382089e+01]
- [ 1.42425102e+01 -1.22210301e+02  3.49577875e+02 -4.08051581e+02
-   1.67441496e+02]
- [-4.84281195e+00  1.13263772e+01  2.62546208e+01 -8.13197582e+01
-   4.95815722e+01]]</t>
+          <t>[[ 2.41256658e-01 -5.82920418e-01  7.82540462e+00 -1.10876449e+01
+   4.60390403e+00]
+ [ 4.73294566e-01  3.20058457e+00 -5.69742020e+00  4.04448466e+00
+  -1.02094360e+00]
+ [ 1.78903381e+00 -1.93138559e+01  5.15068093e+01 -5.50676657e+01
+   2.20856785e+01]
+ [-6.35702626e+02  4.26266002e+04 -1.33941819e+05  1.49065458e+05
+  -6.08665379e+04]
+ [ 1.82854282e+00 -1.05256997e+01  3.56654954e+01 -5.65667799e+01
+   3.05984413e+01]
+ [ 1.99837428e+00 -3.35789829e+00 -6.15220680e-01 -2.40077603e+00
+   5.37552072e+00]
+ [ 7.19332077e+00 -7.91478759e+01  2.55717369e+02 -3.21517208e+02
+   1.38754394e+02]
+ [-4.28381404e+00  7.22150393e+00  3.54066144e+01 -8.90402367e+01
+   5.16959323e+01]
+ [-1.81642908e+05  1.35233945e+06 -3.51465931e+06  3.83557261e+06
+  -1.49765631e+06]
+ [ 2.49697030e+01 -1.88394907e+02  4.93617970e+02 -5.42290339e+02
+   2.13097573e+02]]</t>
         </is>
       </c>
       <c r="D1183" t="inlineStr">
@@ -32374,7 +32410,7 @@
       </c>
       <c r="C1184" t="inlineStr">
         <is>
-          <t>[ 0.58971311  1.69176047  3.29988048  7.61942099 10.93851804]</t>
+          <t>[0.48376794 1.91393545 3.38508001 5.95236759 7.78548957]</t>
         </is>
       </c>
       <c r="D1184" t="inlineStr">
@@ -32396,7 +32432,7 @@
       </c>
       <c r="C1185" t="inlineStr">
         <is>
-          <t>[0.89366771 2.66278862 4.88079197 5.8239762  9.72007212]</t>
+          <t>[ 0.77555807  2.85313168  5.04057647  9.74351024 14.4304181 ]</t>
         </is>
       </c>
       <c r="D1185" t="inlineStr">
@@ -32418,8 +32454,8 @@
       </c>
       <c r="C1186" t="inlineStr">
         <is>
-          <t>[ 0.58971311  0.89366771  1.69176047  2.66278862  3.29988048  4.88079197
-  5.8239762   7.61942099  9.72007212 10.93851804]</t>
+          <t>[ 0.48376794  0.77555807  1.91393545  2.85313168  3.38508001  5.04057647
+  5.95236759  7.78548957  9.74351024 11.30834587]</t>
         </is>
       </c>
       <c r="D1186" t="inlineStr">
@@ -32437,7 +32473,7 @@
       <c r="B1187" t="inlineStr"/>
       <c r="C1187" t="inlineStr">
         <is>
-          <t>[1.51542793]</t>
+          <t>[1.60316137]</t>
         </is>
       </c>
       <c r="D1187" t="inlineStr">
@@ -32459,14 +32495,14 @@
       </c>
       <c r="C1188" t="inlineStr">
         <is>
-          <t>[-0.00000000e+00  3.62257302e-03  1.46067558e-02  3.40081513e-02
-  6.47822091e-02  1.11807196e-01  1.80358160e-01  2.74871366e-01
-  3.99208476e-01  5.56530990e-01  7.48709828e-01  9.76759059e-01
-  1.24138144e+00  1.54330722e+00  1.88372388e+00  2.26447964e+00
-  2.68800876e+00  3.15694247e+00  3.67375910e+00  4.23754569e+00
-  4.84222409e+00  5.48511184e+00  6.17336881e+00  6.91721439e+00
-  7.72424190e+00  8.60061714e+00  9.55168191e+00  1.05795522e+01
-  1.16777518e+01  1.28191983e+01]</t>
+          <t>[-0.00000000e+00  3.68652757e-03  1.50458215e-02  3.55678467e-02
+  6.89667358e-02  1.21513091e-01  2.00196839e-01  3.10870179e-01
+  4.58759620e-01  6.48269046e-01  8.81564546e-01  1.15953368e+00
+  1.48321251e+00  1.85382864e+00  2.27278150e+00  2.74180402e+00
+  3.26330878e+00  3.83243816e+00  4.43573364e+00  5.06257771e+00
+  5.70593618e+00  6.36315546e+00  7.03947970e+00  7.74127786e+00
+  8.47435389e+00  9.24890376e+00  1.00845766e+01  1.10035073e+01
+  1.20042177e+01  1.30530476e+01]</t>
         </is>
       </c>
       <c r="D1188" t="inlineStr">
@@ -32488,14 +32524,14 @@
       </c>
       <c r="C1189" t="inlineStr">
         <is>
-          <t>[ 0.00000000e+00 -1.14049591e-03 -4.98778076e-03 -1.28618214e-02
- -2.71745532e-02 -5.13435812e-02 -8.79775034e-02 -1.37462783e-01
- -1.98918678e-01 -2.71570997e-01 -3.55180606e-01 -4.49686385e-01
- -5.54929653e-01 -6.70720126e-01 -7.96840552e-01 -9.32978402e-01
- -1.07872365e+00 -1.23362827e+00 -1.39730365e+00 -1.56905449e+00
- -1.74764532e+00 -1.93218372e+00 -2.12228781e+00 -2.31692914e+00
- -2.51406660e+00 -2.71120529e+00 -2.90579373e+00 -3.09552897e+00
- -3.27892727e+00 -3.45731950e+00]</t>
+          <t>[ 0.00000000e+00 -1.07918079e-03 -4.72984982e-03 -1.22918960e-02
+ -2.64009557e-02 -5.10151963e-02 -8.93564771e-02 -1.42106838e-01
+ -2.08436057e-01 -2.87599149e-01 -3.79340558e-01 -4.83585193e-01
+ -6.00246479e-01 -7.29223214e-01 -8.70288562e-01 -1.02298540e+00
+ -1.18672029e+00 -1.35985870e+00 -1.53989111e+00 -1.72503770e+00
+ -1.91361168e+00 -2.10441396e+00 -2.29796510e+00 -2.49444423e+00
+ -2.69285534e+00 -2.89175054e+00 -3.08866729e+00 -3.28008991e+00
+ -3.46399705e+00 -3.64229652e+00]</t>
         </is>
       </c>
       <c r="D1189" t="inlineStr">
@@ -32517,14 +32553,14 @@
       </c>
       <c r="C1190" t="inlineStr">
         <is>
-          <t>[-0.00000000e+00 -5.80751903e-05 -1.27153576e-04 -2.02543284e-04
- -2.93472040e-04 -3.93040394e-04 -4.95677262e-04 -5.98762054e-04
- -7.01748823e-04 -8.04206011e-04 -9.06229563e-04 -1.00760907e-03
- -1.10790865e-03 -1.20681289e-03 -1.30385197e-03 -1.39875651e-03
- -1.49109875e-03 -1.58059883e-03 -1.66732872e-03 -1.74129156e-03
- -1.79496641e-03 -1.83588103e-03 -1.87733642e-03 -1.91752857e-03
- -1.95364174e-03 -1.98494890e-03 -2.01087837e-03 -2.03069001e-03
- -2.04368758e-03 -2.04917353e-03]</t>
+          <t>[-0.00000000e+00 -7.05080503e-05 -1.56202740e-04 -2.51835955e-04
+ -3.71502995e-04 -5.07045990e-04 -6.49960273e-04 -7.95806993e-04
+ -9.44860836e-04 -1.09572271e-03 -1.24619266e-03 -1.39736657e-03
+ -1.55025808e-03 -1.70423120e-03 -1.85785541e-03 -2.01070794e-03
+ -2.16369703e-03 -2.28082152e-03 -2.35577524e-03 -2.40606437e-03
+ -2.42984048e-03 -2.44714857e-03 -2.47097972e-03 -2.49298948e-03
+ -2.51360874e-03 -2.53411418e-03 -2.55686360e-03 -2.57870723e-03
+ -2.59261326e-03 -2.59821336e-03]</t>
         </is>
       </c>
       <c r="D1190" t="inlineStr">
@@ -32546,14 +32582,14 @@
       </c>
       <c r="C1191" t="inlineStr">
         <is>
-          <t>[7.98151328e+10 6.48327786e+10 4.94870403e+10 3.20696826e+10
- 1.96317514e+10 1.42042769e+10 1.22158885e+10 1.03262351e+10
- 8.71029175e+09 7.52241410e+09 6.57289377e+09 5.71270912e+09
- 4.95546712e+09 4.15944350e+09 3.42728594e+09 2.72656780e+09
- 2.14973242e+09 1.67609121e+09 1.28750310e+09 1.24488262e+09
- 1.14251653e+09 6.30203214e+08 3.63366228e+08 2.18784126e+08
- 1.25969222e+08 6.68792057e+07 3.21470736e+07 1.31539898e+07
- 4.00574656e+06 6.63549801e+05]</t>
+          <t>[7.98151328e+10 6.47758219e+10 4.83872302e+10 3.00887306e+10
+ 1.76083779e+10 1.21366076e+10 1.01654099e+10 8.36035901e+09
+ 6.82960402e+09 5.93489499e+09 5.26650075e+09 4.49956942e+09
+ 3.87571871e+09 3.23194176e+09 2.70924934e+09 2.17597268e+09
+ 1.72329164e+09 2.37126535e+09 2.70655281e+09 2.68639124e+09
+ 3.34783563e+09 1.34451786e+09 8.23136227e+08 4.58362950e+08
+ 2.22255852e+08 8.79867697e+07 2.69280138e+07 1.15103452e+07
+ 3.71248087e+06 6.63549801e+05]</t>
         </is>
       </c>
       <c r="D1191" t="inlineStr">
@@ -32575,14 +32611,14 @@
       </c>
       <c r="C1192" t="inlineStr">
         <is>
-          <t>[7.98188341e+10 7.64659055e+10 7.25670659e+10 6.04406830e+10
- 4.85081958e+10 3.87034794e+10 3.18332565e+10 2.66917303e+10
- 2.37498192e+10 2.22579837e+10 2.12101646e+10 2.01398001e+10
- 1.89930228e+10 1.72865436e+10 1.49860851e+10 1.19523989e+10
- 9.55490336e+09 7.22140055e+09 5.31049305e+09 4.01485570e+09
- 3.00302662e+09 1.97316894e+09 1.29451027e+09 8.49407922e+08
- 5.18654908e+08 3.11502258e+08 1.78519654e+08 9.46513925e+07
- 4.24686035e+07 7.80100709e+06]</t>
+          <t>[7.98188341e+10 7.19162200e+10 6.62704498e+10 5.46276126e+10
+ 4.34274774e+10 3.50330604e+10 2.94151672e+10 2.51463158e+10
+ 2.25058229e+10 2.11622396e+10 2.02581063e+10 1.91829375e+10
+ 1.80786201e+10 1.64234741e+10 1.43057988e+10 1.14523265e+10
+ 9.17003948e+09 7.68912295e+09 6.16488105e+09 4.91376748e+09
+ 1.37520882e+10 2.55650008e+09 1.75369937e+09 1.15972010e+09
+ 6.75868108e+08 3.56793812e+08 1.62880330e+08 8.65149705e+07
+ 3.98197715e+07 7.80100709e+06]</t>
         </is>
       </c>
       <c r="D1192" t="inlineStr">
@@ -32604,11 +32640,11 @@
       </c>
       <c r="C1193" t="inlineStr">
         <is>
-          <t>[30.55251326 50.72304745 37.73448418 33.396764   32.52131522 29.69836566
- 25.89232328 19.85013459 15.39255336 14.31705478 13.44238579 12.5747098
- 11.81181196 10.94780474  9.85917236  8.77100584  7.63139564  6.85847097
-  6.23765047  6.43557556  6.36878563  4.08533143  1.99325604 -0.09540907
- -1.93580583 -3.16122874 -3.82525706 -4.09053094 -4.52338717 -5.37331236]</t>
+          <t>[30.55251326 49.43486844 30.64944808 28.35224956 27.60702659 24.90731949
+ 21.43894558 16.30997632 12.62418539 12.03105717 11.59505421 10.89656444
+ 10.3218013   9.65342811  8.82213662  7.89686379  6.91112837  8.37367625
+ 10.55739414 12.69020784  3.36010519  6.99239523  2.96477795 -0.33022947
+ -2.47344663 -3.40911355 -3.72244464 -4.06744114 -4.51670881 -5.37331236]</t>
         </is>
       </c>
       <c r="D1193" t="inlineStr">
@@ -32630,14 +32666,14 @@
       </c>
       <c r="C1194" t="inlineStr">
         <is>
-          <t>[-3.48176418e+07 -3.26389882e+07 -2.92716934e+07 -3.19960854e+07
- -3.11989678e+07 -2.99064659e+07 -2.88189400e+07 -2.75536837e+07
- -2.56726448e+07 -2.32654324e+07 -2.07774528e+07 -1.83832677e+07
- -1.61037967e+07 -1.39572094e+07 -1.19590939e+07 -1.01150856e+07
- -8.42836025e+06 -6.90453071e+06 -5.54903682e+06 -4.36358600e+06
- -3.34616543e+06 -2.48286920e+06 -1.75960673e+06 -1.18496156e+06
- -7.48517220e+05 -4.32339997e+05 -2.16572064e+05 -8.36799124e+04
- -1.71054148e+04  2.83850017e+00]</t>
+          <t>[-3.49475571e+07 -3.27227091e+07 -3.12035510e+07 -3.40649595e+07
+ -3.25038652e+07 -3.08643310e+07 -2.93712780e+07 -2.76651160e+07
+ -2.54786421e+07 -2.29635206e+07 -2.04477650e+07 -1.80461145e+07
+ -1.57738394e+07 -1.36445712e+07 -1.16723102e+07 -9.86345069e+06
+ -8.22088493e+06 -6.74834090e+06 -5.44164119e+06 -4.29289835e+06
+ -3.31671456e+06 -2.47551879e+06 -1.76914295e+06 -1.19522074e+06
+ -7.57111476e+05 -4.39065623e+05 -2.20785699e+05 -8.54283199e+04
+ -1.75485171e+04  3.01134316e+00]</t>
         </is>
       </c>
       <c r="D1194" t="inlineStr">
@@ -32659,14 +32695,14 @@
       </c>
       <c r="C1195" t="inlineStr">
         <is>
-          <t>[ 3.46361181e+07  3.25690789e+07  3.16723777e+07  2.42880821e+07
-  2.03409180e+07  1.69123952e+07  1.27651238e+07  8.17190417e+06
-  4.29760102e+06  2.52610201e+06  1.96553843e+06  1.53341102e+06
-  1.18081099e+06  8.75478933e+05  5.51845758e+05  2.37571304e+05
- -1.16923027e+04 -1.57155828e+05 -2.11192828e+05 -1.93997314e+05
- -1.56239687e+05 -1.77002675e+05 -2.05047295e+05 -1.94972087e+05
- -1.59687243e+05 -1.10136881e+05 -6.15145142e+04 -2.54398971e+04
- -5.54443133e+03  9.37112041e-02]</t>
+          <t>[ 3.43400918e+07  3.22608410e+07  2.94824675e+07  2.08362140e+07
+  1.76112084e+07  1.43746365e+07  1.04687516e+07  6.32816123e+06
+  3.00404280e+06  1.63019453e+06  1.33881701e+06  1.08276032e+06
+  8.42829073e+05  6.35584012e+05  4.00694135e+05  1.54319027e+05
+ -5.16331437e+04 -4.66363925e+04  1.15751955e+05  2.37519564e+05
+ -3.81283481e+04 -1.65991616e+05 -1.38048934e+05 -1.84504514e+05
+ -1.64668214e+05 -1.14022991e+05 -6.25543725e+04 -2.56714985e+04
+ -5.62488618e+03  9.62241177e-02]</t>
         </is>
       </c>
       <c r="D1195" t="inlineStr">
@@ -32688,14 +32724,14 @@
       </c>
       <c r="C1196" t="inlineStr">
         <is>
-          <t>[ 6.34509588e+05  6.32399112e+05  6.06559344e+05  7.02049212e+05
-  7.30612347e+05  7.49174784e+05  7.72904831e+05  7.92222826e+05
-  7.93250671e+05  7.75947406e+05  7.50568152e+05  7.20397053e+05
-  6.85032483e+05  6.44904686e+05  6.00952595e+05  5.54032281e+05
-  5.05142628e+05  4.55000711e+05  4.04309168e+05  3.53652171e+05
-  2.99688337e+05  2.46335801e+05  2.00944807e+05  1.55971782e+05
-  1.16085825e+05  8.25695642e+04  5.44152764e+04  3.09274739e+04
-  1.23548449e+04 -6.72107320e+02]</t>
+          <t>[ 6.48030117e+05  6.45869090e+05  6.57101741e+05  7.59727994e+05
+  7.75643883e+05  7.89436595e+05  8.06116323e+05  8.16139092e+05
+  8.10035043e+05  7.90301618e+05  7.64476750e+05  7.34092595e+05
+  6.98645796e+05  6.58484127e+05  6.14496817e+05  5.67587098e+05
+  5.18796200e+05  4.68801734e+05  4.17335598e+05  3.64316996e+05
+  3.05716034e+05  2.47805650e+05  2.03363417e+05  1.56575169e+05
+  1.15658742e+05  8.20225437e+04  5.42738925e+04  3.10874176e+04
+  1.24867633e+04 -5.93718997e+02]</t>
         </is>
       </c>
       <c r="D1196" t="inlineStr">
@@ -32717,14 +32753,14 @@
       </c>
       <c r="C1197" t="inlineStr">
         <is>
-          <t>[4.92881120e+05 5.40320187e+05 5.65700010e+05 5.75409054e+05
- 5.74065788e+05 5.65496024e+05 5.52107268e+05 5.35195599e+05
- 5.15523047e+05 4.93406624e+05 4.68890922e+05 4.41957740e+05
- 4.12661849e+05 3.81380895e+05 3.48736892e+05 3.15726615e+05
- 2.83145796e+05 2.51559914e+05 2.21662296e+05 1.92452217e+05
- 1.43522212e+05 9.72173309e+04 7.51263028e+04 5.67138934e+04
- 4.12905842e+04 2.85413291e+04 1.81190697e+04 9.88714567e+03
- 3.78358604e+03 1.63709046e-11]</t>
+          <t>[ 5.94274706e+05  6.41624454e+05  6.66828461e+05  6.76425726e+05
+  6.75130244e+05  6.66829377e+05  6.53956750e+05  6.37813032e+05
+  6.19196479e+05  5.98384200e+05  5.75293861e+05  5.49930111e+05
+  5.22379358e+05  4.92960342e+05  4.62193346e+05  4.31008255e+05
+  4.00233218e+05  3.67548724e+05  3.29951026e+05  2.86510401e+05
+  2.08229806e+05  1.33537756e+05  9.73816167e+04  6.76737883e+04
+  4.45757147e+04  2.79644100e+04  1.69643473e+04  9.39730552e+03
+  3.66791413e+03 -1.10958354e-10]</t>
         </is>
       </c>
       <c r="D1197" t="inlineStr">
@@ -32742,14 +32778,14 @@
       <c r="B1198" t="inlineStr"/>
       <c r="C1198" t="inlineStr">
         <is>
-          <t>[ 3.15790711e-04 -1.02896471e-03 -1.31316820e-03 -1.72711262e-03
- -2.11666392e-03 -2.39598236e-03 -2.46919246e-03 -2.55347966e-03
- -2.59981392e-03 -2.58013029e-03 -2.52916225e-03 -2.46879838e-03
- -2.39643356e-03 -2.34466889e-03 -2.28761851e-03 -2.24148992e-03
- -2.17636799e-03 -2.09375943e-03 -1.99408708e-03 -1.46546701e-03
- -1.09338340e-03 -1.30509122e-03 -1.40883807e-03 -1.35072271e-03
- -1.25090346e-03 -1.12026158e-03 -9.30060335e-04 -6.60239420e-04
- -3.03522220e-04  1.78621441e-07]</t>
+          <t>[ 3.03656383e-04 -1.10836038e-03 -1.47078910e-03 -1.96448549e-03
+ -2.50087953e-03 -2.92473702e-03 -3.03869298e-03 -3.17160169e-03
+ -3.29814341e-03 -3.23941097e-03 -3.11616876e-03 -3.08405059e-03
+ -3.00644807e-03 -2.95478378e-03 -2.82958541e-03 -2.74524793e-03
+ -2.65592592e-03 -1.45455475e-03 -9.28467548e-04 -6.61498996e-04
+ -3.59236893e-04 -6.06169899e-04 -6.23469929e-04 -6.49455001e-04
+ -7.16427940e-04 -8.63733625e-04 -1.13272602e-03 -7.70886337e-04
+ -3.36127967e-04  1.89497061e-07]</t>
         </is>
       </c>
       <c r="D1198" t="inlineStr">
@@ -32767,14 +32803,14 @@
       <c r="B1199" t="inlineStr"/>
       <c r="C1199" t="inlineStr">
         <is>
-          <t>[ 3.15790711e-04  9.95012134e-04  1.32620841e-03  1.26261384e-03
-  1.70623817e-03  2.06960338e-03  2.17767584e-03  2.29921748e-03
-  2.33376635e-03  2.28111135e-03  2.23944745e-03  2.19563062e-03
-  2.14486297e-03  2.11750359e-03  2.08802064e-03  2.06589219e-03
-  2.02235974e-03  1.95542034e-03  1.87171199e-03  1.37549151e-03
-  1.03695364e-03  1.25702421e-03  1.36596465e-03  1.33064368e-03
-  1.22761634e-03  1.09311251e-03  9.00925095e-04  6.31343410e-04
-  2.79793523e-04 -1.61251425e-07]</t>
+          <t>[ 3.03656383e-04  1.06635004e-03  1.50492298e-03  1.44168392e-03
+  2.07320581e-03  2.59174839e-03  2.72884745e-03  2.89041854e-03
+  2.99342462e-03  2.89389707e-03  2.78365484e-03  2.77059572e-03
+  2.71788039e-03  2.69124621e-03  2.59693185e-03  2.53696645e-03
+  2.46777809e-03  1.32701478e-03  8.50532381e-04  6.14165110e-04
+  3.68513298e-04  5.78849588e-04  6.05842541e-04  6.42129616e-04
+  7.06531847e-04  8.46374337e-04  1.09458861e-03  7.35448428e-04
+  3.09497576e-04 -1.71064424e-07]</t>
         </is>
       </c>
       <c r="D1199" t="inlineStr">
@@ -32792,14 +32828,14 @@
       <c r="B1200" t="inlineStr"/>
       <c r="C1200" t="inlineStr">
         <is>
-          <t>[ 3.15790711e-04 -2.94600600e-04 -1.12666583e-05 -2.17727189e-04
- -7.21410619e-04 -9.63228329e-04 -9.94908535e-04 -8.69210503e-04
- -8.76437251e-04 -9.66393516e-04 -9.63644803e-04 -9.16018383e-04
- -8.55660335e-04 -7.57253555e-04 -6.62623662e-04 -4.93233691e-04
- -4.34840903e-04 -3.99045986e-04 -3.64565326e-04 -3.10145823e-04
- -2.51477987e-04 -2.11909188e-04 -1.74808140e-04 -1.11203452e-04
- -6.72156416e-05 -2.13049630e-05  2.13547248e-05  4.68739365e-05
-  4.82456123e-05 -7.65542097e-08]</t>
+          <t>[ 3.03656383e-04 -2.35543409e-04  1.61119225e-04 -1.89375742e-04
+ -6.84019989e-04 -9.76624924e-04 -1.04811797e-03 -9.36836516e-04
+ -9.57253517e-04 -1.04936730e-03 -1.04366265e-03 -9.98636443e-04
+ -9.38080445e-04 -8.36941053e-04 -7.26169641e-04 -5.24040023e-04
+ -4.63366673e-04 -3.63840107e-04 -2.94851207e-04 -2.40697108e-04
+ -1.49300924e-05 -1.94371308e-04 -1.10323843e-04 -7.85238663e-05
+ -5.89340747e-05 -2.88176376e-05  3.49399645e-05  5.97900280e-05
+  5.41910139e-05 -8.13158341e-08]</t>
         </is>
       </c>
       <c r="D1200" t="inlineStr">
@@ -32817,14 +32853,14 @@
       <c r="B1201" t="inlineStr"/>
       <c r="C1201" t="inlineStr">
         <is>
-          <t>[ 3.15790711e-04 -2.94600600e-04 -1.12666583e-05 -2.17727189e-04
- -7.21410619e-04 -9.63228329e-04 -9.94908535e-04 -8.69210503e-04
- -8.76437251e-04 -9.66393516e-04 -9.63644803e-04 -9.16018383e-04
- -8.55660335e-04 -7.57253555e-04 -6.62623662e-04 -4.93233691e-04
- -4.34840903e-04 -3.99045986e-04 -3.64565326e-04 -3.10145823e-04
- -2.51477987e-04 -2.11909188e-04 -1.74808140e-04 -1.11203452e-04
- -6.72156416e-05 -2.13049630e-05  2.13547248e-05  4.68739365e-05
-  4.82456123e-05 -7.65542097e-08]</t>
+          <t>[ 3.03656383e-04 -2.35543409e-04  1.61119225e-04 -1.89375742e-04
+ -6.84019989e-04 -9.76624924e-04 -1.04811797e-03 -9.36836516e-04
+ -9.57253517e-04 -1.04936730e-03 -1.04366265e-03 -9.98636443e-04
+ -9.38080445e-04 -8.36941053e-04 -7.26169641e-04 -5.24040023e-04
+ -4.63366673e-04 -3.63840107e-04 -2.94851207e-04 -2.40697108e-04
+ -1.49300924e-05 -1.94371308e-04 -1.10323843e-04 -7.85238663e-05
+ -5.89340747e-05 -2.88176376e-05  3.49399645e-05  5.97900280e-05
+  5.41910139e-05 -8.13158341e-08]</t>
         </is>
       </c>
       <c r="D1201" t="inlineStr">
@@ -32890,7 +32926,7 @@
       </c>
       <c r="C1204" t="inlineStr">
         <is>
-          <t>[ 0.          0.         -0.05554909  0.065782    0.02174742  0.        ]</t>
+          <t>[ 0.          0.         -0.05554909  0.06183423  0.01826913  0.        ]</t>
         </is>
       </c>
       <c r="D1204" t="inlineStr">
@@ -32912,7 +32948,7 @@
       </c>
       <c r="C1205" t="inlineStr">
         <is>
-          <t>[ 0.          0.         -0.05554909  0.065782    0.02174742  0.        ]</t>
+          <t>[ 0.          0.         -0.05554909  0.06183423  0.01826913  0.        ]</t>
         </is>
       </c>
       <c r="D1205" t="inlineStr">
@@ -32934,7 +32970,7 @@
       </c>
       <c r="C1206" t="inlineStr">
         <is>
-          <t>[12.50700477]</t>
+          <t>[12.73527134]</t>
         </is>
       </c>
       <c r="D1206" t="inlineStr">
@@ -33112,11 +33148,9 @@
       <c r="B1215" t="inlineStr"/>
       <c r="C1215" t="inlineStr">
         <is>
-          <t>[9.02259174e-02 3.36727284e-01 4.99318664e-01 6.50964170e-01
- 7.08018515e-01 7.37926687e-01 7.34880773e-01 7.10817331e-01
- 6.81581639e-01 6.57894791e-01 6.35529305e-01 6.03185915e-01
- 5.22044122e-01 3.29180983e-01 3.83803927e-01 3.87668605e-01
- 3.41684674e-01 2.68591693e-01 1.40362319e-01 5.10346974e-05]</t>
+          <t>[8.67589665e-02 5.95338333e-01 8.85075292e-01 9.02071284e-01
+ 8.45864074e-01 7.20697209e-01 1.60212846e-01 1.82258880e-01
+ 3.06557124e-01 5.41420173e-05]</t>
         </is>
       </c>
       <c r="D1215" t="inlineStr">
@@ -33134,11 +33168,9 @@
       <c r="B1216" t="inlineStr"/>
       <c r="C1216" t="inlineStr">
         <is>
-          <t>[9.02259174e-02 3.34093133e-01 3.67417853e-01 5.47602144e-01
- 6.25848485e-01 6.63153663e-01 6.49866525e-01 6.31276432e-01
- 6.11172315e-01 5.98794088e-01 5.86981795e-01 5.62717954e-01
- 4.90003082e-01 3.11544853e-01 3.70617190e-01 3.81246194e-01
- 3.34566615e-01 2.60297206e-01 1.32805651e-01 4.60718356e-05]</t>
+          <t>[8.67589665e-02 4.52006319e-01 8.00187664e-01 8.05829215e-01
+ 7.69773018e-01 6.68864747e-01 1.52080335e-01 1.78857722e-01
+ 2.96979965e-01 4.88755497e-05]</t>
         </is>
       </c>
       <c r="D1216" t="inlineStr">
@@ -33156,14 +33188,14 @@
       <c r="B1217" t="inlineStr"/>
       <c r="C1217" t="inlineStr">
         <is>
-          <t>[7.89476777e-02 7.36501501e-02 2.81666458e-03 5.44317973e-02
- 1.80352655e-01 2.40807082e-01 2.48727134e-01 2.17302626e-01
- 2.19109313e-01 2.41598379e-01 2.40911201e-01 2.29004596e-01
- 2.13915084e-01 1.89313389e-01 1.65655915e-01 1.23308423e-01
- 1.08710226e-01 9.97614966e-02 9.11413314e-02 7.75364557e-02
- 6.28694967e-02 5.29772970e-02 4.37020350e-02 2.78008631e-02
- 1.68039104e-02 5.32624075e-03 5.33868120e-03 1.17184841e-02
- 1.20614031e-02 1.91385524e-05]</t>
+          <t>[7.59140957e-02 5.88858523e-02 4.02798062e-02 4.73439356e-02
+ 1.71004997e-01 2.44156231e-01 2.62029494e-01 2.34209129e-01
+ 2.39313379e-01 2.62341824e-01 2.60915662e-01 2.49659111e-01
+ 2.34520111e-01 2.09235263e-01 1.81542410e-01 1.31010006e-01
+ 1.15841668e-01 9.09600269e-02 7.37128019e-02 6.01742771e-02
+ 3.73252310e-03 4.85928270e-02 2.75809607e-02 1.96309666e-02
+ 1.47335187e-02 7.20440941e-03 8.73499113e-03 1.49475070e-02
+ 1.35477535e-02 2.03289585e-05]</t>
         </is>
       </c>
       <c r="D1217" t="inlineStr">
@@ -33181,14 +33213,14 @@
       <c r="B1218" t="inlineStr"/>
       <c r="C1218" t="inlineStr">
         <is>
-          <t>[7.89476777e-02 7.36501501e-02 2.81666458e-03 5.44317973e-02
- 1.80352655e-01 2.40807082e-01 2.48727134e-01 2.17302626e-01
- 2.19109313e-01 2.41598379e-01 2.40911201e-01 2.29004596e-01
- 2.13915084e-01 1.89313389e-01 1.65655915e-01 1.23308423e-01
- 1.08710226e-01 9.97614966e-02 9.11413314e-02 7.75364557e-02
- 6.28694967e-02 5.29772970e-02 4.37020350e-02 2.78008631e-02
- 1.68039104e-02 5.32624075e-03 5.33868120e-03 1.17184841e-02
- 1.20614031e-02 1.91385524e-05]</t>
+          <t>[7.59140957e-02 5.88858523e-02 4.02798062e-02 4.73439356e-02
+ 1.71004997e-01 2.44156231e-01 2.62029494e-01 2.34209129e-01
+ 2.39313379e-01 2.62341824e-01 2.60915662e-01 2.49659111e-01
+ 2.34520111e-01 2.09235263e-01 1.81542410e-01 1.31010006e-01
+ 1.15841668e-01 9.09600269e-02 7.37128019e-02 6.01742771e-02
+ 3.73252310e-03 4.85928270e-02 2.75809607e-02 1.96309666e-02
+ 1.47335187e-02 7.20440941e-03 8.73499113e-03 1.49475070e-02
+ 1.35477535e-02 2.03289585e-05]</t>
         </is>
       </c>
       <c r="D1218" t="inlineStr">
@@ -33206,7 +33238,7 @@
       <c r="B1219" t="inlineStr"/>
       <c r="C1219" t="inlineStr">
         <is>
-          <t>[-0.13605136 -1.12789399 -2.575202   -6.46278846 -9.4499758 ]</t>
+          <t>[-0.04070071 -1.32785147 -2.65188158 -4.9624404  -6.61225018]</t>
         </is>
       </c>
       <c r="D1219" t="inlineStr">
@@ -33224,7 +33256,7 @@
       <c r="B1220" t="inlineStr"/>
       <c r="C1220" t="inlineStr">
         <is>
-          <t>[-0.40961051 -2.00181932 -3.99802234 -4.84688815 -8.35337447]</t>
+          <t>[ -0.30331183  -2.17312808  -4.14182839  -8.37446878 -12.59268586]</t>
         </is>
       </c>
       <c r="D1220" t="inlineStr">
@@ -33246,7 +33278,7 @@
       </c>
       <c r="C1221" t="inlineStr">
         <is>
-          <t>[5.43024329]</t>
+          <t>[5.42384066]</t>
         </is>
       </c>
       <c r="D1221" t="inlineStr">
@@ -33264,7 +33296,7 @@
       <c r="B1222" t="inlineStr"/>
       <c r="C1222" t="inlineStr">
         <is>
-          <t>[1.21795296]</t>
+          <t>[1.21651691]</t>
         </is>
       </c>
       <c r="D1222" t="inlineStr">
@@ -33286,7 +33318,7 @@
       </c>
       <c r="C1223" t="inlineStr">
         <is>
-          <t>[0.0809377]</t>
+          <t>[0.08293418]</t>
         </is>
       </c>
       <c r="D1223" t="inlineStr">
@@ -33308,7 +33340,7 @@
       </c>
       <c r="C1224" t="inlineStr">
         <is>
-          <t>[1.584]</t>
+          <t>[1.27728]</t>
         </is>
       </c>
       <c r="D1224" t="inlineStr">
@@ -33326,7 +33358,7 @@
       <c r="B1225" t="inlineStr"/>
       <c r="C1225" t="inlineStr">
         <is>
-          <t>[1.98]</t>
+          <t>[1.]</t>
         </is>
       </c>
       <c r="D1225" t="inlineStr">
@@ -33344,7 +33376,7 @@
       <c r="B1226" t="inlineStr"/>
       <c r="C1226" t="inlineStr">
         <is>
-          <t>[2.05196433]</t>
+          <t>[1.]</t>
         </is>
       </c>
       <c r="D1226" t="inlineStr">
@@ -33366,7 +33398,7 @@
       </c>
       <c r="C1227" t="inlineStr">
         <is>
-          <t>[0.33194954]</t>
+          <t>[0.]</t>
         </is>
       </c>
       <c r="D1227" t="inlineStr">
@@ -33384,7 +33416,7 @@
       <c r="B1228" t="inlineStr"/>
       <c r="C1228" t="inlineStr">
         <is>
-          <t>[22.]</t>
+          <t>[17.72]</t>
         </is>
       </c>
       <c r="D1228" t="inlineStr">
@@ -33406,7 +33438,7 @@
       </c>
       <c r="C1229" t="inlineStr">
         <is>
-          <t>[976.61986675]</t>
+          <t>[786.34407823]</t>
         </is>
       </c>
       <c r="D1229" t="inlineStr">
@@ -33454,8 +33486,8 @@
       </c>
       <c r="C1231" t="inlineStr">
         <is>
-          <t>[  0.81891207   8.1331339    2.10972041   1.88240942   0.37027748
- -16.82621162   4.91128476   2.15633535   2.43307155   9.31732766
+          <t>[  0.81891207   8.1331339    2.7550697    2.75165494   0.37027748
+ -16.82621162   4.86149381   2.11602898   2.37607035   9.2540771
    7.91668029   0.05980584   0.74488503   0.06224921   0.13957751
    1.96811402   0.14821459]</t>
         </is>
@@ -33479,8 +33511,8 @@
       </c>
       <c r="C1232" t="inlineStr">
         <is>
-          <t>[  0.81891207   0.         -16.45593414   3.99212983   0.40984714
-  16.04981419  21.53101836   0.           0.           0.        ]</t>
+          <t>[  0.81891207   0.         -16.45593414   5.50672465   0.40984714
+  16.04981419  21.32066929   0.           0.           0.        ]</t>
         </is>
       </c>
       <c r="D1232" t="inlineStr">
@@ -33502,8 +33534,8 @@
       </c>
       <c r="C1233" t="inlineStr">
         <is>
-          <t>[  1011.35640166    287.68539615 -31924.51223611   6387.40772574
-    795.10345651  31136.63952099   2799.0323871       0.
+          <t>[  1011.35640166    287.68539615 -31924.51223611   8810.75943256
+    795.10345651  31136.63952099   2771.6870075       0.
       0.              0.        ]</t>
         </is>
       </c>
@@ -33526,8 +33558,8 @@
       </c>
       <c r="C1234" t="inlineStr">
         <is>
-          <t>[  7312.10678398   2079.96541418 -44479.70983959  99894.14343995
-   1777.21906957  66348.91729222  36387.42103232   5134.42856522
+          <t>[  7312.10678398   2079.96541418 -44479.70983959 137793.50001793
+   1777.21906957  66348.91729222  36031.93109744   7079.86735371
       0.              0.        ]</t>
         </is>
       </c>
@@ -33550,8 +33582,8 @@
       </c>
       <c r="C1235" t="inlineStr">
         <is>
-          <t>[  9140.13347997   2079.96541418 -46703.69533157 104888.85061195
-   2043.80193001  76301.25488605  43664.90523878   5134.42856522
+          <t>[  9140.13347997   2079.96541418 -46703.69533157 144683.17501882
+   2043.80193001  76301.25488605  43238.31731693   7079.86735371
       0.              0.        ]</t>
         </is>
       </c>
@@ -33574,7 +33606,7 @@
       </c>
       <c r="C1236" t="inlineStr">
         <is>
-          <t>[2219.23132657]</t>
+          <t>[2219.69525514]</t>
         </is>
       </c>
       <c r="D1236" t="inlineStr">
@@ -33618,7 +33650,7 @@
       </c>
       <c r="C1238" t="inlineStr">
         <is>
-          <t>[225.22287087]</t>
+          <t>[225.34020711]</t>
         </is>
       </c>
       <c r="D1238" t="inlineStr">
@@ -33662,7 +33694,7 @@
       </c>
       <c r="C1240" t="inlineStr">
         <is>
-          <t>[12265.7221686]</t>
+          <t>[12290.68039925]</t>
         </is>
       </c>
       <c r="D1240" t="inlineStr">
@@ -33684,7 +33716,7 @@
       </c>
       <c r="C1241" t="inlineStr">
         <is>
-          <t>[266475.08947182]</t>
+          <t>[307813.22297597]</t>
         </is>
       </c>
       <c r="D1241" t="inlineStr">
@@ -33706,7 +33738,7 @@
       </c>
       <c r="C1242" t="inlineStr">
         <is>
-          <t>[74984.73423427]</t>
+          <t>[75000.66630404]</t>
         </is>
       </c>
       <c r="D1242" t="inlineStr">
@@ -33728,7 +33760,7 @@
       </c>
       <c r="C1243" t="inlineStr">
         <is>
-          <t>[1178.83057437]</t>
+          <t>[1198.03641206]</t>
         </is>
       </c>
       <c r="D1243" t="inlineStr">
@@ -33750,7 +33782,7 @@
       </c>
       <c r="C1244" t="inlineStr">
         <is>
-          <t>[342638.65428045]</t>
+          <t>[384011.92569207]</t>
         </is>
       </c>
       <c r="D1244" t="inlineStr">
@@ -33772,7 +33804,7 @@
       </c>
       <c r="C1245" t="inlineStr">
         <is>
-          <t>[14501.0051151]</t>
+          <t>[14502.56336444]</t>
         </is>
       </c>
       <c r="D1245" t="inlineStr">
@@ -33794,7 +33826,7 @@
       </c>
       <c r="C1246" t="inlineStr">
         <is>
-          <t>[22083.00015169]</t>
+          <t>[22132.89385145]</t>
         </is>
       </c>
       <c r="D1246" t="inlineStr">
@@ -33816,7 +33848,7 @@
       </c>
       <c r="C1247" t="inlineStr">
         <is>
-          <t>[1428.81554829]</t>
+          <t>[1429.51413205]</t>
         </is>
       </c>
       <c r="D1247" t="inlineStr">
@@ -33838,7 +33870,7 @@
       </c>
       <c r="C1248" t="inlineStr">
         <is>
-          <t>[11048.26072826]</t>
+          <t>[11057.70532047]</t>
         </is>
       </c>
       <c r="D1248" t="inlineStr">
@@ -33860,7 +33892,7 @@
       </c>
       <c r="C1249" t="inlineStr">
         <is>
-          <t>[22495.42027028]</t>
+          <t>[22500.19989121]</t>
         </is>
       </c>
       <c r="D1249" t="inlineStr">
@@ -33882,7 +33914,7 @@
       </c>
       <c r="C1250" t="inlineStr">
         <is>
-          <t>[22667.97967399]</t>
+          <t>[23372.94774269]</t>
         </is>
       </c>
       <c r="D1250" t="inlineStr">
@@ -33904,7 +33936,7 @@
       </c>
       <c r="C1251" t="inlineStr">
         <is>
-          <t>[94224.48148762]</t>
+          <t>[94995.82430231]</t>
         </is>
       </c>
       <c r="D1251" t="inlineStr">
@@ -33926,7 +33958,7 @@
       </c>
       <c r="C1252" t="inlineStr">
         <is>
-          <t>[436863.13576807]</t>
+          <t>[479007.74999438]</t>
         </is>
       </c>
       <c r="D1252" t="inlineStr">
@@ -34661,7 +34693,7 @@
       </c>
       <c r="C1294" t="inlineStr">
         <is>
-          <t>[187361.07439584]</t>
+          <t>[194394.44415464]</t>
         </is>
       </c>
       <c r="D1294" t="inlineStr"/>
@@ -34679,7 +34711,7 @@
       </c>
       <c r="C1295" t="inlineStr">
         <is>
-          <t>[421443.65817399]</t>
+          <t>[428477.0279328]</t>
         </is>
       </c>
       <c r="D1295" t="inlineStr"/>
@@ -34697,7 +34729,7 @@
       </c>
       <c r="C1296" t="inlineStr">
         <is>
-          <t>[-5.21344714 -0.07454204  2.09295425]</t>
+          <t>[-5.32135284 -0.07331844  2.10755   ]</t>
         </is>
       </c>
       <c r="D1296" t="inlineStr"/>
@@ -34715,8 +34747,8 @@
       </c>
       <c r="C1297" t="inlineStr">
         <is>
-          <t>[ 2.08546242e+08  1.32824718e+08  1.31782070e+08 -1.66639598e+01
- -6.43161299e+05  4.82222779e+04]</t>
+          <t>[ 2.50905849e+08  1.55068890e+08  1.54066831e+08 -1.66639598e+01
+ -1.87087268e+06  4.82222779e+04]</t>
         </is>
       </c>
       <c r="D1297" t="inlineStr"/>
@@ -34734,7 +34766,7 @@
       </c>
       <c r="C1298" t="inlineStr">
         <is>
-          <t>[0.00198911]</t>
+          <t>[0.00199447]</t>
         </is>
       </c>
       <c r="D1298" t="inlineStr"/>
@@ -34771,9 +34803,9 @@
       <c r="C1300" t="inlineStr">
         <is>
           <t>[[3.79442275e+06]
- [2.30298378e+08]
- [2.14183597e+08]
- [2.51810441e+08]]</t>
+ [2.30930085e+08]
+ [2.14783899e+08]
+ [2.54139928e+08]]</t>
         </is>
       </c>
       <c r="D1300" t="inlineStr"/>
@@ -34794,7 +34826,7 @@
           <t>[[1.00720901e+09]
  [1.00811611e+09]
  [1.00820964e+09]
- [1.00427825e+09]]</t>
+ [1.00444804e+09]]</t>
         </is>
       </c>
       <c r="D1301" t="inlineStr"/>
@@ -34809,9 +34841,9 @@
       <c r="C1302" t="inlineStr">
         <is>
           <t>[[6.80371107]
- [6.86879756]
- [6.86148963]
- [6.85461241]]</t>
+ [6.86912014]
+ [6.86177503]
+ [6.85705482]]</t>
         </is>
       </c>
       <c r="D1302" t="inlineStr"/>
@@ -34937,7 +34969,7 @@
       </c>
       <c r="C1309" t="inlineStr">
         <is>
-          <t>[0.00014631]</t>
+          <t>[0.0001501]</t>
         </is>
       </c>
       <c r="D1309" t="inlineStr"/>
@@ -34955,7 +34987,7 @@
       </c>
       <c r="C1310" t="inlineStr">
         <is>
-          <t>[9.41546115e-05]</t>
+          <t>[9.62538683e-05]</t>
         </is>
       </c>
       <c r="D1310" t="inlineStr"/>
@@ -34973,7 +35005,7 @@
       </c>
       <c r="C1311" t="inlineStr">
         <is>
-          <t>[0.00012558]</t>
+          <t>[0.00012813]</t>
         </is>
       </c>
       <c r="D1311" t="inlineStr"/>
@@ -34991,7 +35023,7 @@
       </c>
       <c r="C1312" t="inlineStr">
         <is>
-          <t>[4.44154339e-05]</t>
+          <t>[4.38364248e-05]</t>
         </is>
       </c>
       <c r="D1312" t="inlineStr"/>
@@ -35009,7 +35041,7 @@
       </c>
       <c r="C1313" t="inlineStr">
         <is>
-          <t>[5.50718309e-05]</t>
+          <t>[5.46621387e-05]</t>
         </is>
       </c>
       <c r="D1313" t="inlineStr"/>
@@ -35027,7 +35059,7 @@
       </c>
       <c r="C1314" t="inlineStr">
         <is>
-          <t>[7.35565128e-05]</t>
+          <t>[7.35566408e-05]</t>
         </is>
       </c>
       <c r="D1314" t="inlineStr"/>
@@ -35045,9 +35077,9 @@
       </c>
       <c r="C1315" t="inlineStr">
         <is>
-          <t>[[ 2199361.42160199]
- [   41405.95953997]
- [-2466864.63319846]]</t>
+          <t>[[ 2199361.16592555]
+ [   41406.03687367]
+ [-2486818.06298609]]</t>
         </is>
       </c>
       <c r="D1315" t="inlineStr"/>
@@ -35065,9 +35097,9 @@
       </c>
       <c r="C1316" t="inlineStr">
         <is>
-          <t>[[15682220.2180832 ]
- [ 2135803.94066418]
- [ 1127332.34182628]]</t>
+          <t>[[15682220.23527616]
+ [ 2104472.63685562]
+ [ 1127331.99235724]]</t>
         </is>
       </c>
       <c r="D1316" t="inlineStr"/>
@@ -35085,28 +35117,28 @@
       </c>
       <c r="C1317" t="inlineStr">
         <is>
-          <t>[[6.27374596e+04]
- [8.24472170e+05]
- [4.43143679e+05]
- [1.51818246e+06]
- [3.18686809e+06]
- [1.33413150e+07]
- [1.27503722e+07]
- [8.16251593e+06]
- [6.05887902e+06]
- [6.27383157e+04]
- [1.03041608e+00]
- [6.27359792e+04]
- [3.64115419e+05]
- [1.23637959e+06]
- [2.31141761e+06]
- [4.49405727e+06]
- [2.19311258e+07]
- [2.20158312e+07]
- [8.05318810e+06]
- [6.02243524e+06]
- [6.27385900e+04]
- [9.53738917e-01]]</t>
+          <t>[[6.27380451e+04]
+ [8.24469818e+05]
+ [4.43147308e+05]
+ [1.51818789e+06]
+ [3.18687661e+06]
+ [1.33159290e+07]
+ [1.27325081e+07]
+ [8.20008661e+06]
+ [6.05887953e+06]
+ [6.27406480e+04]
+ [2.42589210e+00]
+ [6.27364152e+04]
+ [3.64117425e+05]
+ [1.23638407e+06]
+ [2.31142420e+06]
+ [4.49406778e+06]
+ [2.19057106e+07]
+ [2.19979200e+07]
+ [8.09075607e+06]
+ [6.02243299e+06]
+ [6.27400901e+04]
+ [2.37243757e+00]]</t>
         </is>
       </c>
       <c r="D1317" t="inlineStr"/>
@@ -35124,28 +35156,28 @@
       </c>
       <c r="C1318" t="inlineStr">
         <is>
-          <t>[[3.16204518e+05]
- [6.54097161e+05]
- [8.90667384e+05]
- [1.12782043e+06]
- [1.51993488e+06]
- [1.26972604e+07]
- [1.26645891e+07]
- [1.10683884e+07]
- [1.09102864e+07]
- [3.16200144e+05]
- [1.15466424e+00]
- [3.16197089e+05]
- [5.98467819e+06]
- [6.22135709e+06]
- [6.45850451e+06]
- [6.85036136e+06]
- [1.01312264e+07]
- [1.00989204e+07]
- [1.10683837e+07]
- [1.09102850e+07]
- [3.16201725e+05]
- [1.47026157e+00]]</t>
+          <t>[[3.16206408e+05]
+ [6.54102076e+05]
+ [8.90670473e+05]
+ [1.12782308e+06]
+ [1.51993821e+06]
+ [1.28865623e+07]
+ [1.28538915e+07]
+ [1.12577007e+07]
+ [1.10995984e+07]
+ [3.16196418e+05]
+ [2.17121741e+00]
+ [3.16198210e+05]
+ [5.98468130e+06]
+ [6.22136592e+06]
+ [6.45851495e+06]
+ [6.85037288e+06]
+ [1.03205508e+07]
+ [1.02882434e+07]
+ [1.12577012e+07]
+ [1.10996056e+07]
+ [3.16204864e+05]
+ [2.29501233e+00]]</t>
         </is>
       </c>
       <c r="D1318" t="inlineStr"/>
@@ -35198,28 +35230,28 @@
       <c r="B1320" t="inlineStr"/>
       <c r="C1320" t="inlineStr">
         <is>
-          <t>[[2.14992918e-03]
- [5.46457174e-03]
- [6.25976302e-03]
- [9.64870936e-03]
- [1.61210803e-02]
- [1.00318125e-01]
- [9.89514964e-02]
- [8.12618448e-02]
- [7.73944230e-02]
- [2.14990021e-03]
- [8.77413834e-09]
- [2.14987867e-03]
- [4.04514232e-02]
- [4.23009768e-02]
- [4.45487720e-02]
- [4.94822101e-02]
- [1.09540685e-01]
- [1.09662938e-01]
- [8.10957330e-02]
- [7.73511378e-02]
- [2.14991094e-03]
- [1.06052935e-08]]</t>
+          <t>[[2.14994213e-03]
+ [5.46459318e-03]
+ [6.25978698e-03]
+ [9.64873650e-03]
+ [1.61211202e-02]
+ [1.01362825e-01]
+ [1.00024496e-01]
+ [8.24966528e-02]
+ [7.86131342e-02]
+ [2.14987624e-03]
+ [1.74533203e-08]
+ [2.14988639e-03]
+ [4.04514446e-02]
+ [4.23010381e-02]
+ [4.45488463e-02]
+ [4.94822974e-02]
+ [1.10267386e-01]
+ [1.10408741e-01]
+ [8.23323014e-02]
+ [7.85705725e-02]
+ [2.14993267e-03]
+ [1.80539694e-08]]</t>
         </is>
       </c>
       <c r="D1320" t="inlineStr"/>
@@ -35233,7 +35265,7 @@
       <c r="B1321" t="inlineStr"/>
       <c r="C1321" t="inlineStr">
         <is>
-          <t>[0.00508963]</t>
+          <t>[0.00502328]</t>
         </is>
       </c>
       <c r="D1321" t="inlineStr"/>
@@ -35247,7 +35279,7 @@
       <c r="B1322" t="inlineStr"/>
       <c r="C1322" t="inlineStr">
         <is>
-          <t>[0.00070605]</t>
+          <t>[0.0007008]</t>
         </is>
       </c>
       <c r="D1322" t="inlineStr"/>
@@ -35283,7 +35315,7 @@
       </c>
       <c r="C1324" t="inlineStr">
         <is>
-          <t>[2176787.80088246]</t>
+          <t>[2390466.84783703]</t>
         </is>
       </c>
       <c r="D1324" t="inlineStr"/>
@@ -36014,7 +36046,7 @@
       </c>
       <c r="C1360" t="inlineStr">
         <is>
-          <t>[1283916.81761933]</t>
+          <t>[1290950.18737814]</t>
         </is>
       </c>
       <c r="D1360" t="inlineStr"/>
@@ -36032,7 +36064,7 @@
       </c>
       <c r="C1361" t="inlineStr">
         <is>
-          <t>[-1.71130575e+00 -2.44683058e-02  8.23609247e+01]</t>
+          <t>[-1.76620095e+00 -2.43349972e-02  8.26912019e+01]</t>
         </is>
       </c>
       <c r="D1361" t="inlineStr"/>
@@ -36050,8 +36082,8 @@
       </c>
       <c r="C1362" t="inlineStr">
         <is>
-          <t>[ 1.23481278e+10  1.22838588e+10  1.50850833e+08 -1.63798510e+05
-  3.11559817e+08  4.51211070e+06]</t>
+          <t>[ 1.25342714e+10  1.24505652e+10  1.73813801e+08 -1.67188396e+05
+  3.22145347e+08  4.51256922e+06]</t>
         </is>
       </c>
       <c r="D1362" t="inlineStr"/>
@@ -36636,7 +36668,7 @@
       </c>
       <c r="C1393" t="inlineStr">
         <is>
-          <t>[2199361.42160199]</t>
+          <t>[2199361.16592555]</t>
         </is>
       </c>
       <c r="D1393" t="inlineStr"/>
@@ -36654,7 +36686,7 @@
       </c>
       <c r="C1394" t="inlineStr">
         <is>
-          <t>[41405.95953997]</t>
+          <t>[41406.03687367]</t>
         </is>
       </c>
       <c r="D1394" t="inlineStr"/>
@@ -36672,7 +36704,7 @@
       </c>
       <c r="C1395" t="inlineStr">
         <is>
-          <t>[-2466864.63319846]</t>
+          <t>[-2486818.06298609]</t>
         </is>
       </c>
       <c r="D1395" t="inlineStr"/>
@@ -36690,7 +36722,7 @@
       </c>
       <c r="C1396" t="inlineStr">
         <is>
-          <t>[15682220.2180832]</t>
+          <t>[15682220.23527616]</t>
         </is>
       </c>
       <c r="D1396" t="inlineStr"/>
@@ -36708,7 +36740,7 @@
       </c>
       <c r="C1397" t="inlineStr">
         <is>
-          <t>[2135803.94066418]</t>
+          <t>[2104472.63685562]</t>
         </is>
       </c>
       <c r="D1397" t="inlineStr"/>
@@ -36726,7 +36758,7 @@
       </c>
       <c r="C1398" t="inlineStr">
         <is>
-          <t>[1127332.34182628]</t>
+          <t>[1127331.99235724]</t>
         </is>
       </c>
       <c r="D1398" t="inlineStr"/>
@@ -36762,7 +36794,7 @@
       </c>
       <c r="C1400" t="inlineStr">
         <is>
-          <t>[0.46294619]</t>
+          <t>[0.46290446]</t>
         </is>
       </c>
       <c r="D1400" t="inlineStr"/>
@@ -36780,7 +36812,7 @@
       </c>
       <c r="C1401" t="inlineStr">
         <is>
-          <t>[0.46294619]</t>
+          <t>[0.46290446]</t>
         </is>
       </c>
       <c r="D1401" t="inlineStr"/>
@@ -36798,7 +36830,7 @@
       </c>
       <c r="C1402" t="inlineStr">
         <is>
-          <t>[0.46294619 0.46294619 2.16372761 2.16372761 5.40762355 5.40762355]</t>
+          <t>[0.46290446 0.46290446 2.16367621 2.16367621 5.40757735 5.40757735]</t>
         </is>
       </c>
       <c r="D1402" t="inlineStr"/>
@@ -36812,12 +36844,12 @@
       <c r="B1403" t="inlineStr"/>
       <c r="C1403" t="inlineStr">
         <is>
-          <t>[[  -433.80397148    139.33102692    -80.63468224    138.76542179
-     -59.25414178]
- [  2147.42650842  -2462.70759351  -2940.47260178   4075.36193459
-   -1142.8812346 ]
- [ -5543.17270673  18257.379219   -10809.1456805  -11159.21351035
-    9003.16034234]]</t>
+          <t>[[ 1.46743345e+00 -4.71184250e-01  2.72670249e-01 -4.69305223e-01
+   2.00385774e-01]
+ [ 2.14609541e+03 -2.46114339e+03 -2.93859293e+03  4.07263192e+03
+  -1.14206788e+03]
+ [ 2.20848254e+01 -7.27391460e+01  4.30617947e+01  4.44638547e+01
+  -3.58713288e+01]]</t>
         </is>
       </c>
       <c r="D1403" t="inlineStr"/>
@@ -36831,12 +36863,12 @@
       <c r="B1404" t="inlineStr"/>
       <c r="C1404" t="inlineStr">
         <is>
-          <t>[[ 1.46755525e+00 -4.71355713e-01  2.72786464e-01 -4.69442276e-01
-   2.00456272e-01]
- [ 2.14742651e+03 -2.46270759e+03 -2.94047260e+03  4.07536193e+03
-  -1.14288123e+03]
- [ 2.20850277e+01 -7.27407836e+01  4.30656403e+01  4.44603755e+01
-  -3.58702599e+01]]</t>
+          <t>[[ 1.46743345e+00 -4.71184250e-01  2.72670249e-01 -4.69305223e-01
+   2.00385774e-01]
+ [ 2.14609541e+03 -2.46114339e+03 -2.93859293e+03  4.07263192e+03
+  -1.14206788e+03]
+ [-7.00196994e+03  2.30618673e+04 -1.36526953e+04 -1.40972169e+04
+   1.13729659e+04]]</t>
         </is>
       </c>
       <c r="D1404" t="inlineStr"/>
@@ -36850,12 +36882,9 @@
       <c r="B1405" t="inlineStr"/>
       <c r="C1405" t="inlineStr">
         <is>
-          <t>[[ -2597.2179641    9865.10086231 -17529.38575002  14767.89840998
-   -4708.96922768]
- [     0.              0.              0.              0.
-       0.        ]
- [     0.              0.              0.              0.
-       0.        ]]</t>
+          <t>[[ 12.82110341 -48.69883083  86.53338705 -72.90137186  23.24571223]
+ [  0.           0.           0.           0.           0.        ]
+ [  0.           0.           0.           0.           0.        ]]</t>
         </is>
       </c>
       <c r="D1405" t="inlineStr"/>
@@ -36873,7 +36902,7 @@
       </c>
       <c r="C1406" t="inlineStr">
         <is>
-          <t>[0.46294619 2.16372761 5.40762355]</t>
+          <t>[0.46290446 2.16367621 5.40757735]</t>
         </is>
       </c>
       <c r="D1406" t="inlineStr"/>
@@ -36891,7 +36920,7 @@
       </c>
       <c r="C1407" t="inlineStr">
         <is>
-          <t>[0.46294619 2.16372761 5.40762355]</t>
+          <t>[0.46290446 2.16367621 5.40757735]</t>
         </is>
       </c>
       <c r="D1407" t="inlineStr"/>
@@ -36927,12 +36956,12 @@
       </c>
       <c r="C1409" t="inlineStr">
         <is>
-          <t>[0.         0.00332462 0.01271223 0.027958   0.04920565 0.07652809
- 0.10969425 0.14885086 0.19405898 0.24505692 0.3019559  0.36477158
- 0.43320902 0.50735878 0.58719809 0.67239356 0.76303837 0.85907884
- 0.96013255 1.06628864 1.17744027 1.29314025 1.41343403 1.53810858
- 1.66663193 1.79891407 1.93458965 2.07306861 2.21392317 2.35655924
- 2.50027913]</t>
+          <t>[0.         0.00332481 0.01271297 0.02795967 0.04920863 0.07653277
+ 0.10970102 0.14886011 0.1940711  0.24507228 0.30197488 0.36479453
+ 0.43323627 0.50739063 0.58723482 0.67243539 0.7630855  0.85913139
+ 0.96019058 1.06635217 1.17750918 1.29321436 1.41351303 1.538192
+ 1.66671917 1.79900434 1.93468193 2.07316165 2.21401547 2.35664895
+ 2.50036403]</t>
         </is>
       </c>
       <c r="D1409" t="inlineStr"/>
@@ -36950,7 +36979,7 @@
       </c>
       <c r="C1410" t="inlineStr">
         <is>
-          <t>[2.50027913]</t>
+          <t>[2.50036403]</t>
         </is>
       </c>
       <c r="D1410" t="inlineStr"/>
@@ -36968,14 +36997,14 @@
       </c>
       <c r="C1411" t="inlineStr">
         <is>
-          <t>[-9931629.12087864 -9492004.72238001 -9052380.32388137 -8659115.29522039
- -8265850.26655938 -7872585.23789839 -7523691.55816138 -7174797.87842438
- -6825904.19868737 -6515970.87015947 -6206037.54163157 -5896104.21310369
- -5622459.95773027 -5348815.70235683 -5075171.44698341 -4837701.64147476
- -4600231.83596612 -4362762.0304575  -4161055.65345227 -3959349.27644706
- -3757642.89944181 -3589530.81123417 -3421418.72302654 -3253306.63481891
- -3113092.20878868 -2973733.87135341 -2835231.63344629 -2709850.8539877
- -2587061.8575495  -2466864.63319846]</t>
+          <t>[-9951582.55066614 -9511958.15216751 -9072333.75366888 -8679068.72500789
+ -8285803.69634688 -7892538.66768589 -7543644.98794887 -7194751.30821188
+ -6845857.62847487 -6535924.29994697 -6225990.97141909 -5916057.64289117
+ -5642413.3875178  -5368769.13214438 -5095124.87677096 -4857655.07126236
+ -4620185.26575373 -4382715.4602451  -4181009.08323988 -3979302.70623463
+ -3777596.32922941 -3609484.24102176 -3441372.15281411 -3273260.06460648
+ -3133045.63857625 -2993687.301141   -2855185.06323387 -2729804.28377531
+ -2607015.28733709 -2486818.06298608]</t>
         </is>
       </c>
       <c r="D1411" t="inlineStr"/>
@@ -36993,14 +37022,14 @@
       </c>
       <c r="C1412" t="inlineStr">
         <is>
-          <t>[2280562.64427271 2279770.05413786 2278672.81598016 2277253.63856015
- 2275732.35833533 2274043.21671441 2272030.05823047 2270053.33291015
- 2267950.19580608 2265500.8753819  2263168.55372593 2260731.31672743
- 2257913.05778896 2255280.40975585 2252556.37080163 2249398.64370402
- 2246501.6974388  2243522.81235573 2240061.78120053 2236926.30139759
- 2233715.94206915 2230001.97457721 2226647.5214219  2223223.70876772
- 2219347.82260043 2215810.02359946 2212229.49023216 2208447.70998157
- 2204837.86516156 2201243.30517403]</t>
+          <t>[2280562.39752461 2279769.82516708 2278672.60460251 2277253.43891874
+ 2275732.17555393 2274043.0502648  2272029.89658648 2270053.18618753
+ 2267950.06313824 2265500.74143011 2263168.43175552 2260731.20554176
+ 2257912.93876146 2255280.29880151 2252556.26640344 2249398.52413985
+ 2246501.58111301 2243522.69746062 2240061.64495677 2236926.16270557
+ 2233715.79884497 2230001.8068529  2226647.34477608 2223223.5208791
+ 2219347.6113174  2215809.79584213 2212229.24333136 2208447.44141973
+ 2204837.57149407 2201242.98291472]</t>
         </is>
       </c>
       <c r="D1412" t="inlineStr"/>
@@ -37018,14 +37047,14 @@
       </c>
       <c r="C1413" t="inlineStr">
         <is>
-          <t>[41401.1098487  41390.8990243  41380.51372095 41373.22447787
- 41362.5188499  41351.64440961 41347.38331438 41336.19915007
- 41324.85121511 41323.06853921 41311.41831745 41299.60875452
- 41300.82174096 41288.71741515 41276.45761438 41282.01341695
- 41269.46666053 41256.76785922 41267.38656577 41254.40769817
- 41241.27998078 41256.57123133 41243.16897376 41229.62106681
- 41246.31712174 41233.34537042 41220.14177334 41223.71171475
- 41212.23825929 41200.27735505]</t>
+          <t>[41401.18551928 41390.97136982 41380.5827479  41373.2912497
+ 41362.5823369  41351.7046329  41347.44241337 41336.25504951
+ 41324.90395267 41323.1210767  41311.46779132 41299.6552213
+ 41300.86904498 41288.76184978 41276.49925778 41282.05724227
+ 41269.50787807 41256.80657225 41267.42886736 41254.44773215
+ 41241.31788054 41256.61385096 41243.20976042 41229.6601903
+ 41246.36119382 41233.3883504  41220.18387274 41223.75629844
+ 41212.28288922 41200.32232042]</t>
         </is>
       </c>
       <c r="D1413" t="inlineStr"/>
@@ -37043,14 +37072,14 @@
       </c>
       <c r="C1414" t="inlineStr">
         <is>
-          <t>[10873069.40812827 11059049.17163842 11243118.5144097  11425323.66089842
- 11605674.86920421 11784335.27992343 11961350.62867679 12136698.20588863
- 12310551.54049785 12482965.2016698  12653898.90033725 12823536.29826988
- 12991933.21968439 13159018.92345533 13324986.751249   13489880.15524416
- 13653571.12292981 13816261.93245484 13977974.43914849 14138507.18803503
- 14298070.56567955 14456660.41819829 14614001.05176772 14770310.19945163
- 14925566.84352306 15079436.13724521 15232084.82694429 15383532.24029338
- 15533572.27781731 15682226.55215925]</t>
+          <t>[10876605.76965806 11062578.61179022 11246636.11783682 11428824.22239867
+ 11609152.86208236 11787785.16332132 11964766.50090758 12140073.75971516
+ 12313880.44867646 12486240.72048981 12657113.8158561  12826683.36918215
+ 12995004.69444892 13162006.47474091 13327882.01459575 13492674.0852527
+ 13656253.90966897 13818823.71530198 13980404.4223942  14140793.53596996
+ 14300201.37354428 14458622.51067519 14615779.85780394 14771891.05533159
+ 14926933.46794325 15080570.33000097 15232967.91770947 15384143.9746539
+ 15533890.20674071 15682226.56941667]</t>
         </is>
       </c>
       <c r="D1414" t="inlineStr"/>
@@ -37068,14 +37097,14 @@
       </c>
       <c r="C1415" t="inlineStr">
         <is>
-          <t>[3.10579367e+08 3.00074687e+08 2.89524225e+08 2.78932991e+08
- 2.68305283e+08 2.57648563e+08 2.46966951e+08 2.36263308e+08
- 2.25544286e+08 2.14813680e+08 2.04073538e+08 1.93329802e+08
- 1.82585846e+08 1.71842844e+08 1.61106073e+08 1.50378355e+08
- 1.39659812e+08 1.28955097e+08 1.18266530e+08 1.07593320e+08
- 9.69395530e+07 8.63071897e+07 7.56949521e+07 6.51064059e+07
- 5.45433984e+07 4.40047383e+07 3.34931699e+07 2.30106844e+07
- 1.25576362e+07 2.13580689e+06]</t>
+          <t>[3.10598174e+08 3.00093301e+08 2.89542528e+08 2.78950859e+08
+ 2.68322594e+08 2.57665196e+08 2.46982785e+08 2.36278220e+08
+ 2.25558160e+08 2.14826396e+08 2.04084977e+08 1.93339852e+08
+ 1.82594392e+08 1.71849773e+08 1.61111278e+08 1.50381728e+08
+ 1.39661246e+08 1.28954495e+08 1.18263790e+08 1.07588346e+08
+ 9.69322558e+07 8.62974805e+07 7.56827467e+07 6.50916311e+07
+ 5.45259834e+07 4.39846201e+07 3.34702978e+07 2.29850165e+07
+ 1.25291438e+07 2.10447557e+06]</t>
         </is>
       </c>
       <c r="D1415" t="inlineStr"/>
@@ -37093,14 +37122,14 @@
       </c>
       <c r="C1416" t="inlineStr">
         <is>
-          <t>[1127486.62417985 1127480.08348777 1127473.54287157 1127482.87867613
- 1127476.33802734 1127469.79745443 1127479.90856295 1127473.3679488
- 1127466.82741054 1127476.37242403 1127469.83185071 1127463.29135328
- 1127473.25137812 1127466.71084154 1127460.17038084 1127472.10847033
- 1127465.56794643 1127459.02749841 1127473.79208699 1127467.25154368
- 1127460.71107625 1127478.51922755 1127471.97862944 1127465.43810721
- 1127484.08113859 1127478.43255931 1127472.75465461 1127480.22606922
- 1127476.66926903 1127473.10010393]</t>
+          <t>[1127486.57153003 1127480.03083652 1127473.49021891 1127482.86102093
+ 1127476.32037032 1127469.77979559 1127479.93311182 1127473.39249536
+ 1127466.85195479 1127476.44399328 1127469.90341711 1127463.36291682
+ 1127473.3787872  1127466.83824711 1127460.2977829  1127472.30852958
+ 1127465.76800132 1127459.22754896 1127474.08958915 1127467.54904036
+ 1127461.00856745 1127478.94602959 1127472.4054245  1127465.8648953
+ 1127484.66240744 1127479.01953842 1127473.34741464 1127480.91745227
+ 1127477.38261744 1127473.83636465]</t>
         </is>
       </c>
       <c r="D1416" t="inlineStr"/>
@@ -37118,7 +37147,7 @@
       </c>
       <c r="C1417" t="inlineStr">
         <is>
-          <t>[  2281018.64130019     41401.1098487  -10371253.51937727]</t>
+          <t>[  2281018.39455209     41401.18551928 -10391206.94916477]</t>
         </is>
       </c>
       <c r="D1417" t="inlineStr"/>
@@ -37136,7 +37165,7 @@
       </c>
       <c r="C1418" t="inlineStr">
         <is>
-          <t>[1.06850272e+07 3.21029059e+08 1.12748662e+06]</t>
+          <t>[1.06885656e+07 3.21047933e+08 1.12748657e+06]</t>
         </is>
       </c>
       <c r="D1418" t="inlineStr"/>
@@ -37154,14 +37183,14 @@
       </c>
       <c r="C1419" t="inlineStr">
         <is>
-          <t>[1.74527528e+08 1.68726021e+08 1.62898159e+08 1.75111870e+08
- 1.68518216e+08 1.61906464e+08 1.74595214e+08 1.67078644e+08
- 1.59552303e+08 1.70752184e+08 1.62235136e+08 1.53717881e+08
- 1.64115164e+08 1.54443869e+08 1.44783648e+08 1.55388568e+08
- 1.44254308e+08 1.33146050e+08 1.43391043e+08 1.30346041e+08
- 1.17353662e+08 1.25008304e+08 1.09540955e+08 9.42027040e+07
- 9.48815356e+07 7.79278950e+07 6.11181232e+07 4.97792399e+07
- 3.56285157e+07 2.82828570e+07]</t>
+          <t>[1.74521399e+08 1.68719783e+08 1.62891740e+08 1.75104386e+08
+ 1.68510369e+08 1.61898175e+08 1.74585260e+08 1.67068013e+08
+ 1.59540909e+08 1.70738381e+08 1.62220280e+08 1.53701879e+08
+ 1.64095620e+08 1.54422817e+08 1.44760989e+08 1.55360484e+08
+ 1.44224149e+08 1.33113714e+08 1.43350295e+08 1.30302501e+08
+ 1.17307234e+08 1.24949049e+08 1.09478056e+08 9.41361357e+07
+ 9.47973320e+07 7.78388681e+07 6.10249788e+07 4.96746652e+07
+ 3.55280847e+07 2.82100940e+07]</t>
         </is>
       </c>
       <c r="D1419" t="inlineStr"/>
@@ -37179,14 +37208,14 @@
       </c>
       <c r="C1420" t="inlineStr">
         <is>
-          <t>[ 3569471.36076223  3568344.45389243  3566785.23501533  3986075.0533961
-  3983658.09658659  3980974.71412821  4484802.4563222   4481261.56846858
-  4477494.41364573  5036510.96960268  5031806.45816263  5026890.45922068
-  5688236.79117436  5682220.33836755  5675995.14686489  6533616.31308603
-  6525984.75591466  6518137.45542345  7664577.6442654   7654849.8458601
-  7644889.84573259  9160400.87290704  9147909.96201869  9135160.89463519
- 10940107.95473212 10997717.47947424 11055924.8494285  12210356.09598101
- 12474894.6446966  12752036.27236886]</t>
+          <t>[ 3569470.99705384  3568344.11532488  3566784.92132764  3986074.73265852
+  3983657.80251383  3980974.44588256  4484802.17799834  4481261.3167483
+  4477494.18697909  5036510.73124929  5031806.24384822  5026890.26653515
+  5688236.58113353  5682220.14664569  5675994.97000035  6533616.10848771
+  6525984.55971642  6518137.26287063  7664577.41311293  7654849.60698537
+  7644889.59268102  9160400.57625039  9147909.63202895  9135160.5226842
+ 10940107.54636361 10997717.00310677 11055924.29235239 12210355.48385798
+ 12474893.93139104 12752035.4382348 ]</t>
         </is>
       </c>
       <c r="D1420" t="inlineStr"/>
@@ -37244,11 +37273,11 @@
       <c r="B1423" t="inlineStr"/>
       <c r="C1423" t="inlineStr">
         <is>
-          <t>[0.68108668 0.65847834 0.63576637 0.68347568 0.65778144 0.63201812
- 0.68160767 0.65232295 0.62300279 0.66681873 0.63364676 0.6004787
- 0.64122263 0.60357467 0.56597892 0.60764701 0.56434354 0.52116086
- 0.56165027 0.51100696 0.46061845 0.49148633 0.43169917 0.37258089
- 0.37739833 0.31291987 0.24983929 0.21098935 0.16255825 0.14000005]</t>
+          <t>[0.68106279 0.65845403 0.63574135 0.68344651 0.65775086 0.63198583
+ 0.68156888 0.65228154 0.62295841 0.66676497 0.6335889  0.60041639
+ 0.64114654 0.60349273 0.56589075 0.60753777 0.56422628 0.5210352
+ 0.56149203 0.51083803 0.46043852 0.49125707 0.43145639 0.37232486
+ 0.3770763  0.31258261 0.24949266 0.21061403 0.16222343 0.13977646]</t>
         </is>
       </c>
       <c r="D1423" t="inlineStr"/>
@@ -37262,11 +37291,11 @@
       <c r="B1424" t="inlineStr"/>
       <c r="C1424" t="inlineStr">
         <is>
-          <t>[0.02290787 0.02189353 0.02087938 0.02266949 0.02164005 0.0206106
- 0.02266045 0.02161013 0.02055978 0.02266173 0.02158491 0.02050806
- 0.02382179 0.02266869 0.02151548 0.02614315 0.02487059 0.02359791
- 0.030538   0.02907721 0.02761625 0.03773563 0.03598704 0.03423833
- 0.04465948 0.04274449 0.04083752 0.04581297 0.04391382 0.04206078]</t>
+          <t>[0.0229539  0.02193956 0.0209254  0.02272173 0.02169229 0.02066284
+ 0.02272054 0.02167021 0.02061986 0.02273108 0.02165426 0.02057742
+ 0.02390605 0.02275295 0.02159974 0.02625038 0.02497782 0.02370514
+ 0.0306831  0.0292223  0.02776134 0.0379438  0.03619521 0.03444649
+ 0.04494225 0.04302765 0.04112108 0.04614509 0.04424719 0.04239556]</t>
         </is>
       </c>
       <c r="D1424" t="inlineStr"/>
@@ -37280,11 +37309,11 @@
       <c r="B1425" t="inlineStr"/>
       <c r="C1425" t="inlineStr">
         <is>
-          <t>[1.05594513 1.01617334 0.97649202 1.05660197 1.01268426 0.96892586
- 1.05258616 1.00384176 0.95533044 1.0300521  0.97615479 0.92257278
- 0.99340003 0.93358909 0.8741896  0.94871265 0.88134626 0.81451747
- 0.89084976 0.81352087 0.73693317 0.80328793 0.71324629 0.62442959
- 0.6546969  0.5596753  0.46564501 0.41918125 0.34536732 0.30747999]</t>
+          <t>[1.05636418 1.01658605 0.97689807 1.05706797 1.01314126 0.96937354
+ 1.05310356 1.00434677 0.95582273 1.03061711 0.97670332 0.92310454
+ 0.99401175 0.93417922 0.87475787 0.94937717 0.8819822  0.81512464
+ 0.89157389 0.81420645 0.73758019 0.8040684  0.71397417 0.62510556
+ 0.6554987  0.5604271  0.46635012 0.41994767 0.34618218 0.30849059]</t>
         </is>
       </c>
       <c r="D1425" t="inlineStr"/>
@@ -37342,7 +37371,7 @@
       <c r="B1428" t="inlineStr"/>
       <c r="C1428" t="inlineStr">
         <is>
-          <t>[-0.02196114]</t>
+          <t>[-0.02192358]</t>
         </is>
       </c>
       <c r="D1428" t="inlineStr">
@@ -37360,7 +37389,7 @@
       <c r="B1429" t="inlineStr"/>
       <c r="C1429" t="inlineStr">
         <is>
-          <t>[-0.2850881]</t>
+          <t>[-0.28505054]</t>
         </is>
       </c>
       <c r="D1429" t="inlineStr">
@@ -37378,7 +37407,7 @@
       <c r="B1430" t="inlineStr"/>
       <c r="C1430" t="inlineStr">
         <is>
-          <t>[0.75737894]</t>
+          <t>[0.77120194]</t>
         </is>
       </c>
       <c r="D1430" t="inlineStr"/>
@@ -37414,7 +37443,7 @@
       </c>
       <c r="C1432" t="inlineStr">
         <is>
-          <t>[1.19725892e+08]</t>
+          <t>[1.19739796e+08]</t>
         </is>
       </c>
       <c r="D1432" t="inlineStr">
@@ -37458,7 +37487,7 @@
       </c>
       <c r="C1434" t="inlineStr">
         <is>
-          <t>[1.38882035e+08]</t>
+          <t>[1.38898164e+08]</t>
         </is>
       </c>
       <c r="D1434" t="inlineStr">
@@ -37502,7 +37531,7 @@
       </c>
       <c r="C1436" t="inlineStr">
         <is>
-          <t>[43576751.]</t>
+          <t>[43588678.]</t>
         </is>
       </c>
       <c r="D1436" t="inlineStr">
@@ -37564,7 +37593,7 @@
       </c>
       <c r="C1439" t="inlineStr">
         <is>
-          <t>[{'Module': 'FoundationCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 1.2800099319185887, 'Cost / project': 768005.9591511532, 'Cost / turbine': 6400.0496595929435, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'FoundationCost', 'Type of cost': 'Labor', 'Cost / kW': 13.64150123117051, 'Cost / project': 8184900.7387023065, 'Cost / turbine': 68207.50615585255, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'FoundationCost', 'Type of cost': 'Materials', 'Cost / kW': 23.671944594627803, 'Cost / project': 14203166.756776681, 'Cost / turbine': 118359.72297313901, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'FoundationCost', 'Type of cost': 'Mobilization', 'Cost / kW': 1.929672787885845, 'Cost / project': 1157803.672731507, 'Cost / turbine': 9648.363939429226, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Materials', 'Cost / kW': 5.476570135242568, 'Cost / project': 3285942.081145541, 'Cost / turbine': 27382.85067621284, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 3.0249317184701137, 'Cost / project': 1814959.031082068, 'Cost / turbine': 15124.658592350568, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Labor', 'Cost / kW': 3.2721485433158644, 'Cost / project': 1963289.1259895186, 'Cost / turbine': 16360.742716579321, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Other', 'Cost / kW': 2.86459986, 'Cost / project': 1718759.9160000002, 'Cost / turbine': 14322.999300000001, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Mobilization', 'Cost / kW': 0.38864554432410786, 'Cost / project': 233187.3265944647, 'Cost / turbine': 1943.2277216205393, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SubstationCost', 'Type of cost': 'Other', 'Cost / kW': 16.911599000804763, 'Cost / project': 10146959.400482858, 'Cost / turbine': 84557.99500402382, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'GridConnectionCost', 'Type of cost': 'Other', 'Cost / kW': 6.794429688199228, 'Cost / project': 4076657.812919537, 'Cost / turbine': 33972.14844099614, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'CollectionCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 4.4995824058955645, 'Cost / project': 2699749.4435373386, 'Cost / turbine': 22497.912029477822, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'CollectionCost', 'Type of cost': 'Labor', 'Cost / kW': 8.396861124129725, 'Cost / project': 5038116.674477834, 'Cost / turbine': 41984.30562064862, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'CollectionCost', 'Type of cost': 'Materials', 'Cost / kW': 31.87906207754761, 'Cost / project': 19127437.246528566, 'Cost / turbine': 159395.31038773805, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'CollectionCost', 'Type of cost': 'Mobilization', 'Cost / kW': 2.238775280378645, 'Cost / project': 1343265.1682271871, 'Cost / turbine': 11193.876401893225, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Labor', 'Cost / kW': 1.6666666666666667, 'Cost / project': 1000000.0, 'Cost / turbine': 8333.333333333334, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Materials', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Mobilization', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Other', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 6.130945857678428, 'Cost / project': 3678567.514607057, 'Cost / turbine': 30654.72928839214, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Fuel', 'Cost / kW': 0.189045, 'Cost / project': 113427.0, 'Cost / turbine': 945.225, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Labor', 'Cost / kW': 21.827617384093614, 'Cost / project': 13096570.430456169, 'Cost / turbine': 109138.08692046808, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Mobilization', 'Cost / kW': 3.957288666666667, 'Cost / project': 2374373.2, 'Cost / turbine': 19786.443333333336, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Other', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Materials', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'insurance', 'Cost / kW': 0.8962346259944913, 'Cost / project': 537740.7755966948, 'Cost / turbine': 4481.173129972457, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Construction Permitting', 'Cost / kW': 1.1437959042453882, 'Cost / project': 686277.5425472329, 'Cost / turbine': 5718.979521226941, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Project Management', 'Cost / kW': 3.982776508125, 'Cost / project': 2389665.904875, 'Cost / turbine': 19913.882540625, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Bonding', 'Cost / kW': 1.6004189749901634, 'Cost / project': 960251.384994098, 'Cost / turbine': 8002.094874950816, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Markup Contingency', 'Cost / kW': 20.837455054371922, 'Cost / project': 12502473.032623153, 'Cost / turbine': 104187.27527185962, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Engineering Foundation and Collections System (includes met mast)', 'Cost / kW': 7.80445, 'Cost / project': 4682670.0, 'Cost / turbine': 39022.25, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Site Facility', 'Cost / kW': 3.23625, 'Cost / project': 1941750.0, 'Cost / turbine': 16181.25, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}]</t>
+          <t>[{'Module': 'FoundationCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 1.2806673417942633, 'Cost / project': 768400.405076558, 'Cost / turbine': 6403.3367089713165, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'FoundationCost', 'Type of cost': 'Labor', 'Cost / kW': 13.647237809908829, 'Cost / project': 8188342.685945297, 'Cost / turbine': 68236.18904954413, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'FoundationCost', 'Type of cost': 'Materials', 'Cost / kW': 23.684379543220818, 'Cost / project': 14210627.72593249, 'Cost / turbine': 118421.89771610408, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'FoundationCost', 'Type of cost': 'Mobilization', 'Cost / kW': 1.9306142347461954, 'Cost / project': 1158368.5408477173, 'Cost / turbine': 9653.071173730978, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Materials', 'Cost / kW': 5.476570135242568, 'Cost / project': 3285942.081145541, 'Cost / turbine': 27382.85067621284, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 3.0249317184701137, 'Cost / project': 1814959.031082068, 'Cost / turbine': 15124.658592350568, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Labor', 'Cost / kW': 3.2721485433158644, 'Cost / project': 1963289.1259895186, 'Cost / turbine': 16360.742716579321, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Other', 'Cost / kW': 2.86459986, 'Cost / project': 1718759.9160000002, 'Cost / turbine': 14322.999300000001, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SitePreparationCost', 'Type of cost': 'Mobilization', 'Cost / kW': 0.38864554432410786, 'Cost / project': 233187.3265944647, 'Cost / turbine': 1943.2277216205393, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'SubstationCost', 'Type of cost': 'Other', 'Cost / kW': 16.911599000804763, 'Cost / project': 10146959.400482858, 'Cost / turbine': 84557.99500402382, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'GridConnectionCost', 'Type of cost': 'Other', 'Cost / kW': 6.794429688199228, 'Cost / project': 4076657.812919537, 'Cost / turbine': 33972.14844099614, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'CollectionCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 4.4995824058955645, 'Cost / project': 2699749.4435373386, 'Cost / turbine': 22497.912029477822, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'CollectionCost', 'Type of cost': 'Labor', 'Cost / kW': 8.396861124129725, 'Cost / project': 5038116.674477834, 'Cost / turbine': 41984.30562064862, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'CollectionCost', 'Type of cost': 'Materials', 'Cost / kW': 31.87906207754761, 'Cost / project': 19127437.246528566, 'Cost / turbine': 159395.31038773805, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'CollectionCost', 'Type of cost': 'Mobilization', 'Cost / kW': 2.238775280378645, 'Cost / project': 1343265.1682271871, 'Cost / turbine': 11193.876401893225, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Labor', 'Cost / kW': 1.6666666666666667, 'Cost / project': 1000000.0, 'Cost / turbine': 8333.333333333334, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Materials', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Mobilization', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'DevelopmentCost', 'Type of cost': 'Other', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Equipment rental', 'Cost / kW': 6.130945857678428, 'Cost / project': 3678567.514607057, 'Cost / turbine': 30654.72928839214, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Fuel', 'Cost / kW': 0.189045, 'Cost / project': 113427.0, 'Cost / turbine': 945.225, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Labor', 'Cost / kW': 21.827617384093614, 'Cost / project': 13096570.430456169, 'Cost / turbine': 109138.08692046808, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Mobilization', 'Cost / kW': 3.957288666666667, 'Cost / project': 2374373.2, 'Cost / turbine': 19786.443333333336, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Other', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ErectionCost', 'Type of cost': 'Materials', 'Cost / kW': 0.0, 'Cost / project': 0.0, 'Cost / turbine': 0.0, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'insurance', 'Cost / kW': 0.8963453401452686, 'Cost / project': 537807.2040871611, 'Cost / turbine': 4481.726700726343, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Construction Permitting', 'Cost / kW': 1.1441913119267355, 'Cost / project': 686514.7871560412, 'Cost / turbine': 5720.956559633677, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Project Management', 'Cost / kW': 3.982776508125, 'Cost / project': 2389665.904875, 'Cost / turbine': 19913.882540625, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Bonding', 'Cost / kW': 1.6006166788308367, 'Cost / project': 960370.007298502, 'Cost / turbine': 8003.083394154183, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Markup Contingency', 'Cost / kW': 20.840029158377494, 'Cost / project': 12504017.495026495, 'Cost / turbine': 104200.14579188747, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Engineering Foundation and Collections System (includes met mast)', 'Cost / kW': 7.80445, 'Cost / project': 4682670.0, 'Cost / turbine': 39022.25, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}, {'Module': 'ManagementCost', 'Type of cost': 'Site Facility', 'Cost / kW': 3.23625, 'Cost / project': 1941750.0, 'Cost / turbine': 16181.25, 'Number of turbines': 120, 'Rotor diameter (m)': 206.0, 'Turbine rating (MW)': 5.0, 'Project ID with serial': 'WISDEM'}]</t>
         </is>
       </c>
       <c r="D1439" t="inlineStr">
@@ -37586,7 +37615,7 @@
       </c>
       <c r="C1440" t="inlineStr">
         <is>
-          <t>[{'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'wind_multiplier', 'value': 1.0, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'kN', 'type': 'variable', 'variable_df_key_col_name': 'F_dead', 'value': 10941.528530320948, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'kN', 'type': 'variable', 'variable_df_key_col_name': 'F_horiz', 'value': 1083.292020938473, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'kN_m', 'type': 'variable', 'variable_df_key_col_name': 'M_tot_kN', 'value': 142487.20520072608, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Radius_o', 'value': 9.21345257116941, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Radius_g', 'value': 0.0, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Radius_b', 'value': 10.733751459546049, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Radius', 'value': 10.733751459546049, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'short_ton', 'type': 'variable', 'variable_df_key_col_name': 'steel_mass_short_ton_per_turbine', 'value': 43.774875324099824, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm^3', 'type': 'variable', 'variable_df_key_col_name': 'foundation_volume_concrete_m3_per_turbine', 'value': 384.3947604855974, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'operation_data: Operation ID-Number of days-Number of crews-Number of workers', 'value': 'Rebar installation-4203-47.0-1.0', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'operation_data: Operation ID-Number of days-Number of crews-Number of workers', 'value': 'Concrete placement-298-4.0-3.0', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'operation_data: Operation ID-Number of days-Number of crews-Number of workers', 'value': 'Excavation-147-2.0-nan', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'operation_data: Operation ID-Number of days-Number of crews-Number of workers', 'value': 'Backfill-90-1.0-1.0', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'ton (short)', 'type': 'dataframe', 'variable_df_key_col_name': 'material_needs_per_turbine: Material type ID-Quantity of material', 'value': '0-Steel - rebar-4.38e+01', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'cubic yards', 'type': 'dataframe', 'variable_df_key_col_name': 'material_needs_per_turbine: Material type ID-Quantity of material', 'value': '1-Concrete 5000 psi-4.95e+02', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'cubic_yards', 'type': 'dataframe', 'variable_df_key_col_name': 'material_needs_per_turbine: Material type ID-Quantity of material', 'value': '2-Excavated dirt-1.22e+03', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'cubic_yards', 'type': 'dataframe', 'variable_df_key_col_name': 'material_needs_per_turbine: Material type ID-Quantity of material', 'value': '3-Backfill-1.22e+03', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Equipment rental &lt;--&gt; Foundation &lt;--&gt; 768006', 'last_number': 768005.9591511532, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Labor &lt;--&gt; Foundation &lt;--&gt; 8184901', 'last_number': 8184900.7387023065, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Materials &lt;--&gt; Foundation &lt;--&gt; 14203167', 'last_number': 14203166.756776681, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Mobilization &lt;--&gt; Foundation &lt;--&gt; 1157804', 'last_number': 1157803.672731507, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm^3', 'type': 'variable', 'variable_df_key_col_name': 'Total road volume', 'value': 226917.6, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Depth to subgrade', 'value': 0.1, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'ft', 'type': 'variable', 'variable_df_key_col_name': 'Crane path width', 'value': 13.7, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Road length', 'value': 176598.0, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Road width', 'value': 6.0, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Road thickness', 'value': 0.2, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'cubic yards', 'type': 'variable', 'variable_df_key_col_name': 'Material volume', 'value': 412547.6561387999, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'cubic yards', 'type': 'variable', 'variable_df_key_col_name': 'Topsoil volume', 'value': 316444.455117, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'cubic yards', 'type': 'variable', 'variable_df_key_col_name': 'Embankment volume crane', 'value': 316444.455117, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'cubic yards', 'type': 'variable', 'variable_df_key_col_name': 'Embankment volume road', 'value': 277177.62492, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'ft^2', 'type': 'variable', 'variable_df_key_col_name': 'Rough grading area', 'value': 114.05299273199999, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Materials &lt;--&gt; Roads &lt;--&gt; 3285943', 'last_number': 3285942.081145541, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Equipment rental &lt;--&gt; Roads &lt;--&gt; 1814960', 'last_number': 1814959.031082068, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Labor &lt;--&gt; Roads &lt;--&gt; 1963290', 'last_number': 1963289.1259895186, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Other &lt;--&gt; Roads &lt;--&gt; 1718760', 'last_number': 1718759.9160000002, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Mobilization &lt;--&gt; Roads &lt;--&gt; 233188', 'last_number': 233187.3265944647, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Other &lt;--&gt; Substation &lt;--&gt; 10146960', 'last_number': 10146959.400482858, 'project_id_with_serial': 'WISDEM', 'module': 'SubstationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Other &lt;--&gt; Transmission and Distribution &lt;--&gt; 4076658', 'last_number': 4076657.812919537, 'project_id_with_serial': 'WISDEM', 'module': 'GridConnectionCost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Total Number of Turbines', 'value': 120.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total trench length', 'value': 388.66358074952393, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length', 'value': 388.66358074952393, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Number of Turbines Per String in Full String', 'value': 11.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Number of Full Strings', 'value': 10.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Number of Turbines in Partial String', 'value': 10.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Number of Partial Strings', 'value': 1.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Total number of strings full + partial', 'value': 11.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Trench Length to Substation (km)', 'value': 231.48558074952393, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Cable Length to Substation (km)', 'value': 231.48558074952393, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  AWG 1/0', 'value': 2.884, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  AWG 1/0', 'value': 31.724, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  AWG 1/0', 'value': 624488.188976378, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  AWG 4/0', 'value': 2.884, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  AWG 4/0', 'value': 31.724, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  AWG 4/0', 'value': 936732.283464567, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  MCM 500', 'value': 2.884, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  MCM 500', 'value': 31.724, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  MCM 500', 'value': 1353057.7427821523, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  MCM1000', 'value': 4.326, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  MCM1000', 'value': 47.586, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  MCM1000', 'value': 2497952.755905512, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  MCM1250', 'value': 1.442, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  MCM1250', 'value': 245.90558074952392, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  MCM1250', 'value': 13715206.275399957, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'list', 'variable_df_key_col_name': 'Number of turbines per cable type in full strings [AWG 1/0  ,  AWG 4/0  ,  MCM 500  ,  MCM1000  ,  MCM1250]', 'value': '[3.0, 2.0, 2.0, 3.0, 1.0]', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '0 &lt;--&gt; Project manager &lt;--&gt; 119.0 &lt;--&gt; 149 &lt;--&gt; (50% burden) https://www.salary.com/tools/salary-calculator/project-manager-sr-construction-hourly?type=base; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 107100.0 &lt;--&gt; 120510.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '1 &lt;--&gt; Site manager &lt;--&gt; 112.2 &lt;--&gt; 149 &lt;--&gt; (50% burden) https://www.salary.com/tools/salary-calculator/construction-manager-ii-hourly; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 100980.0 &lt;--&gt; 114390.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '2 &lt;--&gt; Construction manager &lt;--&gt; 112.2 &lt;--&gt; 149 &lt;--&gt; (50% burden) https://www.salary.com/tools/salary-calculator/construction-manager-ii-hourly; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 100980.0 &lt;--&gt; 114390.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '3 &lt;--&gt; Project engineer &lt;--&gt; 93.5 &lt;--&gt; 149 &lt;--&gt; (50% burden) https://www.salary.com/tools/salary-calculator/project-engineer-iii-construction-hourly; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 84150.0 &lt;--&gt; 97560.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '4 &lt;--&gt; Safety or qc manager &lt;--&gt; 106.11764705882352 &lt;--&gt; 149 &lt;--&gt; (70% burden) https://www.salary.com/tools/salary-calculator/construction-site-safety-manager-hourly; plus 35% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 95505.88235294116 &lt;--&gt; 108915.88235294116', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '5 &lt;--&gt; Logistics manager &lt;--&gt; 99.9 &lt;--&gt; 149 &lt;--&gt; (50 % burden) https://www.salary.com/research/salary/benchmark/logistics-manager-hourly-wages; plus 35% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 89910.0 &lt;--&gt; 103320.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '6 &lt;--&gt; Office admin &lt;--&gt; 44.56249999999999 &lt;--&gt; 149 &lt;--&gt; (35% burden) https://www.salary.com/tools/salary-calculator/administrative-assistant-ii-hourly ; 25% for work on a ladder or a scaffold, in a crawl space, in a congested area or remote from the material storage point; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 40106.24999999999 &lt;--&gt; 53516.24999999999', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'list', 'variable_df_key_col_name': 'Percent length of cable in partial string [AWG 1/0  ,  AWG 4/0  ,  MCM 500  ,  MCM1000  ,  MCM1250]', 'value': '[1. 1. 1. 1. 0.]', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Equipment rental &lt;--&gt; Collection &lt;--&gt; 2699750', 'last_number': 2699749.4435373386, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Labor &lt;--&gt; Collection &lt;--&gt; 5038117', 'last_number': 5038116.674477834, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Materials &lt;--&gt; Collection &lt;--&gt; 19127438', 'last_number': 19127437.246528566, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Mobilization &lt;--&gt; Collection &lt;--&gt; 1343266', 'last_number': 1343265.1682271871, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Equipment rental - Development - 0', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Labor - Development - 1000000', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Materials - Development - 0', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Mobilization - Development - 0', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Other - Development - 0', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': '_number_of_equip: Operation-Crane name-Boom system-Number of equipment', 'value': 'Top-Big LR110000-Big PDW3B2 Derrick-3', 'last_number': 3, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': '_number_of_equip: Operation-Crane name-Boom system-Number of equipment', 'value': 'Offload-LB 75-Hydraulic-2', 'last_number': 2, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': '_number_of_equip: Operation-Crane name-Boom system-Number of equipment', 'value': 'Base-LR1750/2-SX3D4F2B Derrick (walk)-3', 'last_number': 3, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'erection_selected_detailed_data: Operation-Crane name-Boom system-Operational construct days over time construct days', 'value': 'Top-Big LR110000-Big PDW3B2 Derrick-3.0', 'last_number': 3.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'erection_selected_detailed_data: Operation-Crane name-Boom system-Operational construct days over time construct days', 'value': 'Offload-LB 75-Hydraulic-1.0', 'last_number': 1.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'erection_selected_detailed_data: Operation-Crane name-Boom system-Operational construct days over time construct days', 'value': 'Base-LR1750/2-SX3D4F2B Derrick (walk)-2.0', 'last_number': 2.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Nacelle - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Hub - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Blade 1 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Blade 2 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Blade 3 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 1 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 2 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 3 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 4 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 5 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 6 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 7 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 8 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 9 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 10 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 11 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_choice: Crew name - Boom system - Operation', 'value': 'Big LR110000 - Big PDW3B2 Derrick - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_choice: Crew name - Boom system - Operation', 'value': 'LB 75 - Hydraulic - Offload', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_choice: Crew name - Boom system - Operation', 'value': 'LR1750/2 - SX3D4F2B Derrick (walk) - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Equipment rental cost USD - 2452310.014545454', 'last_number': 2452310.014545454, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Equipment rental cost USD - 58546.0706713781', 'last_number': 58546.0706713781, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Equipment rental cost USD - 1167711.4293902244', 'last_number': 1167711.4293902244, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Fuel cost USD - 72540.0', 'last_number': 72540.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Fuel cost USD - 5544.0', 'last_number': 5544.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Fuel cost USD - 35343.0', 'last_number': 35343.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Labor cost USD without management - 3746069.9467044845', 'last_number': 3746069.9467044845, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Labor cost USD without management - 882394.6829100354', 'last_number': 882394.6829100354, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Labor cost USD without management - 2311965.0408416493', 'last_number': 2311965.0408416493, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Mobilization cost USD - 1621827.2', 'last_number': 1621827.2, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Mobilization cost USD - 32160.0', 'last_number': 32160.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Mobilization cost USD - 720386.0', 'last_number': 720386.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Subtotal for hourly labor (non-management) USD - 3228741.9467044845', 'last_number': 3228741.9467044845, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Subtotal for hourly labor (non-management) USD - 757234.6829100354', 'last_number': 757234.6829100354, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Subtotal for hourly labor (non-management) USD - 1992807.040841649', 'last_number': 1992807.040841649, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Subtotal for per diem labor (non-management) USD - 517328.0', 'last_number': 517328.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Subtotal for per diem labor (non-management) USD - 125160.0', 'last_number': 125160.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Subtotal for per diem labor (non-management) USD - 319158.0', 'last_number': 319158.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Total cost USD - 7892747.161249938', 'last_number': 7892747.161249938, 'project_id_with_serial': 'WISDEM', 'mod</t>
+          <t>[{'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'wind_multiplier', 'value': 1.0, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'kN', 'type': 'variable', 'variable_df_key_col_name': 'F_dead', 'value': 11001.140727222379, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'kN', 'type': 'variable', 'variable_df_key_col_name': 'F_horiz', 'value': 1083.292020938473, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'kN_m', 'type': 'variable', 'variable_df_key_col_name': 'M_tot_kN', 'value': 142487.20520072608, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Radius_o', 'value': 9.202237310016663, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Radius_g', 'value': 0.0, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Radius_b', 'value': 10.736570326478265, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Radius', 'value': 10.736570326478265, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'short_ton', 'type': 'variable', 'variable_df_key_col_name': 'steel_mass_short_ton_per_turbine', 'value': 43.79787040682931, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm^3', 'type': 'variable', 'variable_df_key_col_name': 'foundation_volume_concrete_m3_per_turbine', 'value': 384.59668428898226, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'operation_data: Operation ID-Number of days-Number of crews-Number of workers', 'value': 'Rebar installation-4205-47.0-1.0', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'operation_data: Operation ID-Number of days-Number of crews-Number of workers', 'value': 'Concrete placement-298-4.0-3.0', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'operation_data: Operation ID-Number of days-Number of crews-Number of workers', 'value': 'Excavation-147-2.0-nan', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'operation_data: Operation ID-Number of days-Number of crews-Number of workers', 'value': 'Backfill-90-1.0-1.0', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'ton (short)', 'type': 'dataframe', 'variable_df_key_col_name': 'material_needs_per_turbine: Material type ID-Quantity of material', 'value': '0-Steel - rebar-4.38e+01', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'cubic yards', 'type': 'dataframe', 'variable_df_key_col_name': 'material_needs_per_turbine: Material type ID-Quantity of material', 'value': '1-Concrete 5000 psi-4.95e+02', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'cubic_yards', 'type': 'dataframe', 'variable_df_key_col_name': 'material_needs_per_turbine: Material type ID-Quantity of material', 'value': '2-Excavated dirt-1.22e+03', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'cubic_yards', 'type': 'dataframe', 'variable_df_key_col_name': 'material_needs_per_turbine: Material type ID-Quantity of material', 'value': '3-Backfill-1.22e+03', 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Equipment rental &lt;--&gt; Foundation &lt;--&gt; 768401', 'last_number': 768400.405076558, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Labor &lt;--&gt; Foundation &lt;--&gt; 8188343', 'last_number': 8188342.685945297, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Materials &lt;--&gt; Foundation &lt;--&gt; 14210628', 'last_number': 14210627.72593249, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Mobilization &lt;--&gt; Foundation &lt;--&gt; 1158369', 'last_number': 1158368.5408477173, 'project_id_with_serial': 'WISDEM', 'module': 'FoundationCost'}, {'unit': 'm^3', 'type': 'variable', 'variable_df_key_col_name': 'Total road volume', 'value': 226917.6, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Depth to subgrade', 'value': 0.1, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'ft', 'type': 'variable', 'variable_df_key_col_name': 'Crane path width', 'value': 13.7, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Road length', 'value': 176598.0, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Road width', 'value': 6.0, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'm', 'type': 'variable', 'variable_df_key_col_name': 'Road thickness', 'value': 0.2, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'cubic yards', 'type': 'variable', 'variable_df_key_col_name': 'Material volume', 'value': 412547.6561387999, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'cubic yards', 'type': 'variable', 'variable_df_key_col_name': 'Topsoil volume', 'value': 316444.455117, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'cubic yards', 'type': 'variable', 'variable_df_key_col_name': 'Embankment volume crane', 'value': 316444.455117, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'cubic yards', 'type': 'variable', 'variable_df_key_col_name': 'Embankment volume road', 'value': 277177.62492, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': 'ft^2', 'type': 'variable', 'variable_df_key_col_name': 'Rough grading area', 'value': 114.05299273199999, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Materials &lt;--&gt; Roads &lt;--&gt; 3285943', 'last_number': 3285942.081145541, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Equipment rental &lt;--&gt; Roads &lt;--&gt; 1814960', 'last_number': 1814959.031082068, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Labor &lt;--&gt; Roads &lt;--&gt; 1963290', 'last_number': 1963289.1259895186, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Other &lt;--&gt; Roads &lt;--&gt; 1718760', 'last_number': 1718759.9160000002, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Mobilization &lt;--&gt; Roads &lt;--&gt; 233188', 'last_number': 233187.3265944647, 'project_id_with_serial': 'WISDEM', 'module': 'SitePreparationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Other &lt;--&gt; Substation &lt;--&gt; 10146960', 'last_number': 10146959.400482858, 'project_id_with_serial': 'WISDEM', 'module': 'SubstationCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Other &lt;--&gt; Transmission and Distribution &lt;--&gt; 4076658', 'last_number': 4076657.812919537, 'project_id_with_serial': 'WISDEM', 'module': 'GridConnectionCost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Total Number of Turbines', 'value': 120.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total trench length', 'value': 388.66358074952393, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length', 'value': 388.66358074952393, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Number of Turbines Per String in Full String', 'value': 11.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Number of Full Strings', 'value': 10.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Number of Turbines in Partial String', 'value': 10.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Number of Partial Strings', 'value': 1.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Total number of strings full + partial', 'value': 11.0, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Trench Length to Substation (km)', 'value': 231.48558074952393, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'variable', 'variable_df_key_col_name': 'Cable Length to Substation (km)', 'value': 231.48558074952393, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  AWG 1/0', 'value': 2.884, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  AWG 1/0', 'value': 31.724, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  AWG 1/0', 'value': 624488.188976378, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  AWG 4/0', 'value': 2.884, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  AWG 4/0', 'value': 31.724, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  AWG 4/0', 'value': 936732.283464567, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  MCM 500', 'value': 2.884, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  MCM 500', 'value': 31.724, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  MCM 500', 'value': 1353057.7427821523, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  MCM1000', 'value': 4.326, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  MCM1000', 'value': 47.586, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  MCM1000', 'value': 2497952.755905512, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Array cable length for cable  MCM1250', 'value': 1.442, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'km', 'type': 'variable', 'variable_df_key_col_name': 'Total cable length for cable  MCM1250', 'value': 245.90558074952392, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': 'usd', 'type': 'variable', 'variable_df_key_col_name': 'Total cable cost for cable  MCM1250', 'value': 13715206.275399957, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'list', 'variable_df_key_col_name': 'Number of turbines per cable type in full strings [AWG 1/0  ,  AWG 4/0  ,  MCM 500  ,  MCM1000  ,  MCM1250]', 'value': '[3.0, 2.0, 2.0, 3.0, 1.0]', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '0 &lt;--&gt; Project manager &lt;--&gt; 119.0 &lt;--&gt; 149 &lt;--&gt; (50% burden) https://www.salary.com/tools/salary-calculator/project-manager-sr-construction-hourly?type=base; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 107100.0 &lt;--&gt; 120510.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '1 &lt;--&gt; Site manager &lt;--&gt; 112.2 &lt;--&gt; 149 &lt;--&gt; (50% burden) https://www.salary.com/tools/salary-calculator/construction-manager-ii-hourly; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 100980.0 &lt;--&gt; 114390.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '2 &lt;--&gt; Construction manager &lt;--&gt; 112.2 &lt;--&gt; 149 &lt;--&gt; (50% burden) https://www.salary.com/tools/salary-calculator/construction-manager-ii-hourly; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 100980.0 &lt;--&gt; 114390.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '3 &lt;--&gt; Project engineer &lt;--&gt; 93.5 &lt;--&gt; 149 &lt;--&gt; (50% burden) https://www.salary.com/tools/salary-calculator/project-engineer-iii-construction-hourly; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 84150.0 &lt;--&gt; 97560.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '4 &lt;--&gt; Safety or qc manager &lt;--&gt; 106.11764705882352 &lt;--&gt; 149 &lt;--&gt; (70% burden) https://www.salary.com/tools/salary-calculator/construction-site-safety-manager-hourly; plus 35% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 95505.88235294116 &lt;--&gt; 108915.88235294116', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '5 &lt;--&gt; Logistics manager &lt;--&gt; 99.9 &lt;--&gt; 149 &lt;--&gt; (50 % burden) https://www.salary.com/research/salary/benchmark/logistics-manager-hourly-wages; plus 35% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 89910.0 &lt;--&gt; 103320.0', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Labor type ID &lt;--&gt; Hourly rate USD per hour &lt;--&gt; Per diem USD per day &lt;--&gt; Operation &lt;--&gt; Crew type &lt;--&gt; Crew name &lt;--&gt; Number of workers &lt;--&gt; Per Diem Total &lt;--&gt; Hourly costs total &lt;--&gt; Crew total cost ', 'value': '6 &lt;--&gt; Office admin &lt;--&gt; 44.56249999999999 &lt;--&gt; 149 &lt;--&gt; (35% burden) https://www.salary.com/tools/salary-calculator/administrative-assistant-ii-hourly ; 25% for work on a ladder or a scaffold, in a crawl space, in a congested area or remote from the material storage point; plus 20% for demanding specs, rigid inspec-tions, unreliable suppliers. &lt;--&gt; M0 &lt;--&gt; Management &lt;--&gt; Management - project size &lt;--&gt; 1 &lt;--&gt; 13410.0 &lt;--&gt; 40106.24999999999 &lt;--&gt; 53516.24999999999', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'list', 'variable_df_key_col_name': 'Percent length of cable in partial string [AWG 1/0  ,  AWG 4/0  ,  MCM 500  ,  MCM1000  ,  MCM1250]', 'value': '[1. 1. 1. 1. 0.]', 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Equipment rental &lt;--&gt; Collection &lt;--&gt; 2699750', 'last_number': 2699749.4435373386, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Labor &lt;--&gt; Collection &lt;--&gt; 5038117', 'last_number': 5038116.674477834, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Materials &lt;--&gt; Collection &lt;--&gt; 19127438', 'last_number': 19127437.246528566, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost &lt;--&gt; Phase of Construction &lt;--&gt; Cost in USD ', 'value': 'Mobilization &lt;--&gt; Collection &lt;--&gt; 1343266', 'last_number': 1343265.1682271871, 'project_id_with_serial': 'WISDEM', 'module': 'Collection Cost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Equipment rental - Development - 0', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Labor - Development - 1000000', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Materials - Development - 0', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Mobilization - Development - 0', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'Type of Cost - Phase of Construction - Cost in USD', 'value': 'Other - Development - 0', 'last_number': 'Development', 'project_id_with_serial': 'WISDEM', 'module': 'DevelopmentCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': '_number_of_equip: Operation-Crane name-Boom system-Number of equipment', 'value': 'Top-Big LR110000-Big PDW3B2 Derrick-3', 'last_number': 3, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': '_number_of_equip: Operation-Crane name-Boom system-Number of equipment', 'value': 'Offload-LB 75-Hydraulic-2', 'last_number': 2, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': '_number_of_equip: Operation-Crane name-Boom system-Number of equipment', 'value': 'Base-LR1750/2-SX3D4F2B Derrick (walk)-3', 'last_number': 3, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'erection_selected_detailed_data: Operation-Crane name-Boom system-Operational construct days over time construct days', 'value': 'Top-Big LR110000-Big PDW3B2 Derrick-3.0', 'last_number': 3.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'erection_selected_detailed_data: Operation-Crane name-Boom system-Operational construct days over time construct days', 'value': 'Offload-LB 75-Hydraulic-1.0', 'last_number': 1.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'erection_selected_detailed_data: Operation-Crane name-Boom system-Operational construct days over time construct days', 'value': 'Base-LR1750/2-SX3D4F2B Derrick (walk)-2.0', 'last_number': 2.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Nacelle - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Hub - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Blade 1 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Blade 2 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Blade 3 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 1 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 2 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 3 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 4 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 5 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 6 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 7 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 8 - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 9 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 10 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'component_name_topvbase: Operation - Top or Base', 'value': 'Tower 11 - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_choice: Crew name - Boom system - Operation', 'value': 'Big LR110000 - Big PDW3B2 Derrick - Top', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_choice: Crew name - Boom system - Operation', 'value': 'LB 75 - Hydraulic - Offload', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_choice: Crew name - Boom system - Operation', 'value': 'LR1750/2 - SX3D4F2B Derrick (walk) - Base', 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Equipment rental cost USD - 2452310.014545454', 'last_number': 2452310.014545454, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Equipment rental cost USD - 58546.0706713781', 'last_number': 58546.0706713781, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Equipment rental cost USD - 1167711.4293902244', 'last_number': 1167711.4293902244, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Fuel cost USD - 72540.0', 'last_number': 72540.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Fuel cost USD - 5544.0', 'last_number': 5544.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Fuel cost USD - 35343.0', 'last_number': 35343.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Labor cost USD without management - 3746069.9467044845', 'last_number': 3746069.9467044845, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Labor cost USD without management - 882394.6829100354', 'last_number': 882394.6829100354, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Labor cost USD without management - 2311965.0408416493', 'last_number': 2311965.0408416493, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Mobilization cost USD - 1621827.2', 'last_number': 1621827.2, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Mobilization cost USD - 32160.0', 'last_number': 32160.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Mobilization cost USD - 720386.0', 'last_number': 720386.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Subtotal for hourly labor (non-management) USD - 3228741.9467044845', 'last_number': 3228741.9467044845, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Subtotal for hourly labor (non-management) USD - 757234.6829100354', 'last_number': 757234.6829100354, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Subtotal for hourly labor (non-management) USD - 1992807.040841649', 'last_number': 1992807.040841649, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Subtotal for per diem labor (non-management) USD - 517328.0', 'last_number': 517328.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LB 75-Hydraulic-Offload - Subtotal for per diem labor (non-management) USD - 125160.0', 'last_number': 125160.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'LR1750/2-SX3D4F2B Derrick (walk)-Base - Subtotal for per diem labor (non-management) USD - 319158.0', 'last_number': 319158.0, 'project_id_with_serial': 'WISDEM', 'module': 'ErectionCost'}, {'unit': '', 'type': 'dataframe', 'variable_df_key_col_name': 'crane_data_output: crane_boom_operation_concat - variable - value', 'value': 'Big LR110000-Big PDW3B2 Derrick-Top - Total cost USD - 7892747.161249938', 'last_number': 7892747.161249938, 'project_id_with_serial': 'WISDEM', 'modu</t>
         </is>
       </c>
       <c r="D1440" t="inlineStr">
@@ -37673,10 +37702,10 @@
         <is>
           <t xml:space="preserve">  Component  Mass tonne  Lift height m  Surface area sq m  Coeff drag  Coeff drag (installed)  Section height m  Lever arm m  Cycle time installation hrs  Offload hook height m  Offload cycle time hrs  Multplier drag rotor  Multiplier tower drag Operation
 0   Nacelle  234.082584     140.000000          33.000000         0.8                     0.8          0.000000    80.000000                          1.5                      6                     0.5              1.000000                      0       Top
-1       Hub   34.387161     140.000000          11.300000         1.1                     1.1          0.000000    80.000000                          1.0                      6                     0.5              0.000000                      0       Top
-2   Blade 1   51.003992     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
-2   Blade 2   51.003992     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
-2   Blade 3   51.003992     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
+1       Hub   36.410027     140.000000          11.300000         1.1                     1.1          0.000000    80.000000                          1.0                      6                     0.5              0.000000                      0       Top
+2   Blade 1   52.661472     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
+2   Blade 2   52.661472     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
+2   Blade 3   52.661472     140.000000          33.440000         0.1                     1.4          0.000000    80.000000                          1.0                      6                     0.5              0.666667                      0       Top
 5   Tower 1   78.406651      12.727273          67.572802         0.6                     1.1         12.727273     6.363636                          1.0                      6                     0.5              0.000000                      1      Base
 5   Tower 2   78.406651      25.454545          67.572802         0.6                     1.1         12.727273    19.090909                          1.0                      6                     0.5              0.000000                      1      Base
 5   Tower 3   78.406651      38.181818          67.572802         0.6                     1.1         12.727273    31.818182                          1.0                      6                     0.5              0.000000                      1      Base
@@ -37709,7 +37738,7 @@
       </c>
       <c r="C1444" t="inlineStr">
         <is>
-          <t>[0.03802842]</t>
+          <t>[0.03854576]</t>
         </is>
       </c>
       <c r="D1444" t="inlineStr"/>

</xml_diff>